<commit_message>
Auto-committed on 2022/02/22 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -83,7 +83,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月17日 18:44:26</t>
+    <t xml:space="preserve">2022年02月21日 16:36:10</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">擔保品-建物修改原因檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:22:23</t>
+    <t xml:space="preserve">2022年02月22日 09:53:51</t>
   </si>
   <si>
     <t xml:space="preserve">ClEva</t>
@@ -2771,7 +2771,7 @@
     <t xml:space="preserve">傳票媒體檔2022年格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月16日 09:32:50</t>
+    <t xml:space="preserve">2022年02月22日 10:33:03</t>
   </si>
   <si>
     <t xml:space="preserve">UspErrorLog</t>
@@ -2990,7 +2990,7 @@
     <t xml:space="preserve">查詢紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月21日 16:15:59</t>
+    <t xml:space="preserve">2022年02月21日 17:47:42</t>
   </si>
   <si>
     <t xml:space="preserve">TxLock</t>
@@ -3032,7 +3032,7 @@
     <t xml:space="preserve">使用者檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月17日 15:05:28</t>
+    <t xml:space="preserve">2022年02月21日 17:47:35</t>
   </si>
   <si>
     <t xml:space="preserve">TxTellerAuth</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/02/24 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1034">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -2756,6 +2756,15 @@
     <t xml:space="preserve">2021年12月10日 10:15:15</t>
   </si>
   <si>
+    <t xml:space="preserve">SlipEbsRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">傳票上傳EBS紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年02月24日 11:10:20</t>
+  </si>
+  <si>
     <t xml:space="preserve">SlipMedia</t>
   </si>
   <si>
@@ -2990,7 +2999,7 @@
     <t xml:space="preserve">查詢紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月22日 17:17:54</t>
+    <t xml:space="preserve">2022年02月24日 10:25:59</t>
   </si>
   <si>
     <t xml:space="preserve">TxLock</t>
@@ -3216,7 +3225,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="2">
@@ -8864,7 +8873,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -8882,7 +8891,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8900,7 +8909,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8918,7 +8927,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -8927,25 +8936,25 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B319" s="1" t="s">
         <v>926</v>
       </c>
-      <c r="B319" s="1" t="s">
+      <c r="C319" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="C319" s="1" t="s">
+      <c r="D319" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E319" s="1" t="s">
         <v>928</v>
-      </c>
-      <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>930</v>
@@ -8954,7 +8963,7 @@
         <v>931</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -8963,7 +8972,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>933</v>
@@ -8972,7 +8981,7 @@
         <v>934</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -8981,7 +8990,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>936</v>
@@ -8990,7 +8999,7 @@
         <v>937</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -8999,7 +9008,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>939</v>
@@ -9008,7 +9017,7 @@
         <v>940</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9017,7 +9026,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>942</v>
@@ -9026,7 +9035,7 @@
         <v>943</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9035,7 +9044,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>945</v>
@@ -9044,7 +9053,7 @@
         <v>946</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9053,7 +9062,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>948</v>
@@ -9062,7 +9071,7 @@
         <v>949</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9071,7 +9080,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>951</v>
@@ -9080,7 +9089,7 @@
         <v>952</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9089,7 +9098,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>954</v>
@@ -9098,7 +9107,7 @@
         <v>955</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9107,7 +9116,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>957</v>
@@ -9116,7 +9125,7 @@
         <v>958</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9125,7 +9134,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>960</v>
@@ -9134,7 +9143,7 @@
         <v>961</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9143,7 +9152,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>963</v>
@@ -9152,7 +9161,7 @@
         <v>964</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9161,7 +9170,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>966</v>
@@ -9170,7 +9179,7 @@
         <v>967</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9179,7 +9188,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>969</v>
@@ -9188,7 +9197,7 @@
         <v>970</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9197,7 +9206,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>972</v>
@@ -9206,7 +9215,7 @@
         <v>973</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9215,7 +9224,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9224,7 +9233,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9233,7 +9242,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9242,7 +9251,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9251,7 +9260,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9260,7 +9269,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9269,7 +9278,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9278,7 +9287,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9287,7 +9296,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9296,7 +9305,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9305,7 +9314,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9314,7 +9323,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9323,7 +9332,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9332,7 +9341,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9341,7 +9350,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9350,7 +9359,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9359,34 +9368,34 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>985</v>
+        <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>1002</v>
+        <v>988</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9395,7 +9404,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1004</v>
@@ -9404,7 +9413,7 @@
         <v>1005</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9413,7 +9422,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1007</v>
@@ -9422,7 +9431,7 @@
         <v>1008</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9431,34 +9440,34 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1010</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>1005</v>
+        <v>1011</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerTest.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>1013</v>
+        <v>1008</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerTest.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9467,7 +9476,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1015</v>
@@ -9476,7 +9485,7 @@
         <v>1016</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9485,7 +9494,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1018</v>
@@ -9494,7 +9503,7 @@
         <v>1019</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9503,7 +9512,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1021</v>
@@ -9512,7 +9521,7 @@
         <v>1022</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9521,7 +9530,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1024</v>
@@ -9530,7 +9539,7 @@
         <v>1025</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9539,7 +9548,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1027</v>
@@ -9548,11 +9557,29 @@
         <v>1028</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
         <v>1029</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D354" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E354" s="1" t="s">
+        <v>1032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/01 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -851,7 +851,7 @@
     <t xml:space="preserve">法催紀錄面催檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月22日 15:06:53</t>
+    <t xml:space="preserve">2022年03月01日 15:49:05</t>
   </si>
   <si>
     <t xml:space="preserve">CollRemind</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">法催紀錄電催檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月22日 15:06:00</t>
+    <t xml:space="preserve">2022年03月01日 15:42:40</t>
   </si>
   <si>
     <t xml:space="preserve">HlAreaData</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月01日 10:50:23</t>
+    <t xml:space="preserve">2022年03月01日 12:08:17</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1562,7 +1562,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月15日 10:00:04</t>
+    <t xml:space="preserve">2022年03月01日 16:36:01</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>
@@ -3050,7 +3050,7 @@
     <t xml:space="preserve">使用者檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月21日 17:47:35</t>
+    <t xml:space="preserve">2022年03月01日 15:49:10</t>
   </si>
   <si>
     <t xml:space="preserve">TxTellerAuth</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/02 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -677,7 +677,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月17日 17:04:22</t>
+    <t xml:space="preserve">2022年03月02日 10:59:07</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月01日 12:08:17</t>
+    <t xml:space="preserve">2022年03月01日 19:44:20</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">建築造價參考檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:36:58</t>
+    <t xml:space="preserve">2022年03月02日 10:36:32</t>
   </si>
   <si>
     <t xml:space="preserve">CdCashFlow</t>
@@ -1562,7 +1562,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月01日 16:36:01</t>
+    <t xml:space="preserve">2022年03月01日 19:25:54</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/03 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -512,7 +512,7 @@
     <t xml:space="preserve">放款約定還本檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:39:16</t>
+    <t xml:space="preserve">2022年03月03日 15:56:34</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorMain</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">法催紀錄電催檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月01日 15:42:40</t>
+    <t xml:space="preserve">2022年03月03日 14:49:40</t>
   </si>
   <si>
     <t xml:space="preserve">HlAreaData</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">建築造價參考檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月02日 10:36:32</t>
+    <t xml:space="preserve">2022年03月02日 17:15:19</t>
   </si>
   <si>
     <t xml:space="preserve">CdCashFlow</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/09 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -1283,7 +1283,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月01日 19:44:20</t>
+    <t xml:space="preserve">2022年03月08日 18:17:00</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">行業別代號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:42:29</t>
+    <t xml:space="preserve">2022年03月08日 17:34:51</t>
   </si>
   <si>
     <t xml:space="preserve">CdInsurer</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/10 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -584,7 +584,7 @@
     <t xml:space="preserve">放款利率變動檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:45:09</t>
+    <t xml:space="preserve">2022年03月09日 19:44:28</t>
   </si>
   <si>
     <t xml:space="preserve">LoanSynd</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:01:44</t>
+    <t xml:space="preserve">2022年03月09日 20:31:12</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/16 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -593,7 +593,7 @@
     <t xml:space="preserve">聯貸案訂約檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月24日 16:33:21</t>
+    <t xml:space="preserve">2022年03月15日 16:53:40</t>
   </si>
   <si>
     <t xml:space="preserve">LoanSyndItem</t>
@@ -3008,7 +3008,7 @@
     <t xml:space="preserve">輸出檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月15日 10:46:30</t>
+    <t xml:space="preserve">2022年03月15日 17:41:31</t>
   </si>
   <si>
     <t xml:space="preserve">TxFlow</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/17 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -614,7 +614,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月14日 11:38:54</t>
+    <t xml:space="preserve">2022年03月17日 15:20:59</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月24日 16:57:14</t>
+    <t xml:space="preserve">2022年03月17日 15:20:38</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -1400,7 +1400,7 @@
     <t xml:space="preserve">營業單位資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月14日 15:53:02</t>
+    <t xml:space="preserve">2022年03月17日 15:25:23</t>
   </si>
   <si>
     <t xml:space="preserve">CdBranchGroup</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/01 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -356,7 +356,7 @@
     <t xml:space="preserve">結清戶個資控管檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月31日 16:29:15</t>
+    <t xml:space="preserve">2022年03月31日 18:51:12</t>
   </si>
   <si>
     <t xml:space="preserve">CustRmk</t>
@@ -2717,7 +2717,7 @@
     <t xml:space="preserve">LM052備抵損失資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月28日 17:35:16</t>
+    <t xml:space="preserve">2022年03月31日 18:17:37</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM052Ovdu</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/11 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -365,7 +365,7 @@
     <t xml:space="preserve">顧客控管警訊檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月07日 22:09:37</t>
+    <t xml:space="preserve">2022年04月10日 14:25:22</t>
   </si>
   <si>
     <t xml:space="preserve">FacCaseAppl</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">帳務備忘錄明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月23日 10:31:35</t>
+    <t xml:space="preserve">2022年04月10日 14:40:15</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/14 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月17日 15:20:59</t>
+    <t xml:space="preserve">2022年04月13日 18:58:00</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -632,7 +632,7 @@
     <t xml:space="preserve">ACH授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月24日 17:32:54</t>
+    <t xml:space="preserve">2022年04月13日 18:57:51</t>
   </si>
   <si>
     <t xml:space="preserve">AchDeductMedia</t>
@@ -650,7 +650,7 @@
     <t xml:space="preserve">銀扣授權帳號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:55:17</t>
+    <t xml:space="preserve">2022年04月13日 18:57:49</t>
   </si>
   <si>
     <t xml:space="preserve">BankDeductDtl</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/20 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -1661,7 +1661,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月12日 15:17:58</t>
+    <t xml:space="preserve">2022年04月19日 20:14:17</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2951,10 +2951,10 @@
     <t xml:space="preserve">TxAuthority</t>
   </si>
   <si>
-    <t xml:space="preserve">權限檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月28日 16:03:18</t>
+    <t xml:space="preserve">群組權限檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月20日 09:41:36</t>
   </si>
   <si>
     <t xml:space="preserve">TxAuthorize</t>
@@ -3017,7 +3017,7 @@
     <t xml:space="preserve">錯誤代碼</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月15日 11:27:12</t>
+    <t xml:space="preserve">2022年04月20日 09:49:59</t>
   </si>
   <si>
     <t xml:space="preserve">TxFile</t>
@@ -3071,7 +3071,7 @@
     <t xml:space="preserve">印表機設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月30日 18:31:35</t>
+    <t xml:space="preserve">2022年04月20日 09:49:58</t>
   </si>
   <si>
     <t xml:space="preserve">TxProcess</t>

</xml_diff>

<commit_message>
xiangwei manually 20220421 morning version
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月19日 14:47:14</t>
+    <t xml:space="preserve">2022年04月21日 12:53:14</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月19日 14:45:48</t>
+    <t xml:space="preserve">2022年04月21日 13:06:10</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/21 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -176,7 +176,7 @@
     <t xml:space="preserve">擔保品不動產建物檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月20日 15:05:47</t>
+    <t xml:space="preserve">2022年04月21日 13:49:53</t>
   </si>
   <si>
     <t xml:space="preserve">ClBuildingOwner</t>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月13日 09:08:50</t>
+    <t xml:space="preserve">2022年04月21日 17:16:12</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月21日 12:53:14</t>
+    <t xml:space="preserve">2022年04月21日 16:52:04</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -932,7 +932,7 @@
     <t xml:space="preserve">介紹人業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月24日 11:14:15</t>
+    <t xml:space="preserve">2022年04月21日 15:05:37</t>
   </si>
   <si>
     <t xml:space="preserve">HlThreeLaqhcp</t>
@@ -1373,7 +1373,7 @@
     <t xml:space="preserve">指標利率檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月07日 15:20:48</t>
+    <t xml:space="preserve">2022年04月21日 13:56:28</t>
   </si>
   <si>
     <t xml:space="preserve">CdBcm</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">營業單位課組別檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月29日 16:03:52</t>
+    <t xml:space="preserve">2022年04月21日 16:32:09</t>
   </si>
   <si>
     <t xml:space="preserve">CdBudget</t>
@@ -2780,7 +2780,7 @@
     <t xml:space="preserve">報表用公司代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月10日 10:15:15</t>
+    <t xml:space="preserve">2022年04月21日 16:33:25</t>
   </si>
   <si>
     <t xml:space="preserve">SlipEbsRecord</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/25 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1046">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -1232,15 +1232,6 @@
     <t xml:space="preserve">2021年10月19日 14:25:35</t>
   </si>
   <si>
-    <t xml:space="preserve">AcCheque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">應收票據資料檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年05月05日 17:27:16</t>
-  </si>
-  <si>
     <t xml:space="preserve">AcClose</t>
   </si>
   <si>
@@ -1643,7 +1634,7 @@
     <t xml:space="preserve">批次工作主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月01日 10:35:28</t>
+    <t xml:space="preserve">2022年04月25日 11:07:36</t>
   </si>
   <si>
     <t xml:space="preserve">StgCdEmp</t>
@@ -1665,15 +1656,6 @@
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CoreAcMain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">核心會計總帳檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年05月05日 12:16:52</t>
   </si>
   <si>
     <t xml:space="preserve">CreditRating</t>
@@ -3279,7 +3261,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="2">
@@ -5669,7 +5651,7 @@
         <v>407</v>
       </c>
       <c r="D134" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcCheque.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcClose.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E134" s="1" t="s">
@@ -5687,7 +5669,7 @@
         <v>410</v>
       </c>
       <c r="D135" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcClose.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -5705,7 +5687,7 @@
         <v>413</v>
       </c>
       <c r="D136" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -5723,7 +5705,7 @@
         <v>416</v>
       </c>
       <c r="D137" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanRenew.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -5741,7 +5723,7 @@
         <v>419</v>
       </c>
       <c r="D138" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanRenew.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -5759,7 +5741,7 @@
         <v>422</v>
       </c>
       <c r="D139" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcReceivable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E139" s="1" t="s">
@@ -5777,7 +5759,7 @@
         <v>425</v>
       </c>
       <c r="D140" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcReceivable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcBook.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E140" s="1" t="s">
@@ -5795,7 +5777,7 @@
         <v>428</v>
       </c>
       <c r="D141" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcBook.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E141" s="1" t="s">
@@ -5813,7 +5795,7 @@
         <v>431</v>
       </c>
       <c r="D142" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAoDept.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E142" s="1" t="s">
@@ -5831,7 +5813,7 @@
         <v>434</v>
       </c>
       <c r="D143" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAoDept.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E143" s="1" t="s">
@@ -5849,7 +5831,7 @@
         <v>437</v>
       </c>
       <c r="D144" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -5867,7 +5849,7 @@
         <v>440</v>
       </c>
       <c r="D145" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E145" s="1" t="s">
@@ -5885,7 +5867,7 @@
         <v>443</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E146" s="1" t="s">
@@ -5903,7 +5885,7 @@
         <v>446</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBankOld.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E147" s="1" t="s">
@@ -5921,7 +5903,7 @@
         <v>449</v>
       </c>
       <c r="D148" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBankOld.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E148" s="1" t="s">
@@ -5939,7 +5921,7 @@
         <v>452</v>
       </c>
       <c r="D149" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E149" s="1" t="s">
@@ -5957,7 +5939,7 @@
         <v>455</v>
       </c>
       <c r="D150" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E150" s="1" t="s">
@@ -5975,7 +5957,7 @@
         <v>458</v>
       </c>
       <c r="D151" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E151" s="1" t="s">
@@ -5993,7 +5975,7 @@
         <v>461</v>
       </c>
       <c r="D152" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E152" s="1" t="s">
@@ -6011,7 +5993,7 @@
         <v>464</v>
       </c>
       <c r="D153" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E153" s="1" t="s">
@@ -6029,7 +6011,7 @@
         <v>467</v>
       </c>
       <c r="D154" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -6047,7 +6029,7 @@
         <v>470</v>
       </c>
       <c r="D155" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -6065,7 +6047,7 @@
         <v>473</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -6083,7 +6065,7 @@
         <v>476</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -6101,7 +6083,7 @@
         <v>479</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E158" s="1" t="s">
@@ -6119,7 +6101,7 @@
         <v>482</v>
       </c>
       <c r="D159" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E159" s="1" t="s">
@@ -6137,7 +6119,7 @@
         <v>485</v>
       </c>
       <c r="D160" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -6155,7 +6137,7 @@
         <v>488</v>
       </c>
       <c r="D161" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E161" s="1" t="s">
@@ -6173,7 +6155,7 @@
         <v>491</v>
       </c>
       <c r="D162" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -6191,7 +6173,7 @@
         <v>494</v>
       </c>
       <c r="D163" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -6209,7 +6191,7 @@
         <v>497</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -6227,7 +6209,7 @@
         <v>500</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E165" s="1" t="s">
@@ -6245,7 +6227,7 @@
         <v>503</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -6263,7 +6245,7 @@
         <v>506</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -6281,7 +6263,7 @@
         <v>509</v>
       </c>
       <c r="D168" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E168" s="1" t="s">
@@ -6299,7 +6281,7 @@
         <v>512</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E169" s="1" t="s">
@@ -6317,7 +6299,7 @@
         <v>515</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E170" s="1" t="s">
@@ -6335,7 +6317,7 @@
         <v>518</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E171" s="1" t="s">
@@ -6353,7 +6335,7 @@
         <v>521</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E172" s="1" t="s">
@@ -6371,7 +6353,7 @@
         <v>524</v>
       </c>
       <c r="D173" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E173" s="1" t="s">
@@ -6389,7 +6371,7 @@
         <v>527</v>
       </c>
       <c r="D174" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E174" s="1" t="s">
@@ -6407,7 +6389,7 @@
         <v>530</v>
       </c>
       <c r="D175" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E175" s="1" t="s">
@@ -6425,7 +6407,7 @@
         <v>533</v>
       </c>
       <c r="D176" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E176" s="1" t="s">
@@ -6443,7 +6425,7 @@
         <v>536</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E177" s="1" t="s">
@@ -6461,7 +6443,7 @@
         <v>539</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E178" s="1" t="s">
@@ -6479,7 +6461,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6497,7 +6479,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6506,25 +6488,25 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="s">
-        <v>399</v>
+        <v>547</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>551</v>
@@ -6533,7 +6515,7 @@
         <v>552</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CoreAcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6542,7 +6524,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>554</v>
@@ -6551,7 +6533,7 @@
         <v>555</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6560,7 +6542,7 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>557</v>
@@ -6569,7 +6551,7 @@
         <v>558</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6578,7 +6560,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>560</v>
@@ -6587,7 +6569,7 @@
         <v>561</v>
       </c>
       <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E185" s="1" t="s">
@@ -6596,7 +6578,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>563</v>
@@ -6605,7 +6587,7 @@
         <v>564</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6614,7 +6596,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>566</v>
@@ -6623,7 +6605,7 @@
         <v>567</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6632,7 +6614,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>569</v>
@@ -6641,7 +6623,7 @@
         <v>570</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6650,7 +6632,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>572</v>
@@ -6659,7 +6641,7 @@
         <v>573</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6668,7 +6650,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>575</v>
@@ -6677,7 +6659,7 @@
         <v>576</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E190" s="1" t="s">
@@ -6686,7 +6668,7 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6695,7 +6677,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6704,7 +6686,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6713,7 +6695,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6722,7 +6704,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6731,7 +6713,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6740,7 +6722,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6749,7 +6731,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6758,7 +6740,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6767,7 +6749,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6776,7 +6758,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6785,7 +6767,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6794,7 +6776,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6803,7 +6785,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6812,7 +6794,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6821,7 +6803,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6830,7 +6812,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6839,7 +6821,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6848,43 +6830,43 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>612</v>
@@ -6893,7 +6875,7 @@
         <v>613</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -6902,7 +6884,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>615</v>
@@ -6911,7 +6893,7 @@
         <v>616</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -6920,7 +6902,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>618</v>
@@ -6929,7 +6911,7 @@
         <v>619</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -6938,7 +6920,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>621</v>
@@ -6947,7 +6929,7 @@
         <v>622</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -6956,7 +6938,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>624</v>
@@ -6965,7 +6947,7 @@
         <v>625</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -6974,7 +6956,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>627</v>
@@ -6983,7 +6965,7 @@
         <v>628</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -6992,7 +6974,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>630</v>
@@ -7001,7 +6983,7 @@
         <v>631</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7010,7 +6992,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>633</v>
@@ -7019,7 +7001,7 @@
         <v>634</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7028,7 +7010,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>636</v>
@@ -7037,7 +7019,7 @@
         <v>637</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7046,7 +7028,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>639</v>
@@ -7055,7 +7037,7 @@
         <v>640</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -7064,7 +7046,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7073,7 +7055,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7082,7 +7064,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7091,7 +7073,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7100,7 +7082,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7109,7 +7091,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7118,7 +7100,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7127,7 +7109,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7136,7 +7118,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7145,7 +7127,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7154,7 +7136,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7163,7 +7145,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7172,1348 +7154,1348 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D218" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E218" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B219" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="C219" s="1" t="s">
+      <c r="D219" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E219" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D220" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E220" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B221" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C221" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="C221" s="1" t="s">
+      <c r="D221" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D222" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E222" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B223" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="D223" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B224" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D224" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E224" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C225" s="1" t="s">
+      <c r="D225" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E225" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B226" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D226" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E226" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B227" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C227" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="C227" s="1" t="s">
+      <c r="D227" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E227" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D228" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E228" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B229" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C229" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="C229" s="1" t="s">
+      <c r="D229" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E229" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B230" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D230" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B231" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C231" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="C231" s="1" t="s">
+      <c r="D231" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E231" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B232" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D232" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>696</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C233" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C233" s="1" t="s">
+      <c r="D233" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E233" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B234" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D234" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E234" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="C235" s="1" t="s">
+      <c r="D235" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E235" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B236" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D236" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E236" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C237" s="1" t="s">
+      <c r="D237" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B238" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D238" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="C239" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="C239" s="1" t="s">
+      <c r="D239" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E239" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B240" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D240" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E240" s="1" t="s">
         <v>716</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="C241" s="1" t="s">
+      <c r="D241" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E241" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D242" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B243" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C243" s="1" t="s">
+      <c r="D243" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E243" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B244" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D244" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C245" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C245" s="1" t="s">
+      <c r="D245" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E245" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B246" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D246" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>731</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B247" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="C247" s="1" t="s">
+      <c r="D247" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E247" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B248" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D248" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E248" s="1" t="s">
         <v>736</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C249" s="1" t="s">
+      <c r="D249" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E249" s="1" t="s">
         <v>739</v>
-      </c>
-      <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B250" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="D250" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D251" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E251" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>744</v>
+        <v>708</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D253" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E253" s="1" t="s">
         <v>748</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B254" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D254" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="C255" s="1" t="s">
+      <c r="D255" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E255" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B256" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D256" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E256" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="C257" s="1" t="s">
+      <c r="D257" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B258" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D258" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>760</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B259" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="C259" s="1" t="s">
+      <c r="D259" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E259" s="1" t="s">
         <v>763</v>
-      </c>
-      <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B260" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D260" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E260" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="C261" s="1" t="s">
+      <c r="D261" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E261" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B262" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D262" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E262" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="C263" s="1" t="s">
+      <c r="D263" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E263" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B264" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D264" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E264" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B265" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C265" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="C265" s="1" t="s">
+      <c r="D265" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E265" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B266" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D266" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E266" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="C266" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B267" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C267" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="C267" s="1" t="s">
+      <c r="D267" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E267" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B268" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="D268" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E268" s="1" t="s">
         <v>785</v>
-      </c>
-      <c r="C268" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B269" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="C269" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="C269" s="1" t="s">
+      <c r="D269" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E269" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B270" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D270" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E270" s="1" t="s">
         <v>790</v>
-      </c>
-      <c r="C270" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C271" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="C271" s="1" t="s">
+      <c r="D271" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E271" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B272" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D272" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E272" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C273" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C273" s="1" t="s">
+      <c r="D273" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E273" s="1" t="s">
         <v>798</v>
-      </c>
-      <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B274" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D274" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E274" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="C275" s="1" t="s">
+      <c r="D275" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E275" s="1" t="s">
         <v>803</v>
-      </c>
-      <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B276" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="D276" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E276" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="C276" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="C277" s="1" t="s">
+      <c r="D277" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E277" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B278" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="D278" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E278" s="1" t="s">
         <v>810</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="C279" s="1" t="s">
+      <c r="D279" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E279" s="1" t="s">
         <v>813</v>
-      </c>
-      <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E279" s="1" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B280" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D280" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E280" s="1" t="s">
         <v>815</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E280" s="1" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="C281" s="1" t="s">
+      <c r="D281" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E281" s="1" t="s">
         <v>818</v>
-      </c>
-      <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B282" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D282" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E282" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="C283" s="1" t="s">
+      <c r="D283" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E283" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B284" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D284" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E284" s="1" t="s">
         <v>825</v>
-      </c>
-      <c r="C284" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E284" s="1" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C285" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C285" s="1" t="s">
+      <c r="D285" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E285" s="1" t="s">
         <v>828</v>
-      </c>
-      <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B286" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D286" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E286" s="1" t="s">
         <v>830</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="C287" s="1" t="s">
+      <c r="D287" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E287" s="1" t="s">
         <v>833</v>
-      </c>
-      <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E287" s="1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B288" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="D288" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E288" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="C289" s="1" t="s">
+      <c r="D289" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E289" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B290" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D290" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E290" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="C291" s="1" t="s">
+      <c r="D291" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E291" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B292" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C292" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="C292" s="1" t="s">
-        <v>843</v>
-      </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
@@ -8522,7 +8504,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>847</v>
@@ -8531,7 +8513,7 @@
         <v>848</v>
       </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
@@ -8540,7 +8522,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>850</v>
@@ -8549,7 +8531,7 @@
         <v>851</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
@@ -8558,7 +8540,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>853</v>
@@ -8567,7 +8549,7 @@
         <v>854</v>
       </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
@@ -8576,7 +8558,7 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>856</v>
@@ -8585,7 +8567,7 @@
         <v>857</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -8594,7 +8576,7 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>859</v>
@@ -8603,7 +8585,7 @@
         <v>860</v>
       </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
@@ -8612,7 +8594,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>862</v>
@@ -8621,7 +8603,7 @@
         <v>863</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
@@ -8630,43 +8612,43 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>611</v>
+        <v>865</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>611</v>
+        <v>865</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>872</v>
@@ -8675,7 +8657,7 @@
         <v>873</v>
       </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
@@ -8684,7 +8666,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>875</v>
@@ -8693,7 +8675,7 @@
         <v>876</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
@@ -8702,7 +8684,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>878</v>
@@ -8711,7 +8693,7 @@
         <v>879</v>
       </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
@@ -8720,7 +8702,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>881</v>
@@ -8729,7 +8711,7 @@
         <v>882</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8738,7 +8720,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>884</v>
@@ -8747,7 +8729,7 @@
         <v>885</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8756,7 +8738,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>887</v>
@@ -8765,7 +8747,7 @@
         <v>888</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8774,7 +8756,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>890</v>
@@ -8783,7 +8765,7 @@
         <v>891</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8792,7 +8774,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>893</v>
@@ -8801,7 +8783,7 @@
         <v>894</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8810,7 +8792,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>896</v>
@@ -8819,7 +8801,7 @@
         <v>897</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8828,7 +8810,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>899</v>
@@ -8837,7 +8819,7 @@
         <v>900</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8846,7 +8828,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>902</v>
@@ -8855,7 +8837,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8864,7 +8846,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8873,7 +8855,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8882,7 +8864,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -8891,7 +8873,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -8900,7 +8882,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -8909,7 +8891,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -8918,7 +8900,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -8927,7 +8909,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -8936,7 +8918,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -8945,7 +8927,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8954,7 +8936,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -8963,7 +8945,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8972,7 +8954,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -8981,7 +8963,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -8990,7 +8972,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -8999,7 +8981,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9008,7 +8990,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9017,7 +8999,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9026,7 +9008,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9035,7 +9017,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9044,43 +9026,43 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>871</v>
+        <v>935</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>871</v>
+        <v>935</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>942</v>
@@ -9089,7 +9071,7 @@
         <v>943</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9098,7 +9080,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>945</v>
@@ -9107,7 +9089,7 @@
         <v>946</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9116,7 +9098,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>948</v>
@@ -9125,7 +9107,7 @@
         <v>949</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9134,7 +9116,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>951</v>
@@ -9143,7 +9125,7 @@
         <v>952</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9152,7 +9134,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>954</v>
@@ -9161,7 +9143,7 @@
         <v>955</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9170,7 +9152,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>957</v>
@@ -9179,7 +9161,7 @@
         <v>958</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9188,7 +9170,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>960</v>
@@ -9197,7 +9179,7 @@
         <v>961</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9206,7 +9188,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>963</v>
@@ -9215,7 +9197,7 @@
         <v>964</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9224,7 +9206,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>966</v>
@@ -9233,7 +9215,7 @@
         <v>967</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9242,7 +9224,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>969</v>
@@ -9251,7 +9233,7 @@
         <v>970</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9260,7 +9242,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>972</v>
@@ -9269,7 +9251,7 @@
         <v>973</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9278,7 +9260,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9287,7 +9269,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9296,7 +9278,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9305,7 +9287,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9314,7 +9296,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9323,7 +9305,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9332,7 +9314,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9341,7 +9323,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9350,7 +9332,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9359,7 +9341,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9368,7 +9350,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9377,7 +9359,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9386,7 +9368,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9395,7 +9377,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9404,7 +9386,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9413,7 +9395,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9422,7 +9404,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9431,7 +9413,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9440,7 +9422,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9449,7 +9431,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9458,7 +9440,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9467,7 +9449,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9476,7 +9458,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9485,7 +9467,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9494,7 +9476,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9503,7 +9485,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9512,52 +9494,52 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C348" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D348" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E348" s="1" t="s">
         <v>1015</v>
-      </c>
-      <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E348" s="1" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B349" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C349" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="C349" s="1" t="s">
+      <c r="D349" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E349" s="1" t="s">
         <v>1018</v>
-      </c>
-      <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E349" s="1" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B350" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C350" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="C350" s="1" t="s">
-        <v>1006</v>
-      </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9566,7 +9548,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1022</v>
@@ -9575,7 +9557,7 @@
         <v>1023</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9584,52 +9566,52 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1025</v>
       </c>
       <c r="C352" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D352" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerTest.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E352" s="1" t="s">
         <v>1026</v>
-      </c>
-      <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E352" s="1" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B353" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C353" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C353" s="1" t="s">
+      <c r="D353" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E353" s="1" t="s">
         <v>1029</v>
-      </c>
-      <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E353" s="1" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B354" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C354" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="C354" s="1" t="s">
-        <v>1026</v>
-      </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerTest.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9638,7 +9620,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1033</v>
@@ -9647,7 +9629,7 @@
         <v>1034</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9656,7 +9638,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1036</v>
@@ -9665,7 +9647,7 @@
         <v>1037</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9674,7 +9656,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1039</v>
@@ -9683,7 +9665,7 @@
         <v>1040</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9692,7 +9674,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1042</v>
@@ -9701,47 +9683,11 @@
         <v>1043</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
         <v>1044</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" s="1" t="s">
-        <v>941</v>
-      </c>
-      <c r="B359" s="1" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C359" s="1" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E359" s="1" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" s="1" t="s">
-        <v>941</v>
-      </c>
-      <c r="B360" s="1" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C360" s="1" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E360" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/26 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1044">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月21日 18:31:53</t>
+    <t xml:space="preserve">2022年04月26日 16:25:06</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -3087,12 +3087,6 @@
   </si>
   <si>
     <t xml:space="preserve">2021年11月19日 18:33:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxTellerTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月01日 13:02:18</t>
   </si>
   <si>
     <t xml:space="preserve">TxTemp</t>
@@ -3261,7 +3255,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="2">
@@ -9572,14 +9566,14 @@
         <v>1025</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerTest.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="353">
@@ -9587,17 +9581,17 @@
         <v>935</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="354">
@@ -9605,17 +9599,17 @@
         <v>935</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="355">
@@ -9623,17 +9617,17 @@
         <v>935</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="356">
@@ -9641,17 +9635,17 @@
         <v>935</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="357">
@@ -9659,35 +9653,17 @@
         <v>935</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" s="1" t="s">
-        <v>935</v>
-      </c>
-      <c r="B358" s="1" t="s">
         <v>1042</v>
-      </c>
-      <c r="C358" s="1" t="s">
-        <v>1043</v>
-      </c>
-      <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E358" s="1" t="s">
-        <v>1044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/27 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -530,7 +530,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 15:56:01</t>
+    <t xml:space="preserve">2022年04月26日 17:44:19</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月11日 21:22:15</t>
+    <t xml:space="preserve">2022年04月26日 17:44:11</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1247,7 +1247,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月11日 11:35:06</t>
+    <t xml:space="preserve">2022年04月26日 19:39:38</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/28 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1047">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -1466,6 +1466,15 @@
     <t xml:space="preserve">2022年02月09日 13:53:03</t>
   </si>
   <si>
+    <t xml:space="preserve">CdConvertCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代碼轉換檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月28日 16:39:43</t>
+  </si>
+  <si>
     <t xml:space="preserve">CdEmp</t>
   </si>
   <si>
@@ -2837,7 +2846,7 @@
     <t xml:space="preserve">AML定審資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月28日 14:05:55</t>
+    <t xml:space="preserve">2022年04月28日 14:17:55</t>
   </si>
   <si>
     <t xml:space="preserve">TxAmlLog</t>
@@ -3255,7 +3264,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1043</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="2">
@@ -6113,7 +6122,7 @@
         <v>485</v>
       </c>
       <c r="D160" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdConvertCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -6131,7 +6140,7 @@
         <v>488</v>
       </c>
       <c r="D161" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E161" s="1" t="s">
@@ -6149,7 +6158,7 @@
         <v>491</v>
       </c>
       <c r="D162" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -6167,7 +6176,7 @@
         <v>494</v>
       </c>
       <c r="D163" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -6185,7 +6194,7 @@
         <v>497</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -6203,7 +6212,7 @@
         <v>500</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E165" s="1" t="s">
@@ -6221,7 +6230,7 @@
         <v>503</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -6239,7 +6248,7 @@
         <v>506</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -6257,7 +6266,7 @@
         <v>509</v>
       </c>
       <c r="D168" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E168" s="1" t="s">
@@ -6275,7 +6284,7 @@
         <v>512</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E169" s="1" t="s">
@@ -6293,7 +6302,7 @@
         <v>515</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E170" s="1" t="s">
@@ -6311,7 +6320,7 @@
         <v>518</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E171" s="1" t="s">
@@ -6329,7 +6338,7 @@
         <v>521</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E172" s="1" t="s">
@@ -6347,7 +6356,7 @@
         <v>524</v>
       </c>
       <c r="D173" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E173" s="1" t="s">
@@ -6365,7 +6374,7 @@
         <v>527</v>
       </c>
       <c r="D174" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E174" s="1" t="s">
@@ -6383,7 +6392,7 @@
         <v>530</v>
       </c>
       <c r="D175" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E175" s="1" t="s">
@@ -6401,7 +6410,7 @@
         <v>533</v>
       </c>
       <c r="D176" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E176" s="1" t="s">
@@ -6419,7 +6428,7 @@
         <v>536</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E177" s="1" t="s">
@@ -6437,7 +6446,7 @@
         <v>539</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E178" s="1" t="s">
@@ -6455,7 +6464,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6473,7 +6482,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6482,25 +6491,25 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="C181" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="D181" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>551</v>
@@ -6509,7 +6518,7 @@
         <v>552</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6518,7 +6527,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>554</v>
@@ -6527,7 +6536,7 @@
         <v>555</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6536,7 +6545,7 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>557</v>
@@ -6545,7 +6554,7 @@
         <v>558</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6554,7 +6563,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>560</v>
@@ -6563,7 +6572,7 @@
         <v>561</v>
       </c>
       <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E185" s="1" t="s">
@@ -6572,7 +6581,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>563</v>
@@ -6581,7 +6590,7 @@
         <v>564</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6590,7 +6599,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>566</v>
@@ -6599,7 +6608,7 @@
         <v>567</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6608,7 +6617,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>569</v>
@@ -6617,7 +6626,7 @@
         <v>570</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6626,7 +6635,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>572</v>
@@ -6635,7 +6644,7 @@
         <v>573</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6644,7 +6653,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>575</v>
@@ -6653,7 +6662,7 @@
         <v>576</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E190" s="1" t="s">
@@ -6662,7 +6671,7 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6671,7 +6680,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6680,7 +6689,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6689,7 +6698,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6698,7 +6707,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6707,7 +6716,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6716,7 +6725,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6725,7 +6734,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6734,7 +6743,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6743,7 +6752,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6752,7 +6761,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6761,7 +6770,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6770,7 +6779,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6779,7 +6788,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6788,7 +6797,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6797,7 +6806,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6806,7 +6815,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6815,7 +6824,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6824,25 +6833,25 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="C200" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="D200" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E200" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>609</v>
@@ -6851,7 +6860,7 @@
         <v>610</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -6860,7 +6869,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>612</v>
@@ -6869,7 +6878,7 @@
         <v>613</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -6878,7 +6887,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>615</v>
@@ -6887,7 +6896,7 @@
         <v>616</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -6896,7 +6905,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>618</v>
@@ -6905,7 +6914,7 @@
         <v>619</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -6914,7 +6923,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>621</v>
@@ -6923,7 +6932,7 @@
         <v>622</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -6932,7 +6941,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>624</v>
@@ -6941,7 +6950,7 @@
         <v>625</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -6950,7 +6959,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>627</v>
@@ -6959,7 +6968,7 @@
         <v>628</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -6968,7 +6977,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>630</v>
@@ -6977,7 +6986,7 @@
         <v>631</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -6986,7 +6995,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>633</v>
@@ -6995,7 +7004,7 @@
         <v>634</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7004,7 +7013,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>636</v>
@@ -7013,7 +7022,7 @@
         <v>637</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7022,7 +7031,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>639</v>
@@ -7031,7 +7040,7 @@
         <v>640</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -7040,7 +7049,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7049,7 +7058,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7058,7 +7067,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7067,7 +7076,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7076,7 +7085,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7085,7 +7094,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7094,7 +7103,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7103,7 +7112,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7112,7 +7121,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7121,7 +7130,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7130,7 +7139,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7139,7 +7148,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7148,34 +7157,34 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7184,34 +7193,34 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>665</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7220,34 +7229,34 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>670</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7256,34 +7265,34 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>675</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7292,34 +7301,34 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>680</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7328,34 +7337,34 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>685</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7364,34 +7373,34 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>690</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
@@ -7400,34 +7409,34 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>695</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
@@ -7436,34 +7445,34 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>700</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
@@ -7472,34 +7481,34 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>705</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
@@ -7508,34 +7517,34 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>710</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
@@ -7544,34 +7553,34 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>715</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
@@ -7580,34 +7589,34 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>720</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
@@ -7616,34 +7625,34 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>725</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
@@ -7652,34 +7661,34 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>730</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
@@ -7688,34 +7697,34 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>735</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
@@ -7724,70 +7733,70 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>740</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>708</v>
+        <v>741</v>
       </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>747</v>
+        <v>711</v>
       </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
@@ -7796,34 +7805,34 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>749</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
@@ -7832,34 +7841,34 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
@@ -7868,34 +7877,34 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>759</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
@@ -7904,34 +7913,34 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>764</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
@@ -7940,34 +7949,34 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>769</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
@@ -7976,34 +7985,34 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>774</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
@@ -8012,34 +8021,34 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>779</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -8048,34 +8057,34 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>784</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
@@ -8084,34 +8093,34 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>789</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
@@ -8120,34 +8129,34 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>794</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
@@ -8156,34 +8165,34 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>799</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
@@ -8192,34 +8201,34 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>804</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
@@ -8228,34 +8237,34 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>809</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
@@ -8264,34 +8273,34 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>814</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
@@ -8300,34 +8309,34 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>819</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
@@ -8336,34 +8345,34 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>824</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
@@ -8372,34 +8381,34 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>829</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -8408,34 +8417,34 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>834</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
@@ -8444,34 +8453,34 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>839</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
@@ -8480,7 +8489,7 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>844</v>
@@ -8489,7 +8498,7 @@
         <v>845</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
@@ -8498,7 +8507,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>847</v>
@@ -8507,7 +8516,7 @@
         <v>848</v>
       </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
@@ -8516,7 +8525,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>850</v>
@@ -8525,7 +8534,7 @@
         <v>851</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
@@ -8534,7 +8543,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>853</v>
@@ -8543,7 +8552,7 @@
         <v>854</v>
       </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
@@ -8552,7 +8561,7 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>856</v>
@@ -8561,7 +8570,7 @@
         <v>857</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -8570,7 +8579,7 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>859</v>
@@ -8579,7 +8588,7 @@
         <v>860</v>
       </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
@@ -8588,7 +8597,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>862</v>
@@ -8597,7 +8606,7 @@
         <v>863</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
@@ -8606,25 +8615,25 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B299" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="B299" s="1" t="s">
+      <c r="C299" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="C299" s="1" t="s">
+      <c r="D299" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E299" s="1" t="s">
         <v>867</v>
-      </c>
-      <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>869</v>
@@ -8633,7 +8642,7 @@
         <v>870</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
@@ -8642,7 +8651,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>872</v>
@@ -8651,7 +8660,7 @@
         <v>873</v>
       </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
@@ -8660,7 +8669,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>875</v>
@@ -8669,7 +8678,7 @@
         <v>876</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
@@ -8678,7 +8687,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>878</v>
@@ -8687,7 +8696,7 @@
         <v>879</v>
       </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
@@ -8696,7 +8705,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>881</v>
@@ -8705,7 +8714,7 @@
         <v>882</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8714,7 +8723,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>884</v>
@@ -8723,7 +8732,7 @@
         <v>885</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8732,7 +8741,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>887</v>
@@ -8741,7 +8750,7 @@
         <v>888</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8750,7 +8759,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>890</v>
@@ -8759,7 +8768,7 @@
         <v>891</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8768,7 +8777,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>893</v>
@@ -8777,7 +8786,7 @@
         <v>894</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8786,7 +8795,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>896</v>
@@ -8795,7 +8804,7 @@
         <v>897</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8804,7 +8813,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>899</v>
@@ -8813,7 +8822,7 @@
         <v>900</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8822,7 +8831,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>902</v>
@@ -8831,7 +8840,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8840,7 +8849,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8849,7 +8858,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8858,7 +8867,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -8867,7 +8876,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -8876,7 +8885,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -8885,7 +8894,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -8894,7 +8903,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -8903,7 +8912,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -8912,7 +8921,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -8921,7 +8930,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8930,7 +8939,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -8939,7 +8948,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8948,7 +8957,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -8957,7 +8966,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -8966,7 +8975,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -8975,7 +8984,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -8984,7 +8993,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -8993,7 +9002,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9002,7 +9011,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9011,7 +9020,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9020,25 +9029,25 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="C322" s="1" t="s">
+      <c r="D322" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E322" s="1" t="s">
         <v>937</v>
-      </c>
-      <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E322" s="1" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>939</v>
@@ -9047,7 +9056,7 @@
         <v>940</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9056,7 +9065,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>942</v>
@@ -9065,7 +9074,7 @@
         <v>943</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9074,7 +9083,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>945</v>
@@ -9083,7 +9092,7 @@
         <v>946</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9092,7 +9101,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>948</v>
@@ -9101,7 +9110,7 @@
         <v>949</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9110,7 +9119,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>951</v>
@@ -9119,7 +9128,7 @@
         <v>952</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9128,7 +9137,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>954</v>
@@ -9137,7 +9146,7 @@
         <v>955</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9146,7 +9155,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>957</v>
@@ -9155,7 +9164,7 @@
         <v>958</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9164,7 +9173,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>960</v>
@@ -9173,7 +9182,7 @@
         <v>961</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9182,7 +9191,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>963</v>
@@ -9191,7 +9200,7 @@
         <v>964</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9200,7 +9209,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>966</v>
@@ -9209,7 +9218,7 @@
         <v>967</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9218,7 +9227,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>969</v>
@@ -9227,7 +9236,7 @@
         <v>970</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9236,7 +9245,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>972</v>
@@ -9245,7 +9254,7 @@
         <v>973</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9254,7 +9263,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9263,7 +9272,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9272,7 +9281,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9281,7 +9290,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9290,7 +9299,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9299,7 +9308,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9308,7 +9317,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9317,7 +9326,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9326,7 +9335,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9335,7 +9344,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9344,7 +9353,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9353,7 +9362,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9362,7 +9371,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9371,7 +9380,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9380,7 +9389,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9389,7 +9398,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9398,7 +9407,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9407,7 +9416,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9416,7 +9425,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9425,7 +9434,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9434,7 +9443,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9443,7 +9452,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9452,7 +9461,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9461,7 +9470,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9470,7 +9479,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9479,7 +9488,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9488,34 +9497,34 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>1000</v>
+        <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>1017</v>
+        <v>1003</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9524,7 +9533,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1019</v>
@@ -9533,7 +9542,7 @@
         <v>1020</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9542,7 +9551,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1022</v>
@@ -9551,7 +9560,7 @@
         <v>1023</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9560,7 +9569,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1025</v>
@@ -9569,7 +9578,7 @@
         <v>1026</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9578,7 +9587,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1028</v>
@@ -9587,7 +9596,7 @@
         <v>1029</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9596,7 +9605,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1031</v>
@@ -9605,7 +9614,7 @@
         <v>1032</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9614,7 +9623,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1034</v>
@@ -9623,7 +9632,7 @@
         <v>1035</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9632,7 +9641,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1037</v>
@@ -9641,7 +9650,7 @@
         <v>1038</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9650,7 +9659,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1040</v>
@@ -9659,11 +9668,29 @@
         <v>1041</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
         <v>1042</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D358" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>1045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/06 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -347,7 +347,7 @@
     <t xml:space="preserve">擔保品股票檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月02日 10:55:04</t>
+    <t xml:space="preserve">2022年05月04日 09:29:11</t>
   </si>
   <si>
     <t xml:space="preserve">CustDataCtrl</t>
@@ -383,7 +383,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月22日 10:24:10</t>
+    <t xml:space="preserve">2022年05月05日 11:26:01</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">帳務備忘錄明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月29日 10:35:51</t>
+    <t xml:space="preserve">2022年05月03日 09:48:14</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>
@@ -593,7 +593,7 @@
     <t xml:space="preserve">放款利率變動檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月09日 19:44:28</t>
+    <t xml:space="preserve">2022年05月06日 11:56:34</t>
   </si>
   <si>
     <t xml:space="preserve">LoanSynd</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月29日 10:16:44</t>
+    <t xml:space="preserve">2022年05月06日 13:15:24</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -932,7 +932,7 @@
     <t xml:space="preserve">介紹人業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月21日 15:05:37</t>
+    <t xml:space="preserve">2022年05月05日 18:07:24</t>
   </si>
   <si>
     <t xml:space="preserve">HlThreeLaqhcp</t>
@@ -941,7 +941,7 @@
     <t xml:space="preserve">單位、區部、部室業績累計檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月12日 11:54:32</t>
+    <t xml:space="preserve">2022年05月05日 18:11:22</t>
   </si>
   <si>
     <t xml:space="preserve">InnDocRecord</t>
@@ -950,7 +950,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:21:28</t>
+    <t xml:space="preserve">2022年05月04日 14:05:05</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -1472,7 +1472,7 @@
     <t xml:space="preserve">代碼轉換檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月28日 16:49:58</t>
+    <t xml:space="preserve">2022年05月03日 18:38:40</t>
   </si>
   <si>
     <t xml:space="preserve">CdEmp</t>
@@ -2579,7 +2579,7 @@
     <t xml:space="preserve">疑似洗錢交易訪談記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月11日 16:57:05</t>
+    <t xml:space="preserve">2022年05月03日 11:16:46</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyQ53</t>
@@ -2954,7 +2954,7 @@
     <t xml:space="preserve">主管授權紀錄</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月24日 19:54:15</t>
+    <t xml:space="preserve">2022年05月06日 16:50:41</t>
   </si>
   <si>
     <t xml:space="preserve">TxBizDate</t>
@@ -2999,7 +2999,7 @@
     <t xml:space="preserve">資料變更紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月17日 18:44:27</t>
+    <t xml:space="preserve">2022年04月29日 19:24:06</t>
   </si>
   <si>
     <t xml:space="preserve">TxErrCode</t>
@@ -3086,7 +3086,7 @@
     <t xml:space="preserve">使用者檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月12日 14:28:31</t>
+    <t xml:space="preserve">2022年05月06日 17:17:51</t>
   </si>
   <si>
     <t xml:space="preserve">TxTellerAuth</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/10 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">帳務備忘錄明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月03日 09:48:14</t>
+    <t xml:space="preserve">2022年05月10日 09:20:41</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月06日 13:15:24</t>
+    <t xml:space="preserve">2022年05月09日 17:54:56</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -2579,7 +2579,7 @@
     <t xml:space="preserve">疑似洗錢交易訪談記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月03日 11:16:46</t>
+    <t xml:space="preserve">2022年05月10日 10:33:59</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyQ53</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/17 週二 16:31:52.02
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">帳務備忘錄明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月10日 09:20:41</t>
+    <t xml:space="preserve">2022年05月17日 15:28:16</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>
@@ -731,7 +731,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月13日 14:49:38</t>
+    <t xml:space="preserve">2022年05月16日 14:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -941,7 +941,7 @@
     <t xml:space="preserve">介紹人業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月06日 19:11:28</t>
+    <t xml:space="preserve">2022年05月17日 14:29:51</t>
   </si>
   <si>
     <t xml:space="preserve">HlThreeLaqhcp</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月12日 13:09:06</t>
+    <t xml:space="preserve">2022年05月16日 18:45:21</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1517,7 +1517,7 @@
     <t xml:space="preserve">行業別代號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月08日 17:34:51</t>
+    <t xml:space="preserve">2022年05月17日 16:09:36</t>
   </si>
   <si>
     <t xml:space="preserve">CdInsurer</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/06/02 週四 17:29:22.55
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -311,7 +311,7 @@
     <t xml:space="preserve">擔保品他項權利檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月30日 11:43:41</t>
+    <t xml:space="preserve">2022年05月30日 15:16:14</t>
   </si>
   <si>
     <t xml:space="preserve">ClOwnerRelation</t>
@@ -383,7 +383,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月30日 11:43:43</t>
+    <t xml:space="preserve">2022年06月02日 09:59:18</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月29日 10:35:52</t>
+    <t xml:space="preserve">2022年06月02日 16:59:17</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月26日 11:19:16</t>
+    <t xml:space="preserve">2022年05月30日 12:10:19</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批入帳總數檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:00:42</t>
+    <t xml:space="preserve">2022年06月02日 10:32:15</t>
   </si>
   <si>
     <t xml:space="preserve">BatxOthers</t>
@@ -1148,7 +1148,7 @@
     <t xml:space="preserve">業績計算明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月12日 12:42:34</t>
+    <t xml:space="preserve">2022年05月31日 18:31:13</t>
   </si>
   <si>
     <t xml:space="preserve">PfInsCheck</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計借新還舊檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月26日 11:26:11</t>
+    <t xml:space="preserve">2022年06月02日 16:57:25</t>
   </si>
   <si>
     <t xml:space="preserve">AcMain</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月26日 11:32:13</t>
+    <t xml:space="preserve">2022年05月31日 12:56:40</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1400,7 +1400,7 @@
     <t xml:space="preserve">協辦獎勵津貼標準設定</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:36:27</t>
+    <t xml:space="preserve">2022年05月31日 18:31:19</t>
   </si>
   <si>
     <t xml:space="preserve">CdBranch</t>
@@ -1799,7 +1799,7 @@
     <t xml:space="preserve">IFRS9欄位清單4</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:59:26</t>
+    <t xml:space="preserve">2022年05月31日 19:20:52</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIfrs9Fp</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/06/10 週五 17:48:45.69
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月02日 16:59:17</t>
+    <t xml:space="preserve">2022年06月02日 17:24:51</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月30日 12:10:19</t>
+    <t xml:space="preserve">2022年06月10日 17:27:05</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/06/24 週五 17:47:42.62
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -530,7 +530,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月26日 17:44:19</t>
+    <t xml:space="preserve">2022年06月21日 15:18:34</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月17日 16:18:06</t>
+    <t xml:space="preserve">2022年06月20日 09:35:43</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1022,7 +1022,7 @@
     <t xml:space="preserve">最大債權撥付資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月05日 11:38:26</t>
+    <t xml:space="preserve">2022年06月24日 12:48:01</t>
   </si>
   <si>
     <t xml:space="preserve">NegAppr02</t>
@@ -1991,7 +1991,7 @@
     <t xml:space="preserve">聯徵放款月報資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:29:04</t>
+    <t xml:space="preserve">2022年06月22日 13:27:27</t>
   </si>
   <si>
     <t xml:space="preserve">JcicRel</t>
@@ -3095,7 +3095,7 @@
     <t xml:space="preserve">使用者檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月12日 17:24:14</t>
+    <t xml:space="preserve">2022年06月22日 16:24:45</t>
   </si>
   <si>
     <t xml:space="preserve">TxTellerAuth</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/06/27 週一 11:37:22.29
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月20日 09:35:43</t>
+    <t xml:space="preserve">2022年06月27日 08:58:18</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月26日 10:43:02</t>
+    <t xml:space="preserve">2022年06月27日 11:28:27</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計借新還舊檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月14日 10:21:42</t>
+    <t xml:space="preserve">2022年06月25日 19:55:49</t>
   </si>
   <si>
     <t xml:space="preserve">AcMain</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月31日 12:56:40</t>
+    <t xml:space="preserve">2022年06月27日 11:31:22</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/07/04 週一 11:38:11.84
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月02日 17:24:51</t>
+    <t xml:space="preserve">2022年06月27日 12:40:02</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -530,7 +530,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月21日 15:18:34</t>
+    <t xml:space="preserve">2022年07月01日 10:07:09</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月27日 08:58:18</t>
+    <t xml:space="preserve">2022年06月30日 09:35:33</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -611,7 +611,7 @@
     <t xml:space="preserve">聯貸案費用檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月24日 14:49:15</t>
+    <t xml:space="preserve">2022年06月29日 10:25:29</t>
   </si>
   <si>
     <t xml:space="preserve">L4-批次作業</t>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月27日 11:28:27</t>
+    <t xml:space="preserve">2022年06月27日 12:49:12</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1256,7 +1256,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月18日 12:17:17</t>
+    <t xml:space="preserve">2022年07月04日 09:58:33</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月27日 11:31:22</t>
+    <t xml:space="preserve">2022年07月01日 20:08:19</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/08/15 週一 18:59:13.58
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月27日 12:40:02</t>
+    <t xml:space="preserve">2022年08月08日 15:03:06</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月21日 18:53:58</t>
+    <t xml:space="preserve">2022年08月14日 06:43:09</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月18日 17:28:07</t>
+    <t xml:space="preserve">2022年08月04日 12:14:03</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批入帳總數檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月02日 10:32:15</t>
+    <t xml:space="preserve">2022年08月15日 12:54:13</t>
   </si>
   <si>
     <t xml:space="preserve">BatxOthers</t>
@@ -977,7 +977,7 @@
     <t xml:space="preserve">資金運用概況檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年02月22日 13:32:53</t>
+    <t xml:space="preserve">2022年08月10日 17:08:38</t>
   </si>
   <si>
     <t xml:space="preserve">InnLoanMeeting</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月15日 14:49:24</t>
+    <t xml:space="preserve">2022年08月12日 22:26:01</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -2027,7 +2027,7 @@
     <t xml:space="preserve">前置協商受理申請暨請求回報償權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:29:37</t>
+    <t xml:space="preserve">2022年08月15日 17:03:03</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ040Log</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/08/26 週五 17:20:49.47
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月04日 11:41:14</t>
+    <t xml:space="preserve">2022年08月24日 10:44:22</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -311,7 +311,7 @@
     <t xml:space="preserve">擔保品他項權利檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月30日 15:16:14</t>
+    <t xml:space="preserve">2022年08月26日 11:11:27</t>
   </si>
   <si>
     <t xml:space="preserve">ClOwnerRelation</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月14日 06:43:09</t>
+    <t xml:space="preserve">2022年08月26日 10:22:55</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月04日 12:14:03</t>
+    <t xml:space="preserve">2022年08月26日 17:12:56</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -767,7 +767,7 @@
     <t xml:space="preserve">火險佣金檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月14日 16:39:08</t>
+    <t xml:space="preserve">2022年08月19日 14:25:34</t>
   </si>
   <si>
     <t xml:space="preserve">InsuOrignal</t>
@@ -968,7 +968,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月04日 14:05:05</t>
+    <t xml:space="preserve">2022年08月19日 10:44:25</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月12日 22:26:01</t>
+    <t xml:space="preserve">2022年08月26日 11:42:12</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -2042,7 +2042,7 @@
     <t xml:space="preserve">協商開始暨停催通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:30:10</t>
+    <t xml:space="preserve">2022年08月19日 15:29:23</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ041Log</t>
@@ -2057,7 +2057,7 @@
     <t xml:space="preserve">回報無擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:30:32</t>
+    <t xml:space="preserve">2022年08月19日 15:33:04</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ042Log</t>
@@ -2072,7 +2072,7 @@
     <t xml:space="preserve">回報有擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:30:53</t>
+    <t xml:space="preserve">2022年08月19日 16:17:21</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ043Log</t>
@@ -2087,7 +2087,7 @@
     <t xml:space="preserve">請求同意債務清償方案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:31:28</t>
+    <t xml:space="preserve">2022年08月19日 15:31:04</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ044Log</t>
@@ -2102,7 +2102,7 @@
     <t xml:space="preserve">回報是否同意債務清償方案資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:31:53</t>
+    <t xml:space="preserve">2022年08月19日 15:31:26</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ045Log</t>
@@ -2117,7 +2117,7 @@
     <t xml:space="preserve">結案通知資料檔案格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:32:12</t>
+    <t xml:space="preserve">2022年08月19日 15:31:50</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ046Log</t>
@@ -2132,7 +2132,7 @@
     <t xml:space="preserve">金融機構無擔保債務協議資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:32:44</t>
+    <t xml:space="preserve">2022年08月19日 15:32:11</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ047Log</t>
@@ -2147,7 +2147,7 @@
     <t xml:space="preserve">債務人基本資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月14日 17:29:58</t>
+    <t xml:space="preserve">2022年08月19日 15:32:26</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ048Log</t>
@@ -2162,7 +2162,7 @@
     <t xml:space="preserve">債務清償方案法院認可資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:33:38</t>
+    <t xml:space="preserve">2022年08月19日 15:32:44</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ049Log</t>
@@ -2177,7 +2177,7 @@
     <t xml:space="preserve">債務人繳款資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:34:12</t>
+    <t xml:space="preserve">2022年08月19日 15:33:32</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ050Log</t>
@@ -2192,7 +2192,7 @@
     <t xml:space="preserve">延期繳款（喘息期）資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:34:30</t>
+    <t xml:space="preserve">2022年08月19日 15:34:02</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ051Log</t>
@@ -2207,7 +2207,7 @@
     <t xml:space="preserve">前置協商相關資料報送例外處理</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:34:48</t>
+    <t xml:space="preserve">2022年08月19日 15:34:12</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ052Log</t>
@@ -2222,7 +2222,7 @@
     <t xml:space="preserve">同意報送例外處理檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:35:03</t>
+    <t xml:space="preserve">2022年08月19日 15:34:29</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ053Log</t>
@@ -2237,7 +2237,7 @@
     <t xml:space="preserve">單獨全數受清償資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:35:28</t>
+    <t xml:space="preserve">2022年08月19日 15:34:48</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ054Log</t>
@@ -2252,7 +2252,7 @@
     <t xml:space="preserve">消債條例更生案件資料報送</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:36:16</t>
+    <t xml:space="preserve">2022年08月19日 15:35:11</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ055Log</t>
@@ -2267,7 +2267,7 @@
     <t xml:space="preserve">清算案件資料報送</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:36:39</t>
+    <t xml:space="preserve">2022年08月19日 15:35:31</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ056Log</t>
@@ -2279,7 +2279,7 @@
     <t xml:space="preserve">JcicZ060</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:36:53</t>
+    <t xml:space="preserve">2022年08月19日 15:35:46</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ060Log</t>
@@ -2294,7 +2294,7 @@
     <t xml:space="preserve">回報協商剩餘債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:37:04</t>
+    <t xml:space="preserve">2022年08月19日 15:35:59</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ061Log</t>
@@ -2309,7 +2309,7 @@
     <t xml:space="preserve">金融機構無擔保債務變更還款條件協議資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:37:16</t>
+    <t xml:space="preserve">2022年08月19日 15:36:14</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ062Log</t>
@@ -2324,7 +2324,7 @@
     <t xml:space="preserve">變更還款方案結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:37:33</t>
+    <t xml:space="preserve">2022年08月19日 15:36:26</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ063Log</t>
@@ -2339,7 +2339,7 @@
     <t xml:space="preserve">前置調解受理申請暨請求回報債權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:37:59</t>
+    <t xml:space="preserve">2022年08月19日 15:36:38</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ440Log</t>
@@ -2354,7 +2354,7 @@
     <t xml:space="preserve">前置調解回報無擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:38:12</t>
+    <t xml:space="preserve">2022年08月19日 15:36:49</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ442Log</t>
@@ -2369,7 +2369,7 @@
     <t xml:space="preserve">前置調解回報有擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:38:29</t>
+    <t xml:space="preserve">2022年08月19日 15:36:57</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ443Log</t>
@@ -2384,7 +2384,7 @@
     <t xml:space="preserve">前置調解債務人基本資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月15日 20:36:11</t>
+    <t xml:space="preserve">2022年08月19日 15:37:05</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ444Log</t>
@@ -2399,7 +2399,7 @@
     <t xml:space="preserve">前置調解結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:38:59</t>
+    <t xml:space="preserve">2022年08月19日 15:37:14</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ446Log</t>
@@ -2414,7 +2414,7 @@
     <t xml:space="preserve">前置調解金融機構無擔保債務協議資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:39:17</t>
+    <t xml:space="preserve">2022年08月19日 15:37:23</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ447Log</t>
@@ -2429,7 +2429,7 @@
     <t xml:space="preserve">前置調解無擔保債務還款分配資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:39:32</t>
+    <t xml:space="preserve">2022年08月19日 15:37:31</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ448Log</t>
@@ -2444,7 +2444,7 @@
     <t xml:space="preserve">前置調解債務人繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:39:47</t>
+    <t xml:space="preserve">2022年08月19日 15:37:39</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ450Log</t>
@@ -2459,7 +2459,7 @@
     <t xml:space="preserve">前置調解延期繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:40:01</t>
+    <t xml:space="preserve">2022年08月19日 15:37:49</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ451Log</t>
@@ -2474,7 +2474,7 @@
     <t xml:space="preserve">前置調解單獨全數受清償資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:40:19</t>
+    <t xml:space="preserve">2022年08月19日 15:37:58</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ454Log</t>
@@ -2489,7 +2489,7 @@
     <t xml:space="preserve">受理更生款項統一收付通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:40:29</t>
+    <t xml:space="preserve">2022年08月19日 15:38:17</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ570Log</t>
@@ -2504,7 +2504,7 @@
     <t xml:space="preserve">更生款項統一收付回報債權資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:41:14</t>
+    <t xml:space="preserve">2022年08月19日 15:38:27</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ571Log</t>
@@ -2519,7 +2519,7 @@
     <t xml:space="preserve">受理更生款項統一收付款項分配表資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:41:21</t>
+    <t xml:space="preserve">2022年08月19日 15:38:35</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ572Log</t>
@@ -2534,7 +2534,7 @@
     <t xml:space="preserve">更生債務人繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:41:32</t>
+    <t xml:space="preserve">2022年08月19日 15:38:43</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ573Log</t>
@@ -2549,7 +2549,7 @@
     <t xml:space="preserve">更生款項統一收付結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:41:44</t>
+    <t xml:space="preserve">2022年08月19日 15:38:51</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ574Log</t>
@@ -2564,7 +2564,7 @@
     <t xml:space="preserve">更生債權金額異動通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:41:57</t>
+    <t xml:space="preserve">2022年08月19日 15:38:58</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ575Log</t>
@@ -2588,7 +2588,7 @@
     <t xml:space="preserve">疑似洗錢交易合理性明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月18日 14:29:21</t>
+    <t xml:space="preserve">2022年08月25日 19:21:49</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryParas</t>
@@ -2981,7 +2981,7 @@
     <t xml:space="preserve">主管授權紀錄</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月26日 11:35:13</t>
+    <t xml:space="preserve">2022年08月17日 15:06:40</t>
   </si>
   <si>
     <t xml:space="preserve">TxBizDate</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/09/02 週五 12:19:21.83
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月26日 10:22:55</t>
+    <t xml:space="preserve">2022年09月01日 18:58:36</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月26日 17:12:56</t>
+    <t xml:space="preserve">2022年08月26日 20:49:58</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -2027,7 +2027,7 @@
     <t xml:space="preserve">前置協商受理申請暨請求回報償權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月15日 17:03:03</t>
+    <t xml:space="preserve">2022年09月01日 09:28:51</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ040Log</t>
@@ -2606,7 +2606,7 @@
     <t xml:space="preserve">疑似洗錢交易訪談記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月19日 11:51:45</t>
+    <t xml:space="preserve">2022年09月02日 11:42:31</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyQ53</t>
@@ -2672,7 +2672,7 @@
     <t xml:space="preserve">額度月報工作檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月25日 14:25:45</t>
+    <t xml:space="preserve">2022年08月31日 11:53:59</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM003</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/09/16 週五 17:39:19.43
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1059">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月08日 15:03:06</t>
+    <t xml:space="preserve">2022年09月15日 14:09:44</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -530,7 +530,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月01日 10:07:09</t>
+    <t xml:space="preserve">2022年09月08日 09:31:14</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -566,7 +566,7 @@
     <t xml:space="preserve">暫收款指定額度設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月14日 10:24:42</t>
+    <t xml:space="preserve">2022年09月14日 11:16:55</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月26日 16:25:06</t>
+    <t xml:space="preserve">2022年09月06日 10:51:09</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -668,7 +668,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月11日 13:12:31</t>
+    <t xml:space="preserve">2022年09月12日 17:24:29</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月18日 11:30:00</t>
+    <t xml:space="preserve">2022年09月15日 14:52:29</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月26日 20:49:58</t>
+    <t xml:space="preserve">2022年09月15日 14:20:27</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -1301,7 +1301,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月18日 17:59:23</t>
+    <t xml:space="preserve">2022年09月12日 10:33:34</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1964,7 +1964,7 @@
     <t xml:space="preserve">聯徵授信餘額月報資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年07月21日 16:25:37</t>
+    <t xml:space="preserve">2022年09月14日 20:31:59</t>
   </si>
   <si>
     <t xml:space="preserve">JcicB204</t>
@@ -2027,7 +2027,7 @@
     <t xml:space="preserve">前置協商受理申請暨請求回報償權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月01日 09:28:51</t>
+    <t xml:space="preserve">2022年09月07日 11:22:26</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ040Log</t>
@@ -2042,7 +2042,7 @@
     <t xml:space="preserve">協商開始暨停催通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:29:23</t>
+    <t xml:space="preserve">2022年09月07日 09:52:54</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ041Log</t>
@@ -2057,7 +2057,7 @@
     <t xml:space="preserve">回報無擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:33:04</t>
+    <t xml:space="preserve">2022年09月07日 14:37:23</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ042Log</t>
@@ -2072,7 +2072,7 @@
     <t xml:space="preserve">回報有擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 16:17:21</t>
+    <t xml:space="preserve">2022年09月07日 14:38:05</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ043Log</t>
@@ -2087,7 +2087,7 @@
     <t xml:space="preserve">請求同意債務清償方案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:31:04</t>
+    <t xml:space="preserve">2022年09月07日 14:38:23</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ044Log</t>
@@ -2102,7 +2102,7 @@
     <t xml:space="preserve">回報是否同意債務清償方案資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:31:26</t>
+    <t xml:space="preserve">2022年09月07日 14:38:43</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ045Log</t>
@@ -2117,7 +2117,7 @@
     <t xml:space="preserve">結案通知資料檔案格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:31:50</t>
+    <t xml:space="preserve">2022年09月07日 14:39:09</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ046Log</t>
@@ -2132,7 +2132,7 @@
     <t xml:space="preserve">金融機構無擔保債務協議資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:32:11</t>
+    <t xml:space="preserve">2022年09月07日 14:39:28</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ047Log</t>
@@ -2147,7 +2147,7 @@
     <t xml:space="preserve">債務人基本資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:32:26</t>
+    <t xml:space="preserve">2022年09月07日 14:39:44</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ048Log</t>
@@ -2162,7 +2162,7 @@
     <t xml:space="preserve">債務清償方案法院認可資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:32:44</t>
+    <t xml:space="preserve">2022年09月07日 14:39:57</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ049Log</t>
@@ -2177,7 +2177,7 @@
     <t xml:space="preserve">債務人繳款資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:33:32</t>
+    <t xml:space="preserve">2022年09月07日 14:40:13</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ050Log</t>
@@ -2192,7 +2192,7 @@
     <t xml:space="preserve">延期繳款（喘息期）資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:34:02</t>
+    <t xml:space="preserve">2022年09月07日 14:40:39</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ051Log</t>
@@ -2207,7 +2207,7 @@
     <t xml:space="preserve">前置協商相關資料報送例外處理</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:34:12</t>
+    <t xml:space="preserve">2022年09月07日 14:40:52</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ052Log</t>
@@ -2222,7 +2222,7 @@
     <t xml:space="preserve">同意報送例外處理檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:34:29</t>
+    <t xml:space="preserve">2022年09月07日 14:41:04</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ053Log</t>
@@ -2237,7 +2237,7 @@
     <t xml:space="preserve">單獨全數受清償資料檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:34:48</t>
+    <t xml:space="preserve">2022年09月07日 14:41:18</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ054Log</t>
@@ -2252,7 +2252,7 @@
     <t xml:space="preserve">消債條例更生案件資料報送</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:35:11</t>
+    <t xml:space="preserve">2022年09月07日 14:41:30</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ055Log</t>
@@ -2267,7 +2267,7 @@
     <t xml:space="preserve">清算案件資料報送</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:35:31</t>
+    <t xml:space="preserve">2022年09月07日 14:41:47</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ056Log</t>
@@ -2279,7 +2279,7 @@
     <t xml:space="preserve">JcicZ060</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:35:46</t>
+    <t xml:space="preserve">2022年09月07日 14:42:01</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ060Log</t>
@@ -2294,7 +2294,7 @@
     <t xml:space="preserve">回報協商剩餘債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:35:59</t>
+    <t xml:space="preserve">2022年09月07日 14:42:15</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ061Log</t>
@@ -2309,7 +2309,7 @@
     <t xml:space="preserve">金融機構無擔保債務變更還款條件協議資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:36:14</t>
+    <t xml:space="preserve">2022年09月07日 14:42:29</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ062Log</t>
@@ -2324,7 +2324,7 @@
     <t xml:space="preserve">變更還款方案結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:36:26</t>
+    <t xml:space="preserve">2022年09月07日 14:42:40</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ063Log</t>
@@ -2339,7 +2339,7 @@
     <t xml:space="preserve">前置調解受理申請暨請求回報債權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:36:38</t>
+    <t xml:space="preserve">2022年09月07日 14:44:00</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ440Log</t>
@@ -2354,7 +2354,7 @@
     <t xml:space="preserve">前置調解回報無擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:36:49</t>
+    <t xml:space="preserve">2022年09月07日 14:44:38</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ442Log</t>
@@ -2369,7 +2369,7 @@
     <t xml:space="preserve">前置調解回報有擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:36:57</t>
+    <t xml:space="preserve">2022年09月07日 14:44:49</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ443Log</t>
@@ -2384,7 +2384,7 @@
     <t xml:space="preserve">前置調解債務人基本資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:05</t>
+    <t xml:space="preserve">2022年09月07日 14:45:01</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ444Log</t>
@@ -2399,7 +2399,7 @@
     <t xml:space="preserve">前置調解結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:14</t>
+    <t xml:space="preserve">2022年09月07日 14:45:15</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ446Log</t>
@@ -2414,7 +2414,7 @@
     <t xml:space="preserve">前置調解金融機構無擔保債務協議資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:23</t>
+    <t xml:space="preserve">2022年09月07日 14:45:27</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ447Log</t>
@@ -2429,7 +2429,7 @@
     <t xml:space="preserve">前置調解無擔保債務還款分配資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:31</t>
+    <t xml:space="preserve">2022年09月07日 14:45:41</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ448Log</t>
@@ -2444,7 +2444,7 @@
     <t xml:space="preserve">前置調解債務人繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:39</t>
+    <t xml:space="preserve">2022年09月07日 14:47:21</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ450Log</t>
@@ -2459,7 +2459,7 @@
     <t xml:space="preserve">前置調解延期繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:49</t>
+    <t xml:space="preserve">2022年09月07日 14:49:19</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ451Log</t>
@@ -2474,7 +2474,7 @@
     <t xml:space="preserve">前置調解單獨全數受清償資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:37:58</t>
+    <t xml:space="preserve">2022年09月07日 14:49:31</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ454Log</t>
@@ -2489,7 +2489,7 @@
     <t xml:space="preserve">受理更生款項統一收付通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:17</t>
+    <t xml:space="preserve">2022年09月07日 14:49:45</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ570Log</t>
@@ -2504,7 +2504,7 @@
     <t xml:space="preserve">更生款項統一收付回報債權資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:27</t>
+    <t xml:space="preserve">2022年09月07日 14:49:59</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ571Log</t>
@@ -2519,7 +2519,7 @@
     <t xml:space="preserve">受理更生款項統一收付款項分配表資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:35</t>
+    <t xml:space="preserve">2022年09月07日 14:50:14</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ572Log</t>
@@ -2534,7 +2534,7 @@
     <t xml:space="preserve">更生債務人繳款資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:43</t>
+    <t xml:space="preserve">2022年09月07日 14:50:28</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ573Log</t>
@@ -2549,7 +2549,7 @@
     <t xml:space="preserve">更生款項統一收付結案通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:51</t>
+    <t xml:space="preserve">2022年09月07日 14:51:08</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ574Log</t>
@@ -2564,7 +2564,7 @@
     <t xml:space="preserve">更生債權金額異動通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 15:38:58</t>
+    <t xml:space="preserve">2022年09月07日 14:51:22</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ575Log</t>
@@ -2657,6 +2657,15 @@
     <t xml:space="preserve">2022年01月20日 12:43:16</t>
   </si>
   <si>
+    <t xml:space="preserve">DailyTav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">每日暫收款餘額檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年09月14日 11:41:17</t>
+  </si>
+  <si>
     <t xml:space="preserve">GuildBuilders</t>
   </si>
   <si>
@@ -3026,7 +3035,7 @@
     <t xml:space="preserve">資料變更紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月29日 19:24:06</t>
+    <t xml:space="preserve">2022年09月07日 18:30:23</t>
   </si>
   <si>
     <t xml:space="preserve">TxErrCode</t>
@@ -3291,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="2">
@@ -8741,7 +8750,7 @@
         <v>882</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8759,7 +8768,7 @@
         <v>885</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8777,7 +8786,7 @@
         <v>888</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8795,7 +8804,7 @@
         <v>891</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8813,7 +8822,7 @@
         <v>894</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8831,7 +8840,7 @@
         <v>897</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8849,7 +8858,7 @@
         <v>900</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8867,7 +8876,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8885,7 +8894,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8903,7 +8912,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -8921,7 +8930,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -8939,7 +8948,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -8957,7 +8966,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8975,7 +8984,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8993,7 +9002,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9011,7 +9020,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9029,7 +9038,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9047,7 +9056,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9065,7 +9074,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9083,7 +9092,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9101,7 +9110,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9119,7 +9128,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9128,25 +9137,25 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B326" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="B326" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="C326" s="1" t="s">
+      <c r="D326" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E326" s="1" t="s">
         <v>949</v>
-      </c>
-      <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E326" s="1" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>951</v>
@@ -9155,7 +9164,7 @@
         <v>952</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9164,7 +9173,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>954</v>
@@ -9173,7 +9182,7 @@
         <v>955</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9182,7 +9191,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>957</v>
@@ -9191,7 +9200,7 @@
         <v>958</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9200,7 +9209,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>960</v>
@@ -9209,7 +9218,7 @@
         <v>961</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9218,7 +9227,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>963</v>
@@ -9227,7 +9236,7 @@
         <v>964</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9236,7 +9245,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>966</v>
@@ -9245,7 +9254,7 @@
         <v>967</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9254,7 +9263,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>969</v>
@@ -9263,7 +9272,7 @@
         <v>970</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9272,7 +9281,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>972</v>
@@ -9281,7 +9290,7 @@
         <v>973</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9290,7 +9299,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9299,7 +9308,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9308,7 +9317,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9317,7 +9326,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9326,7 +9335,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9335,7 +9344,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9344,7 +9353,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9353,7 +9362,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9362,7 +9371,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9371,7 +9380,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9380,7 +9389,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9389,7 +9398,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9398,7 +9407,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9407,7 +9416,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9416,7 +9425,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9425,7 +9434,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9434,7 +9443,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9443,7 +9452,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9452,7 +9461,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9461,7 +9470,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9470,7 +9479,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9479,7 +9488,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9488,7 +9497,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9497,7 +9506,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9506,7 +9515,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9515,7 +9524,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9524,7 +9533,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9533,7 +9542,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9542,7 +9551,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9551,7 +9560,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9560,7 +9569,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9569,7 +9578,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9578,7 +9587,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9587,7 +9596,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9596,34 +9605,34 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>1012</v>
+        <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>1029</v>
+        <v>1015</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9632,7 +9641,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1031</v>
@@ -9641,7 +9650,7 @@
         <v>1032</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9650,7 +9659,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1034</v>
@@ -9659,7 +9668,7 @@
         <v>1035</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9668,7 +9677,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1037</v>
@@ -9677,7 +9686,7 @@
         <v>1038</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9686,7 +9695,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1040</v>
@@ -9695,7 +9704,7 @@
         <v>1041</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9704,7 +9713,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1043</v>
@@ -9713,7 +9722,7 @@
         <v>1044</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9722,7 +9731,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1046</v>
@@ -9731,7 +9740,7 @@
         <v>1047</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9740,7 +9749,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1049</v>
@@ -9749,7 +9758,7 @@
         <v>1050</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9758,7 +9767,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1052</v>
@@ -9767,11 +9776,29 @@
         <v>1053</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
         <v>1054</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D362" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E362" s="1" t="s">
+        <v>1057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/10/07 週五 17:47:14.94
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="1065">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">擔保品與額度關聯檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月07日 11:30:50</t>
+    <t xml:space="preserve">2022年10月06日 11:27:07</t>
   </si>
   <si>
     <t xml:space="preserve">ClImm</t>
@@ -311,7 +311,7 @@
     <t xml:space="preserve">擔保品他項權利檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月26日 11:11:27</t>
+    <t xml:space="preserve">2022年09月22日 19:35:38</t>
   </si>
   <si>
     <t xml:space="preserve">ClOwnerRelation</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月01日 18:58:36</t>
+    <t xml:space="preserve">2022年10月06日 09:39:51</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月15日 14:52:29</t>
+    <t xml:space="preserve">2022年09月21日 19:38:14</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月27日 12:49:12</t>
+    <t xml:space="preserve">2022年09月21日 14:05:14</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月26日 11:42:12</t>
+    <t xml:space="preserve">2022年10月05日 19:35:14</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1301,7 +1301,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月12日 10:33:34</t>
+    <t xml:space="preserve">2022年09月21日 14:11:06</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1637,6 +1637,15 @@
     <t xml:space="preserve">2022年03月28日 09:43:35</t>
   </si>
   <si>
+    <t xml:space="preserve">CdTeamReward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">團康獎勵津貼標準設定</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年09月20日 17:19:31</t>
+  </si>
+  <si>
     <t xml:space="preserve">CdVarValue</t>
   </si>
   <si>
@@ -1865,6 +1874,15 @@
     <t xml:space="preserve">2021年12月02日 10:13:04</t>
   </si>
   <si>
+    <t xml:space="preserve">StakeholdersStaff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人壽利關人職員名單檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年09月29日 14:40:59</t>
+  </si>
+  <si>
     <t xml:space="preserve">L8-遵循法令作業</t>
   </si>
   <si>
@@ -1964,7 +1982,7 @@
     <t xml:space="preserve">聯徵授信餘額月報資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月14日 20:31:59</t>
+    <t xml:space="preserve">2022年09月16日 18:08:27</t>
   </si>
   <si>
     <t xml:space="preserve">JcicB204</t>
@@ -2027,7 +2045,7 @@
     <t xml:space="preserve">前置協商受理申請暨請求回報償權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月07日 11:22:26</t>
+    <t xml:space="preserve">2022年09月20日 15:34:41</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ040Log</t>
@@ -2588,7 +2606,7 @@
     <t xml:space="preserve">疑似洗錢交易合理性明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月25日 19:21:49</t>
+    <t xml:space="preserve">2022年09月19日 16:41:48</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryParas</t>
@@ -3113,7 +3131,7 @@
     <t xml:space="preserve">交易記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月12日 17:24:17</t>
+    <t xml:space="preserve">2022年09月27日 14:21:37</t>
   </si>
   <si>
     <t xml:space="preserve">TxTeller</t>
@@ -3300,7 +3318,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="2">
@@ -6500,7 +6518,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6518,7 +6536,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6536,7 +6554,7 @@
         <v>548</v>
       </c>
       <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E181" s="1" t="s">
@@ -6554,7 +6572,7 @@
         <v>551</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6572,7 +6590,7 @@
         <v>554</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6590,7 +6608,7 @@
         <v>557</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6599,25 +6617,25 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="C185" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E185" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>563</v>
@@ -6626,7 +6644,7 @@
         <v>564</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6635,7 +6653,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>566</v>
@@ -6644,7 +6662,7 @@
         <v>567</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6653,7 +6671,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>569</v>
@@ -6662,7 +6680,7 @@
         <v>570</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6671,7 +6689,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>572</v>
@@ -6680,7 +6698,7 @@
         <v>573</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6689,7 +6707,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>575</v>
@@ -6698,7 +6716,7 @@
         <v>576</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E190" s="1" t="s">
@@ -6707,7 +6725,7 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6716,7 +6734,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6725,7 +6743,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6734,7 +6752,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6743,7 +6761,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6752,7 +6770,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6761,7 +6779,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6770,7 +6788,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6779,7 +6797,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6788,7 +6806,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6797,7 +6815,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6806,7 +6824,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6815,7 +6833,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6824,7 +6842,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6833,7 +6851,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6842,7 +6860,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6851,7 +6869,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6860,7 +6878,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6869,7 +6887,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>605</v>
@@ -6878,7 +6896,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6887,7 +6905,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>608</v>
@@ -6896,7 +6914,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -6905,7 +6923,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>611</v>
@@ -6914,7 +6932,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -6923,7 +6941,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>614</v>
@@ -6932,7 +6950,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -6941,43 +6959,43 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="C204" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="D204" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E204" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>617</v>
+        <v>562</v>
       </c>
       <c r="B205" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="C205" s="1" t="s">
+      <c r="D205" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E205" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>624</v>
@@ -6986,7 +7004,7 @@
         <v>625</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -6995,7 +7013,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>627</v>
@@ -7004,7 +7022,7 @@
         <v>628</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7013,7 +7031,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>630</v>
@@ -7022,7 +7040,7 @@
         <v>631</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7031,7 +7049,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>633</v>
@@ -7040,7 +7058,7 @@
         <v>634</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7049,7 +7067,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>636</v>
@@ -7058,7 +7076,7 @@
         <v>637</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7067,7 +7085,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>639</v>
@@ -7076,7 +7094,7 @@
         <v>640</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -7085,7 +7103,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7094,7 +7112,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7103,7 +7121,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7112,7 +7130,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7121,7 +7139,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7130,7 +7148,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7139,7 +7157,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7148,7 +7166,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7157,7 +7175,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7166,7 +7184,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7175,7 +7193,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7184,7 +7202,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7193,7 +7211,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7202,7 +7220,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7211,7 +7229,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7220,7 +7238,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7229,7 +7247,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7238,7 +7256,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7247,7 +7265,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7256,7 +7274,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7265,1348 +7283,1348 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>720</v>
+        <v>756</v>
       </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B256" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C256" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="C256" s="1" t="s">
-        <v>720</v>
-      </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>759</v>
+        <v>726</v>
       </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>759</v>
+        <v>726</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -8615,7 +8633,7 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>859</v>
@@ -8624,7 +8642,7 @@
         <v>860</v>
       </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
@@ -8633,7 +8651,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>862</v>
@@ -8642,7 +8660,7 @@
         <v>863</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
@@ -8651,7 +8669,7 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>865</v>
@@ -8660,7 +8678,7 @@
         <v>866</v>
       </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
@@ -8669,7 +8687,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>868</v>
@@ -8678,7 +8696,7 @@
         <v>869</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
@@ -8687,7 +8705,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>871</v>
@@ -8696,7 +8714,7 @@
         <v>872</v>
       </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
@@ -8705,7 +8723,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>874</v>
@@ -8714,7 +8732,7 @@
         <v>875</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
@@ -8723,43 +8741,43 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B303" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="B303" s="1" t="s">
+      <c r="C303" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="C303" s="1" t="s">
+      <c r="D303" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E303" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>877</v>
+        <v>623</v>
       </c>
       <c r="B304" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C304" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="C304" s="1" t="s">
+      <c r="D304" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E304" s="1" t="s">
         <v>882</v>
-      </c>
-      <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>884</v>
@@ -8768,7 +8786,7 @@
         <v>885</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8777,7 +8795,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>887</v>
@@ -8786,7 +8804,7 @@
         <v>888</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8795,7 +8813,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>890</v>
@@ -8804,7 +8822,7 @@
         <v>891</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8813,7 +8831,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>893</v>
@@ -8822,7 +8840,7 @@
         <v>894</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8831,7 +8849,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>896</v>
@@ -8840,7 +8858,7 @@
         <v>897</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8849,7 +8867,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>899</v>
@@ -8858,7 +8876,7 @@
         <v>900</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8867,7 +8885,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>902</v>
@@ -8876,7 +8894,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8885,7 +8903,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8894,7 +8912,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8903,7 +8921,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -8912,7 +8930,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -8921,7 +8939,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -8930,7 +8948,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -8939,7 +8957,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -8948,7 +8966,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -8957,7 +8975,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -8966,7 +8984,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8975,7 +8993,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -8984,7 +9002,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -8993,7 +9011,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9002,7 +9020,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9011,7 +9029,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9020,7 +9038,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9029,7 +9047,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9038,7 +9056,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9047,7 +9065,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9056,7 +9074,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9065,7 +9083,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9074,7 +9092,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9083,7 +9101,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9092,7 +9110,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9101,7 +9119,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9110,7 +9128,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9119,7 +9137,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9128,7 +9146,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9137,7 +9155,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9146,7 +9164,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9155,43 +9173,43 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B327" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="C327" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="C327" s="1" t="s">
+      <c r="D327" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E327" s="1" t="s">
         <v>952</v>
-      </c>
-      <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E327" s="1" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>950</v>
+        <v>883</v>
       </c>
       <c r="B328" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C328" s="1" t="s">
         <v>954</v>
       </c>
-      <c r="C328" s="1" t="s">
+      <c r="D328" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E328" s="1" t="s">
         <v>955</v>
-      </c>
-      <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E328" s="1" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>957</v>
@@ -9200,7 +9218,7 @@
         <v>958</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9209,7 +9227,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>960</v>
@@ -9218,7 +9236,7 @@
         <v>961</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9227,7 +9245,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>963</v>
@@ -9236,7 +9254,7 @@
         <v>964</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9245,7 +9263,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>966</v>
@@ -9254,7 +9272,7 @@
         <v>967</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9263,7 +9281,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>969</v>
@@ -9272,7 +9290,7 @@
         <v>970</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9281,7 +9299,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>972</v>
@@ -9290,7 +9308,7 @@
         <v>973</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9299,7 +9317,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9308,7 +9326,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9317,7 +9335,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9326,7 +9344,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9335,7 +9353,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9344,7 +9362,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9353,7 +9371,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9362,7 +9380,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9371,7 +9389,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9380,7 +9398,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9389,7 +9407,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9398,7 +9416,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9407,7 +9425,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9416,7 +9434,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9425,7 +9443,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9434,7 +9452,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9443,7 +9461,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9452,7 +9470,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9461,7 +9479,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9470,7 +9488,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9479,7 +9497,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9488,7 +9506,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9497,7 +9515,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9506,7 +9524,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9515,7 +9533,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9524,7 +9542,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9533,7 +9551,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9542,7 +9560,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9551,7 +9569,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9560,7 +9578,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9569,7 +9587,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9578,7 +9596,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9587,7 +9605,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9596,7 +9614,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9605,7 +9623,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9614,7 +9632,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9623,52 +9641,52 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>1015</v>
+        <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>1035</v>
+        <v>1021</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9677,7 +9695,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1037</v>
@@ -9686,7 +9704,7 @@
         <v>1038</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9695,7 +9713,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1040</v>
@@ -9704,7 +9722,7 @@
         <v>1041</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9713,7 +9731,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1043</v>
@@ -9722,7 +9740,7 @@
         <v>1044</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9731,7 +9749,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1046</v>
@@ -9740,7 +9758,7 @@
         <v>1047</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9749,7 +9767,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1049</v>
@@ -9758,7 +9776,7 @@
         <v>1050</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9767,7 +9785,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1052</v>
@@ -9776,7 +9794,7 @@
         <v>1053</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9785,7 +9803,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1055</v>
@@ -9794,11 +9812,47 @@
         <v>1056</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
         <v>1057</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D363" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D364" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>1063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/11/11 週五 17:27:19.96
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -677,7 +677,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月12日 09:40:17</t>
+    <t xml:space="preserve">2022年11月10日 10:51:02</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月30日 15:14:07</t>
+    <t xml:space="preserve">2022年11月11日 11:38:00</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -2276,7 +2276,7 @@
     <t xml:space="preserve">同意報送例外處理檔案</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月07日 14:41:04</t>
+    <t xml:space="preserve">2022年11月10日 14:31:04</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ053Log</t>
@@ -2408,13 +2408,13 @@
     <t xml:space="preserve">前置調解回報無擔保債權金額資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月07日 14:44:38</t>
+    <t xml:space="preserve">2022年11月11日 16:20:33</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ442Log</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:38:18</t>
+    <t xml:space="preserve">2022年11月11日 16:25:05</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ443</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/11/25 週五 17:35:47.93
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月24日 10:44:22</t>
+    <t xml:space="preserve">2022年11月21日 10:39:48</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月08日 11:47:54</t>
+    <t xml:space="preserve">2022年11月22日 09:52:44</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">支票檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:44:03</t>
+    <t xml:space="preserve">2022年11月24日 10:20:46</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCustRmk</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月15日 14:20:27</t>
+    <t xml:space="preserve">2022年11月16日 13:25:59</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -740,7 +740,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月20日 19:37:28</t>
+    <t xml:space="preserve">2022年11月15日 20:29:32</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月11日 11:38:00</t>
+    <t xml:space="preserve">2022年11月12日 09:34:40</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -1058,7 +1058,7 @@
     <t xml:space="preserve">債務協商債權機構帳戶檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年06月21日 13:01:23</t>
+    <t xml:space="preserve">2022年11月22日 19:06:45</t>
   </si>
   <si>
     <t xml:space="preserve">NegFinShare</t>
@@ -2720,13 +2720,13 @@
     <t xml:space="preserve">2022年09月14日 11:41:17</t>
   </si>
   <si>
-    <t xml:space="preserve">GuildBuilders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">公會餘額統計建商名單檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年01月13日 15:54:58</t>
+    <t xml:space="preserve">MonthlyDpUnpaidExpense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">每月未銷火險及法拍費明細檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年11月22日 13:11:17</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyFacBal</t>
@@ -8930,7 +8930,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\GuildBuilders.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">

</xml_diff>

<commit_message>
Auto-committed on 2022/12/02 週五 17:19:16.40
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月22日 09:52:44</t>
+    <t xml:space="preserve">2022年12月01日 12:50:44</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1058,7 +1058,7 @@
     <t xml:space="preserve">債務協商債權機構帳戶檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月22日 19:06:45</t>
+    <t xml:space="preserve">2022年11月28日 12:32:08</t>
   </si>
   <si>
     <t xml:space="preserve">NegFinShare</t>
@@ -1445,7 +1445,7 @@
     <t xml:space="preserve">利息收入預算檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年07月16日 10:30:53</t>
+    <t xml:space="preserve">2022年11月29日 14:29:51</t>
   </si>
   <si>
     <t xml:space="preserve">CdBuildingCost</t>
@@ -1463,7 +1463,7 @@
     <t xml:space="preserve">現金流量預估資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年08月06日 17:34:03</t>
+    <t xml:space="preserve">2022年11月29日 14:21:19</t>
   </si>
   <si>
     <t xml:space="preserve">CdCity</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/12/16 週五 17:26:04.96
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -401,7 +401,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月09日 16:39:17</t>
+    <t xml:space="preserve">2022年12月15日 16:42:36</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月01日 12:50:44</t>
+    <t xml:space="preserve">2022年12月15日 14:12:39</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1400,7 +1400,7 @@
     <t xml:space="preserve">指標利率檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月11日 12:22:40</t>
+    <t xml:space="preserve">2022年12月15日 12:19:39</t>
   </si>
   <si>
     <t xml:space="preserve">CdBcm</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/12/23 週五 17:18:57.23
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月06日 17:16:03</t>
+    <t xml:space="preserve">2022年12月20日 17:12:40</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月15日 14:12:39</t>
+    <t xml:space="preserve">2022年12月22日 11:15:28</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1409,7 +1409,7 @@
     <t xml:space="preserve">分公司資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月08日 14:34:20</t>
+    <t xml:space="preserve">2022年12月22日 11:22:59</t>
   </si>
   <si>
     <t xml:space="preserve">CdBonus</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月25日 14:36:54</t>
+    <t xml:space="preserve">2022年12月20日 15:09:26</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2642,7 +2642,7 @@
     <t xml:space="preserve">疑似洗錢樣態檢核明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月18日 13:51:21</t>
+    <t xml:space="preserve">2022年12月21日 11:30:40</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryDetail</t>
@@ -2651,7 +2651,7 @@
     <t xml:space="preserve">疑似洗錢交易合理性明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月19日 16:41:48</t>
+    <t xml:space="preserve">2022年12月23日 14:33:05</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryParas</t>
@@ -2660,7 +2660,7 @@
     <t xml:space="preserve">疑似洗錢樣態條件設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:42:37</t>
+    <t xml:space="preserve">2022年12月18日 18:17:14</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryRecord</t>
@@ -2687,7 +2687,7 @@
     <t xml:space="preserve">聯徵人員名冊</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月01日 10:27:40</t>
+    <t xml:space="preserve">2022年12月19日 16:07:07</t>
   </si>
   <si>
     <t xml:space="preserve">TbJcicW020</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/12/30 週五 17:22:29.06
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月22日 11:15:28</t>
+    <t xml:space="preserve">2022年12月30日 07:55:41</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">支票檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月24日 10:20:46</t>
+    <t xml:space="preserve">2022年12月26日 11:41:54</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCustRmk</t>
@@ -668,7 +668,7 @@
     <t xml:space="preserve">銀行扣款明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月28日 13:59:03</t>
+    <t xml:space="preserve">2022年12月26日 00:24:13</t>
   </si>
   <si>
     <t xml:space="preserve">BankRemit</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月21日 19:38:14</t>
+    <t xml:space="preserve">2022年12月26日 01:37:19</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月16日 13:25:59</t>
+    <t xml:space="preserve">2022年12月26日 11:36:04</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月12日 09:34:40</t>
+    <t xml:space="preserve">2022年12月26日 11:27:13</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -1085,7 +1085,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:24:01</t>
+    <t xml:space="preserve">2022年12月23日 17:39:39</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1247,7 +1247,7 @@
     <t xml:space="preserve">會計業務檢核檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月25日 17:21:37</t>
+    <t xml:space="preserve">2022年12月28日 13:37:35</t>
   </si>
   <si>
     <t xml:space="preserve">AcAcctCheckDetail</t>
@@ -1319,7 +1319,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月21日 14:11:06</t>
+    <t xml:space="preserve">2022年12月30日 14:57:32</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月20日 15:09:26</t>
+    <t xml:space="preserve">2022年12月27日 12:09:19</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2651,7 +2651,7 @@
     <t xml:space="preserve">疑似洗錢交易合理性明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月23日 14:33:05</t>
+    <t xml:space="preserve">2022年12月29日 12:45:23</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryParas</t>
@@ -2999,7 +2999,7 @@
     <t xml:space="preserve">歷史封存表設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月16日 12:53:38</t>
+    <t xml:space="preserve">2022年12月26日 11:00:01</t>
   </si>
   <si>
     <t xml:space="preserve">TxArchiveTableLog</t>
@@ -3008,7 +3008,7 @@
     <t xml:space="preserve">歷史封存表紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月16日 15:34:57</t>
+    <t xml:space="preserve">2022年12月26日 11:10:02</t>
   </si>
   <si>
     <t xml:space="preserve">TxAttachment</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/01/06 週五 17:06:55.26
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月13日 18:57:51</t>
+    <t xml:space="preserve">2023年01月03日 14:51:53</t>
   </si>
   <si>
     <t xml:space="preserve">AchDeductMedia</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月26日 11:36:04</t>
+    <t xml:space="preserve">2023年01月04日 20:29:50</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月21日 14:05:14</t>
+    <t xml:space="preserve">2023年01月05日 12:31:12</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月05日 19:35:14</t>
+    <t xml:space="preserve">2023年01月05日 12:11:12</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1310,7 +1310,7 @@
     <t xml:space="preserve">會計總帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月14日 14:44:52</t>
+    <t xml:space="preserve">2023年01月01日 11:00:40</t>
   </si>
   <si>
     <t xml:space="preserve">AcReceivable</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月27日 12:09:19</t>
+    <t xml:space="preserve">2023年01月05日 11:19:41</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2651,7 +2651,7 @@
     <t xml:space="preserve">疑似洗錢交易合理性明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月29日 12:45:23</t>
+    <t xml:space="preserve">2023年01月04日 12:40:41</t>
   </si>
   <si>
     <t xml:space="preserve">MlaundryParas</t>
@@ -2825,7 +2825,7 @@
     <t xml:space="preserve">每月放款餘額檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月27日 18:25:18</t>
+    <t xml:space="preserve">2023年01月03日 12:04:19</t>
   </si>
   <si>
     <t xml:space="preserve">RptJcic</t>
@@ -3239,7 +3239,7 @@
     <t xml:space="preserve">交易控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月14日 11:55:41</t>
+    <t xml:space="preserve">2023年01月04日 17:25:21</t>
   </si>
   <si>
     <t xml:space="preserve">TxUnLock</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/01/13 週五 17:20:27.53
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月30日 07:55:41</t>
+    <t xml:space="preserve">2023年01月10日 19:05:48</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計業務關帳控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月21日 17:25:28</t>
+    <t xml:space="preserve">2023年01月13日 17:08:51</t>
   </si>
   <si>
     <t xml:space="preserve">AcDetail</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月05日 12:11:12</t>
+    <t xml:space="preserve">2023年01月12日 20:30:51</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1310,7 +1310,7 @@
     <t xml:space="preserve">會計總帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月01日 11:00:40</t>
+    <t xml:space="preserve">2023年01月07日 15:32:43</t>
   </si>
   <si>
     <t xml:space="preserve">AcReceivable</t>
@@ -1562,7 +1562,7 @@
     <t xml:space="preserve">行業別代號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月17日 16:09:36</t>
+    <t xml:space="preserve">2023年01月13日 09:46:57</t>
   </si>
   <si>
     <t xml:space="preserve">CdInsurer</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月05日 11:19:41</t>
+    <t xml:space="preserve">2023年01月11日 16:25:40</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2897,7 +2897,7 @@
     <t xml:space="preserve">傳票媒體檔2022年格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月22日 15:25:24</t>
+    <t xml:space="preserve">2023年01月10日 17:41:58</t>
   </si>
   <si>
     <t xml:space="preserve">UspErrorLog</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/01/19 週四 17:25:12.16
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1083">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月26日 01:37:19</t>
+    <t xml:space="preserve">2023年01月18日 17:55:37</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月05日 12:31:12</t>
+    <t xml:space="preserve">2023年01月17日 15:14:18</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1085,7 +1085,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月23日 17:39:39</t>
+    <t xml:space="preserve">2023年01月18日 18:59:38</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計業務關帳控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月13日 17:08:51</t>
+    <t xml:space="preserve">2023年01月16日 10:12:52</t>
   </si>
   <si>
     <t xml:space="preserve">AcDetail</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月12日 20:30:51</t>
+    <t xml:space="preserve">2023年01月17日 11:32:54</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1319,7 +1319,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月30日 14:57:32</t>
+    <t xml:space="preserve">2023年01月17日 10:31:20</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1517,7 +1517,7 @@
     <t xml:space="preserve">共用代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月09日 13:53:03</t>
+    <t xml:space="preserve">2023年01月17日 10:50:54</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1700,6 +1700,15 @@
     <t xml:space="preserve">2021年11月24日 14:15:28</t>
   </si>
   <si>
+    <t xml:space="preserve">CoreAcMain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">核心會計總帳檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年01月18日 11:59:32</t>
+  </si>
+  <si>
     <t xml:space="preserve">JobDetail</t>
   </si>
   <si>
@@ -2726,7 +2735,7 @@
     <t xml:space="preserve">每日暫收款餘額檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月08日 11:17:33</t>
+    <t xml:space="preserve">2023年01月18日 16:54:35</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyDpUnpaidExpense</t>
@@ -3363,7 +3372,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="2">
@@ -6689,7 +6698,7 @@
         <v>563</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6707,7 +6716,7 @@
         <v>566</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6725,7 +6734,7 @@
         <v>569</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6743,7 +6752,7 @@
         <v>572</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6752,25 +6761,25 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="C190" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E190" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6779,7 +6788,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6788,7 +6797,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6797,7 +6806,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6806,7 +6815,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6815,7 +6824,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6824,7 +6833,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6833,7 +6842,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6842,7 +6851,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6851,7 +6860,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6860,7 +6869,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6869,7 +6878,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6878,7 +6887,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6887,7 +6896,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6896,7 +6905,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6905,7 +6914,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6914,7 +6923,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6923,7 +6932,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6932,7 +6941,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>605</v>
@@ -6941,7 +6950,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6950,7 +6959,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>608</v>
@@ -6959,7 +6968,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -6968,7 +6977,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>611</v>
@@ -6977,7 +6986,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -6986,7 +6995,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>614</v>
@@ -6995,7 +7004,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7004,7 +7013,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>617</v>
@@ -7013,7 +7022,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7022,7 +7031,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>620</v>
@@ -7031,7 +7040,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7040,7 +7049,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>623</v>
@@ -7049,7 +7058,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7058,7 +7067,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>626</v>
@@ -7067,7 +7076,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7076,7 +7085,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>629</v>
@@ -7085,7 +7094,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7094,7 +7103,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>632</v>
@@ -7103,7 +7112,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7112,25 +7121,25 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="C210" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="D210" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E210" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>639</v>
@@ -7139,7 +7148,7 @@
         <v>640</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -7148,7 +7157,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7157,7 +7166,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7166,7 +7175,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7175,7 +7184,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7184,7 +7193,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7193,7 +7202,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7202,7 +7211,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7211,7 +7220,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7220,7 +7229,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7229,7 +7238,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7238,7 +7247,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7247,7 +7256,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7256,7 +7265,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7265,7 +7274,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7274,7 +7283,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7283,7 +7292,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7292,7 +7301,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7301,7 +7310,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7310,7 +7319,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7319,7 +7328,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7328,7 +7337,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7337,7 +7346,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7346,7 +7355,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7355,7 +7364,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7364,7 +7373,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7373,7 +7382,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7382,7 +7391,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7391,7 +7400,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7400,7 +7409,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7409,7 +7418,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7418,7 +7427,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7427,7 +7436,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7436,7 +7445,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7445,7 +7454,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7454,34 +7463,34 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
@@ -7490,34 +7499,34 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>698</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
@@ -7526,34 +7535,34 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>703</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
@@ -7562,34 +7571,34 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>708</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
@@ -7598,34 +7607,34 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>713</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
@@ -7634,34 +7643,34 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>718</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
@@ -7670,34 +7679,34 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>723</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
@@ -7706,34 +7715,34 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>728</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
@@ -7742,34 +7751,34 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>733</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
@@ -7778,34 +7787,34 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>738</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
@@ -7814,34 +7823,34 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>743</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
@@ -7850,34 +7859,34 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>748</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
@@ -7886,34 +7895,34 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>753</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
@@ -7922,34 +7931,34 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>758</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
@@ -7958,34 +7967,34 @@
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>763</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
@@ -7994,34 +8003,34 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>768</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
@@ -8030,70 +8039,70 @@
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>773</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>741</v>
+        <v>774</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>780</v>
+        <v>744</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
@@ -8102,34 +8111,34 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>782</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
@@ -8138,34 +8147,34 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>787</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
@@ -8174,34 +8183,34 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>792</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
@@ -8210,34 +8219,34 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>797</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
@@ -8246,34 +8255,34 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>802</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
@@ -8282,34 +8291,34 @@
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>807</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
@@ -8318,34 +8327,34 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>812</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
@@ -8354,34 +8363,34 @@
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>817</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
@@ -8390,34 +8399,34 @@
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>822</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
@@ -8426,34 +8435,34 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>827</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
@@ -8462,34 +8471,34 @@
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>832</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
@@ -8498,34 +8507,34 @@
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>837</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
@@ -8534,34 +8543,34 @@
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>842</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
@@ -8570,34 +8579,34 @@
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>847</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
@@ -8606,34 +8615,34 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>852</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
@@ -8642,34 +8651,34 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>857</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
@@ -8678,34 +8687,34 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>862</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
@@ -8714,34 +8723,34 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>867</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
@@ -8750,34 +8759,34 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>872</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
@@ -8786,7 +8795,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>877</v>
@@ -8795,7 +8804,7 @@
         <v>878</v>
       </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
@@ -8804,7 +8813,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>880</v>
@@ -8813,7 +8822,7 @@
         <v>881</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8822,7 +8831,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>883</v>
@@ -8831,7 +8840,7 @@
         <v>884</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8840,7 +8849,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>886</v>
@@ -8849,7 +8858,7 @@
         <v>887</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8858,7 +8867,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8867,7 +8876,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8876,7 +8885,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>892</v>
@@ -8885,7 +8894,7 @@
         <v>893</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8894,7 +8903,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>895</v>
@@ -8903,7 +8912,7 @@
         <v>896</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8912,25 +8921,25 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B310" s="1" t="s">
         <v>898</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="C310" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="C310" s="1" t="s">
+      <c r="D310" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E310" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>902</v>
@@ -8939,7 +8948,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8948,7 +8957,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8957,7 +8966,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8966,7 +8975,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -8975,7 +8984,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -8984,7 +8993,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -8993,7 +9002,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9002,7 +9011,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9011,7 +9020,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9020,7 +9029,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9029,7 +9038,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9038,7 +9047,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9047,7 +9056,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9056,7 +9065,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9065,7 +9074,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9074,7 +9083,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9083,7 +9092,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9092,7 +9101,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9101,7 +9110,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9110,7 +9119,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9119,7 +9128,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9128,7 +9137,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9137,7 +9146,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9146,7 +9155,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9155,7 +9164,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9164,7 +9173,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9173,7 +9182,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9182,7 +9191,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9191,7 +9200,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9200,7 +9209,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9209,7 +9218,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9218,7 +9227,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9227,7 +9236,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9236,7 +9245,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9245,7 +9254,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9254,7 +9263,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9263,7 +9272,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9272,7 +9281,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9281,7 +9290,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9290,7 +9299,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9299,7 +9308,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9308,7 +9317,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9317,7 +9326,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9326,7 +9335,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9335,7 +9344,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9344,25 +9353,25 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B334" s="1" t="s">
         <v>971</v>
       </c>
-      <c r="B334" s="1" t="s">
+      <c r="C334" s="1" t="s">
         <v>972</v>
       </c>
-      <c r="C334" s="1" t="s">
+      <c r="D334" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E334" s="1" t="s">
         <v>973</v>
-      </c>
-      <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E334" s="1" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>975</v>
@@ -9371,7 +9380,7 @@
         <v>976</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9380,7 +9389,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>978</v>
@@ -9389,7 +9398,7 @@
         <v>979</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9398,7 +9407,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>981</v>
@@ -9407,7 +9416,7 @@
         <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9416,7 +9425,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9425,7 +9434,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9434,7 +9443,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9443,7 +9452,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9452,7 +9461,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9461,7 +9470,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9470,7 +9479,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9479,7 +9488,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9488,7 +9497,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9497,7 +9506,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9506,7 +9515,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9515,7 +9524,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9524,7 +9533,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9533,7 +9542,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9542,7 +9551,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9551,7 +9560,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9560,7 +9569,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9569,7 +9578,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9578,7 +9587,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9587,7 +9596,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9596,7 +9605,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9605,7 +9614,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9614,7 +9623,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9623,7 +9632,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9632,7 +9641,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9641,7 +9650,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9650,7 +9659,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9659,7 +9668,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9668,7 +9677,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9677,7 +9686,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9686,7 +9695,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9695,7 +9704,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9704,7 +9713,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9713,7 +9722,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9722,7 +9731,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9731,7 +9740,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9740,7 +9749,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9749,7 +9758,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9758,7 +9767,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9767,7 +9776,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9776,7 +9785,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9785,7 +9794,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9794,7 +9803,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9803,7 +9812,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9812,34 +9821,34 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>1036</v>
+        <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>1053</v>
+        <v>1039</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9848,7 +9857,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1055</v>
@@ -9857,7 +9866,7 @@
         <v>1056</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9866,7 +9875,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1058</v>
@@ -9875,7 +9884,7 @@
         <v>1059</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9884,7 +9893,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>1061</v>
@@ -9893,7 +9902,7 @@
         <v>1062</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9902,7 +9911,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1064</v>
@@ -9911,7 +9920,7 @@
         <v>1065</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9920,7 +9929,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1067</v>
@@ -9929,7 +9938,7 @@
         <v>1068</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9938,7 +9947,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1070</v>
@@ -9947,7 +9956,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9956,7 +9965,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1073</v>
@@ -9965,7 +9974,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -9974,7 +9983,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1076</v>
@@ -9983,11 +9992,29 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
         <v>1078</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D370" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>1081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/02/03 週五 17:21:57.66
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1086">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -365,7 +365,7 @@
     <t xml:space="preserve">結清戶個資控管檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月01日 15:40:52</t>
+    <t xml:space="preserve">2023年02月02日 19:28:47</t>
   </si>
   <si>
     <t xml:space="preserve">CustRmk</t>
@@ -401,7 +401,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月15日 16:42:36</t>
+    <t xml:space="preserve">2023年01月30日 10:58:58</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月17日 15:14:18</t>
+    <t xml:space="preserve">2023年02月02日 17:20:40</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1067,7 +1067,7 @@
     <t xml:space="preserve">債務協商債權分攤檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月08日 15:03:18</t>
+    <t xml:space="preserve">2023年02月01日 17:57:44</t>
   </si>
   <si>
     <t xml:space="preserve">NegFinShareLog</t>
@@ -1319,7 +1319,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月17日 10:31:20</t>
+    <t xml:space="preserve">2023年01月31日 14:07:34</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1643,7 +1643,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月01日 18:32:46</t>
+    <t xml:space="preserve">2023年01月30日 15:18:39</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>
@@ -1742,7 +1742,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月11日 16:25:40</t>
+    <t xml:space="preserve">2023年02月01日 10:10:56</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2735,7 +2735,7 @@
     <t xml:space="preserve">每日暫收款餘額檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月18日 16:54:35</t>
+    <t xml:space="preserve">2023年02月03日 10:56:15</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyDpUnpaidExpense</t>
@@ -2982,6 +2982,15 @@
   </si>
   <si>
     <t xml:space="preserve">2021年07月06日 17:07:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlRatingAppl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eloan評級案件申請留存檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年02月03日 09:11:36</t>
   </si>
   <si>
     <t xml:space="preserve">TxApLog</t>
@@ -3372,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="2">
@@ -9470,7 +9479,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9488,7 +9497,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9506,7 +9515,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9524,7 +9533,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9542,7 +9551,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9560,7 +9569,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9578,7 +9587,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9596,7 +9605,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9614,7 +9623,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9632,7 +9641,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9650,7 +9659,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9668,7 +9677,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9686,7 +9695,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9704,7 +9713,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9722,7 +9731,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9740,7 +9749,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9758,7 +9767,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9776,7 +9785,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9794,7 +9803,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9812,7 +9821,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9830,7 +9839,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9845,14 +9854,14 @@
         <v>1053</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>1039</v>
+        <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="362">
@@ -9860,13 +9869,13 @@
         <v>974</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>1056</v>
+        <v>1042</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9884,7 +9893,7 @@
         <v>1059</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9902,7 +9911,7 @@
         <v>1062</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9920,7 +9929,7 @@
         <v>1065</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9938,7 +9947,7 @@
         <v>1068</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9956,7 +9965,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9974,7 +9983,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -9992,7 +10001,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10010,11 +10019,29 @@
         <v>1080</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
         <v>1081</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D371" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>1084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/02/10 週五 17:24:00.48
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1095">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月20日 17:12:40</t>
+    <t xml:space="preserve">2023年02月10日 12:01:49</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月10日 10:51:02</t>
+    <t xml:space="preserve">2023年02月09日 16:39:24</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月17日 11:32:54</t>
+    <t xml:space="preserve">2023年02月07日 13:17:53</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1742,7 +1742,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月01日 10:10:56</t>
+    <t xml:space="preserve">2023年02月10日 10:51:09</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -1775,6 +1775,16 @@
     <t xml:space="preserve">2021年12月06日 10:23:34</t>
   </si>
   <si>
+    <t xml:space="preserve">FinHoldRel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金控利關人名單檔 T044
+(使用報表：LM049、LQ005)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年11月10日 16:06:17</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ias39IntMethod</t>
   </si>
   <si>
@@ -1838,6 +1848,26 @@
     <t xml:space="preserve">2022年01月20日 11:56:19</t>
   </si>
   <si>
+    <t xml:space="preserve">LifeRelEmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人壽利關人職員檔 T07_2
+(使用報表：LM013) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年11月10日 16:15:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LifeRelHead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人壽利關人負責人檔T07、TA07
+(使用報表：LM013、LM042、LM050)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年11月23日 13:58:34</t>
+  </si>
+  <si>
     <t xml:space="preserve">LoanIfrs9Ap</t>
   </si>
   <si>
@@ -1937,7 +1967,7 @@
     <t xml:space="preserve">AML每日有效客戶名單</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月18日 13:58:01</t>
+    <t xml:space="preserve">2023年02月06日 13:36:50</t>
   </si>
   <si>
     <t xml:space="preserve">JcicB080</t>
@@ -2981,7 +3011,7 @@
     <t xml:space="preserve">Eloan評級檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年07月06日 17:07:12</t>
+    <t xml:space="preserve">2023年02月06日 11:44:41</t>
   </si>
   <si>
     <t xml:space="preserve">TxAmlRatingAppl</t>
@@ -3257,7 +3287,7 @@
     <t xml:space="preserve">交易控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月04日 17:25:21</t>
+    <t xml:space="preserve">2023年02月09日 09:56:02</t>
   </si>
   <si>
     <t xml:space="preserve">TxUnLock</t>
@@ -3381,7 +3411,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1085</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="2">
@@ -6851,7 +6881,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6869,7 +6899,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6887,7 +6917,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6905,7 +6935,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loan34Data.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6923,7 +6953,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6941,7 +6971,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6959,7 +6989,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6977,7 +7007,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -6995,7 +7025,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -7013,7 +7043,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7031,7 +7061,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7049,7 +7079,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7067,7 +7097,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7085,7 +7115,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7103,7 +7133,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7121,7 +7151,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7139,7 +7169,7 @@
         <v>636</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7148,61 +7178,61 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="C211" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>638</v>
+        <v>577</v>
       </c>
       <c r="B212" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E212" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>638</v>
+        <v>577</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E213" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7211,7 +7241,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7220,7 +7250,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7229,7 +7259,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7238,7 +7268,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7247,7 +7277,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7256,7 +7286,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7265,7 +7295,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7274,7 +7304,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7283,7 +7313,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7292,7 +7322,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7301,7 +7331,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7310,7 +7340,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7319,7 +7349,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7328,7 +7358,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7337,7 +7367,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7346,7 +7376,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7355,7 +7385,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7364,7 +7394,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7373,7 +7403,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7382,7 +7412,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7391,7 +7421,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7400,7 +7430,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7409,7 +7439,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7418,7 +7448,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7427,7 +7457,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7436,7 +7466,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7445,7 +7475,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7454,7 +7484,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7463,7 +7493,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7472,7 +7502,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
@@ -7481,7 +7511,7 @@
         <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7490,1366 +7520,1366 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>696</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C233" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>704</v>
-      </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>709</v>
-      </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="C237" s="1" t="s">
-        <v>714</v>
-      </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C239" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="C239" s="1" t="s">
-        <v>719</v>
-      </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>724</v>
-      </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B243" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>729</v>
-      </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C245" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>734</v>
-      </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B247" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>739</v>
-      </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="C249" s="1" t="s">
-        <v>744</v>
-      </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C251" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="C251" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C253" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>759</v>
-      </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="C257" s="1" t="s">
-        <v>764</v>
-      </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B259" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="C259" s="1" t="s">
-        <v>769</v>
-      </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="C261" s="1" t="s">
-        <v>774</v>
-      </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="C263" s="1" t="s">
-        <v>744</v>
-      </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>744</v>
+        <v>783</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>783</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>783</v>
+        <v>753</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>788</v>
+        <v>753</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B269" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C269" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="C269" s="1" t="s">
-        <v>793</v>
-      </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="C271" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C271" s="1" t="s">
-        <v>798</v>
-      </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C273" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="C273" s="1" t="s">
-        <v>803</v>
-      </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="C275" s="1" t="s">
-        <v>808</v>
-      </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>813</v>
-      </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="C279" s="1" t="s">
-        <v>818</v>
-      </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="C281" s="1" t="s">
-        <v>823</v>
-      </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>828</v>
-      </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C285" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>833</v>
-      </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>838</v>
-      </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>843</v>
-      </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>848</v>
-      </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B293" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C293" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>853</v>
-      </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>858</v>
-      </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B297" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C297" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>863</v>
-      </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>868</v>
-      </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B301" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>873</v>
-      </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="C303" s="1" t="s">
-        <v>878</v>
-      </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8858,7 +8888,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>886</v>
@@ -8867,7 +8897,7 @@
         <v>887</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8876,7 +8906,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8885,7 +8915,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8894,7 +8924,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>892</v>
@@ -8903,7 +8933,7 @@
         <v>893</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8912,7 +8942,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>895</v>
@@ -8921,7 +8951,7 @@
         <v>896</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8930,7 +8960,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>898</v>
@@ -8939,7 +8969,7 @@
         <v>899</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8948,61 +8978,61 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B311" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="B311" s="1" t="s">
+      <c r="C311" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="C311" s="1" t="s">
+      <c r="D311" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E311" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E311" s="1" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>901</v>
+        <v>647</v>
       </c>
       <c r="B312" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="C312" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="C312" s="1" t="s">
+      <c r="D312" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E312" s="1" t="s">
         <v>906</v>
-      </c>
-      <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E312" s="1" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>901</v>
+        <v>647</v>
       </c>
       <c r="B313" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C313" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="C313" s="1" t="s">
+      <c r="D313" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E313" s="1" t="s">
         <v>909</v>
-      </c>
-      <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E313" s="1" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -9011,7 +9041,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9020,7 +9050,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9029,7 +9059,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9038,7 +9068,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9047,7 +9077,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9056,7 +9086,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9065,7 +9095,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9074,7 +9104,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9083,7 +9113,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9092,7 +9122,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9101,7 +9131,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9110,7 +9140,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9119,7 +9149,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9128,7 +9158,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9137,7 +9167,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9146,7 +9176,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9155,7 +9185,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9164,7 +9194,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9173,7 +9203,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9182,7 +9212,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9191,7 +9221,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9200,7 +9230,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9209,7 +9239,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9218,7 +9248,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9227,7 +9257,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9236,7 +9266,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9245,7 +9275,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9254,7 +9284,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9263,7 +9293,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9272,7 +9302,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9281,7 +9311,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9290,7 +9320,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9299,7 +9329,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9308,7 +9338,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9317,7 +9347,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9326,7 +9356,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9335,7 +9365,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9344,7 +9374,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9353,7 +9383,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9362,7 +9392,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>971</v>
@@ -9371,7 +9401,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9380,61 +9410,61 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B335" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="C335" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="C335" s="1" t="s">
+      <c r="D335" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E335" s="1" t="s">
         <v>976</v>
-      </c>
-      <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E335" s="1" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>974</v>
+        <v>910</v>
       </c>
       <c r="B336" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C336" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="C336" s="1" t="s">
+      <c r="D336" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E336" s="1" t="s">
         <v>979</v>
-      </c>
-      <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>974</v>
+        <v>910</v>
       </c>
       <c r="B337" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C337" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C337" s="1" t="s">
+      <c r="D337" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E337" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9443,7 +9473,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9452,7 +9482,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9461,7 +9491,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9470,7 +9500,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9479,7 +9509,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9488,7 +9518,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9497,7 +9527,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9506,7 +9536,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9515,7 +9545,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9524,7 +9554,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9533,7 +9563,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9542,7 +9572,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9551,7 +9581,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9560,7 +9590,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9569,7 +9599,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLogList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9578,7 +9608,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9587,7 +9617,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9596,7 +9626,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9605,7 +9635,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9614,7 +9644,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9623,7 +9653,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9632,7 +9662,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9641,7 +9671,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9650,7 +9680,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9659,7 +9689,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9668,7 +9698,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9677,7 +9707,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9686,7 +9716,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9695,7 +9725,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9704,7 +9734,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9713,7 +9743,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9722,7 +9752,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9731,7 +9761,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9740,7 +9770,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9749,7 +9779,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9758,7 +9788,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9767,7 +9797,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9776,7 +9806,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9785,7 +9815,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9794,7 +9824,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9803,7 +9833,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9812,7 +9842,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9821,7 +9851,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9830,7 +9860,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9839,7 +9869,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9848,7 +9878,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9857,7 +9887,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9866,70 +9896,70 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>1042</v>
+        <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>1065</v>
+        <v>1051</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9938,7 +9968,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1067</v>
@@ -9947,7 +9977,7 @@
         <v>1068</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9956,7 +9986,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1070</v>
@@ -9965,7 +9995,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9974,7 +10004,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1073</v>
@@ -9983,7 +10013,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -9992,7 +10022,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1076</v>
@@ -10001,7 +10031,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10010,7 +10040,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1079</v>
@@ -10019,7 +10049,7 @@
         <v>1080</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10028,7 +10058,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1082</v>
@@ -10037,11 +10067,65 @@
         <v>1083</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
         <v>1084</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D372" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D373" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D374" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>1093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/03/03 週五 17:12:54.53
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -410,7 +410,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月30日 10:58:58</t>
+    <t xml:space="preserve">2023年03月03日 13:29:15</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月09日 16:39:24</t>
+    <t xml:space="preserve">2023年03月02日 11:43:32</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -1661,7 +1661,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月30日 15:18:39</t>
+    <t xml:space="preserve">2023年03月02日 13:04:19</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/03/10 週五 17:30:35.66
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -410,7 +410,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月03日 13:29:15</t>
+    <t xml:space="preserve">2023年03月08日 10:10:57</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -419,7 +419,7 @@
     <t xml:space="preserve">商品參數主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月22日 14:05:08</t>
+    <t xml:space="preserve">2023年03月10日 10:08:51</t>
   </si>
   <si>
     <t xml:space="preserve">FacProdAcctFee</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月10日 19:05:48</t>
+    <t xml:space="preserve">2023年03月08日 10:49:16</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月06日 10:51:09</t>
+    <t xml:space="preserve">2023年03月09日 18:21:13</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -650,7 +650,7 @@
     <t xml:space="preserve">ACH授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月03日 14:51:53</t>
+    <t xml:space="preserve">2023年03月09日 18:21:36</t>
   </si>
   <si>
     <t xml:space="preserve">AchDeductMedia</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月25日 13:48:24</t>
+    <t xml:space="preserve">2023年03月09日 18:20:16</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -830,7 +830,7 @@
     <t xml:space="preserve">郵局授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月24日 13:59:24</t>
+    <t xml:space="preserve">2023年03月09日 18:20:39</t>
   </si>
   <si>
     <t xml:space="preserve">PostDeductMedia</t>
@@ -1328,7 +1328,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月31日 14:07:34</t>
+    <t xml:space="preserve">2023年03月06日 18:59:26</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1535,7 +1535,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月22日 13:12:09</t>
+    <t xml:space="preserve">2023年03月09日 18:39:55</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -3065,7 +3065,7 @@
     <t xml:space="preserve">ApLog敏感資料查詢紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月14日 17:04:20</t>
+    <t xml:space="preserve">2023年03月03日 17:33:05</t>
   </si>
   <si>
     <t xml:space="preserve">TxArchiveTable</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/03/21 週二 12:15:08.70
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -329,7 +329,7 @@
     <t xml:space="preserve">擔保品他項權利額度關聯檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月21日 11:25:02</t>
+    <t xml:space="preserve">2023年03月19日 18:49:54</t>
   </si>
   <si>
     <t xml:space="preserve">ClOwnerRelation</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月08日 10:49:16</t>
+    <t xml:space="preserve">2023年03月13日 16:08:21</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -593,7 +593,7 @@
     <t xml:space="preserve">計息明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:44:20</t>
+    <t xml:space="preserve">2023年03月13日 16:23:56</t>
   </si>
   <si>
     <t xml:space="preserve">LoanNotYet</t>
@@ -620,7 +620,7 @@
     <t xml:space="preserve">放款利率變動檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月19日 15:21:39</t>
+    <t xml:space="preserve">2023年03月13日 12:05:11</t>
   </si>
   <si>
     <t xml:space="preserve">LoanSynd</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月15日 20:29:32</t>
+    <t xml:space="preserve">2023年03月21日 11:46:41</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -1346,7 +1346,7 @@
     <t xml:space="preserve">會計科子細目設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:35:08</t>
+    <t xml:space="preserve">2023年03月14日 17:11:12</t>
   </si>
   <si>
     <t xml:space="preserve">CdAoDept</t>
@@ -1535,7 +1535,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月09日 18:39:55</t>
+    <t xml:space="preserve">2023年03月14日 11:07:00</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1661,7 +1661,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月02日 13:04:19</t>
+    <t xml:space="preserve">2023年03月16日 15:20:20</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/04/14 週五 17:08:54.34
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月31日 14:47:39</t>
+    <t xml:space="preserve">2023年04月12日 11:07:13</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月18日 17:55:37</t>
+    <t xml:space="preserve">2023年04月14日 14:11:02</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月04日 20:29:50</t>
+    <t xml:space="preserve">2023年04月14日 14:41:32</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -740,7 +740,7 @@
     <t xml:space="preserve">其他還款來源檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:00:58</t>
+    <t xml:space="preserve">2023年04月14日 14:05:01</t>
   </si>
   <si>
     <t xml:space="preserve">BatxRateChange</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/04/21 週五 18:10:56.08
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月12日 11:07:13</t>
+    <t xml:space="preserve">2023年04月17日 10:03:39</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月14日 14:11:02</t>
+    <t xml:space="preserve">2023年04月17日 16:07:13</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月14日 14:41:32</t>
+    <t xml:space="preserve">2023年04月17日 13:26:54</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -740,7 +740,7 @@
     <t xml:space="preserve">其他還款來源檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月14日 14:05:01</t>
+    <t xml:space="preserve">2023年04月18日 17:01:10</t>
   </si>
   <si>
     <t xml:space="preserve">BatxRateChange</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月21日 11:46:41</t>
+    <t xml:space="preserve">2023年04月20日 19:52:32</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -3296,7 +3296,7 @@
     <t xml:space="preserve">交易控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月14日 12:41:41</t>
+    <t xml:space="preserve">2023年04月17日 13:46:19</t>
   </si>
   <si>
     <t xml:space="preserve">TxUnLock</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/04/28 週五 17:19:48.58
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1086">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -284,7 +284,7 @@
     <t xml:space="preserve">擔保品主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月20日 13:49:26</t>
+    <t xml:space="preserve">2023年04月27日 15:19:48</t>
   </si>
   <si>
     <t xml:space="preserve">ClMovables</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月17日 13:26:54</t>
+    <t xml:space="preserve">2023年04月21日 19:39:26</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月20日 19:52:32</t>
+    <t xml:space="preserve">2023年04月26日 11:08:30</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月09日 18:20:16</t>
+    <t xml:space="preserve">2023年04月28日 09:31:55</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -1340,15 +1340,6 @@
     <t xml:space="preserve">2023年03月14日 17:11:12</t>
   </si>
   <si>
-    <t xml:space="preserve">CdAoDept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">放款專員所屬業務部室對照檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020年07月16日 10:19:18</t>
-  </si>
-  <si>
     <t xml:space="preserve">CdAppraisalCompany</t>
   </si>
   <si>
@@ -1385,15 +1376,6 @@
     <t xml:space="preserve">2022年05月30日 09:45:11</t>
   </si>
   <si>
-    <t xml:space="preserve">CdBankOld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">舊行庫資料檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年02月25日 16:31:39</t>
-  </si>
-  <si>
     <t xml:space="preserve">CdBaseRate</t>
   </si>
   <si>
@@ -1526,7 +1508,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月14日 11:07:00</t>
+    <t xml:space="preserve">2023年04月26日 13:55:32</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1782,15 +1764,6 @@
   </si>
   <si>
     <t xml:space="preserve">2022年01月20日 11:49:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataInputRecord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料傳入記錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月06日 10:23:34</t>
   </si>
   <si>
     <t xml:space="preserve">FinHoldRel</t>
@@ -3120,15 +3093,6 @@
   </si>
   <si>
     <t xml:space="preserve">2020年07月02日 18:20:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxControl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">作業流程控制檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月20日 18:42:31</t>
   </si>
   <si>
     <t xml:space="preserve">TxCruiser</t>
@@ -3420,7 +3384,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1097</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="2">
@@ -6026,7 +5990,7 @@
         <v>443</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAoDept.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E146" s="1" t="s">
@@ -6044,7 +6008,7 @@
         <v>446</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E147" s="1" t="s">
@@ -6062,7 +6026,7 @@
         <v>449</v>
       </c>
       <c r="D148" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E148" s="1" t="s">
@@ -6080,7 +6044,7 @@
         <v>452</v>
       </c>
       <c r="D149" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E149" s="1" t="s">
@@ -6098,7 +6062,7 @@
         <v>455</v>
       </c>
       <c r="D150" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E150" s="1" t="s">
@@ -6116,7 +6080,7 @@
         <v>458</v>
       </c>
       <c r="D151" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBankOld.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E151" s="1" t="s">
@@ -6134,7 +6098,7 @@
         <v>461</v>
       </c>
       <c r="D152" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E152" s="1" t="s">
@@ -6152,7 +6116,7 @@
         <v>464</v>
       </c>
       <c r="D153" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E153" s="1" t="s">
@@ -6170,7 +6134,7 @@
         <v>467</v>
       </c>
       <c r="D154" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -6188,7 +6152,7 @@
         <v>470</v>
       </c>
       <c r="D155" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -6206,7 +6170,7 @@
         <v>473</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -6224,7 +6188,7 @@
         <v>476</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -6242,7 +6206,7 @@
         <v>479</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E158" s="1" t="s">
@@ -6260,7 +6224,7 @@
         <v>482</v>
       </c>
       <c r="D159" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E159" s="1" t="s">
@@ -6278,7 +6242,7 @@
         <v>485</v>
       </c>
       <c r="D160" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCityRate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -6296,7 +6260,7 @@
         <v>488</v>
       </c>
       <c r="D161" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E161" s="1" t="s">
@@ -6314,7 +6278,7 @@
         <v>491</v>
       </c>
       <c r="D162" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCityRate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdClBatch.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -6332,7 +6296,7 @@
         <v>494</v>
       </c>
       <c r="D163" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -6350,7 +6314,7 @@
         <v>497</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdClBatch.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdComm.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -6368,7 +6332,7 @@
         <v>500</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdConvertCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E165" s="1" t="s">
@@ -6386,7 +6350,7 @@
         <v>503</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdComm.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -6404,7 +6368,7 @@
         <v>506</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdConvertCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -6422,7 +6386,7 @@
         <v>509</v>
       </c>
       <c r="D168" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E168" s="1" t="s">
@@ -6440,7 +6404,7 @@
         <v>512</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E169" s="1" t="s">
@@ -6458,7 +6422,7 @@
         <v>515</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E170" s="1" t="s">
@@ -6476,7 +6440,7 @@
         <v>518</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLand.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E171" s="1" t="s">
@@ -6494,7 +6458,7 @@
         <v>521</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E172" s="1" t="s">
@@ -6512,7 +6476,7 @@
         <v>524</v>
       </c>
       <c r="D173" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLand.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E173" s="1" t="s">
@@ -6530,7 +6494,7 @@
         <v>527</v>
       </c>
       <c r="D174" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E174" s="1" t="s">
@@ -6548,7 +6512,7 @@
         <v>530</v>
       </c>
       <c r="D175" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E175" s="1" t="s">
@@ -6566,7 +6530,7 @@
         <v>533</v>
       </c>
       <c r="D176" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E176" s="1" t="s">
@@ -6584,7 +6548,7 @@
         <v>536</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E177" s="1" t="s">
@@ -6602,7 +6566,7 @@
         <v>539</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E178" s="1" t="s">
@@ -6620,7 +6584,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6638,7 +6602,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6656,7 +6620,7 @@
         <v>548</v>
       </c>
       <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E181" s="1" t="s">
@@ -6674,7 +6638,7 @@
         <v>551</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6692,7 +6656,7 @@
         <v>554</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6710,7 +6674,7 @@
         <v>557</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6728,7 +6692,7 @@
         <v>560</v>
       </c>
       <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E185" s="1" t="s">
@@ -6746,7 +6710,7 @@
         <v>563</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6764,7 +6728,7 @@
         <v>566</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6782,7 +6746,7 @@
         <v>569</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6800,7 +6764,7 @@
         <v>572</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6818,7 +6782,7 @@
         <v>575</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E190" s="1" t="s">
@@ -6827,43 +6791,43 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>408</v>
+        <v>577</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>408</v>
+        <v>577</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6872,7 +6836,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6881,7 +6845,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6890,7 +6854,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6899,7 +6863,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6908,7 +6872,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\DataInputRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6917,7 +6881,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6926,7 +6890,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6935,7 +6899,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6944,7 +6908,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6953,7 +6917,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6962,7 +6926,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6971,7 +6935,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6980,7 +6944,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6989,7 +6953,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>605</v>
@@ -6998,7 +6962,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -7007,7 +6971,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>608</v>
@@ -7016,7 +6980,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -7025,7 +6989,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>611</v>
@@ -7034,7 +6998,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -7043,7 +7007,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>614</v>
@@ -7052,7 +7016,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7061,7 +7025,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>617</v>
@@ -7070,7 +7034,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7079,7 +7043,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>620</v>
@@ -7088,7 +7052,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7097,7 +7061,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>623</v>
@@ -7106,7 +7070,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7115,7 +7079,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>626</v>
@@ -7124,7 +7088,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7133,7 +7097,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>629</v>
@@ -7142,7 +7106,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7151,7 +7115,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>632</v>
@@ -7160,7 +7124,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7169,7 +7133,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>635</v>
@@ -7178,7 +7142,7 @@
         <v>636</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7187,7 +7151,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>638</v>
@@ -7196,7 +7160,7 @@
         <v>639</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -7205,61 +7169,61 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>583</v>
+        <v>641</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>583</v>
+        <v>641</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>583</v>
+        <v>641</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7268,7 +7232,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7277,7 +7241,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7286,7 +7250,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7295,7 +7259,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7304,7 +7268,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7313,7 +7277,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7322,7 +7286,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7331,7 +7295,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7340,7 +7304,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7349,7 +7313,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7358,7 +7322,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7367,7 +7331,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7376,7 +7340,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7385,7 +7349,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7394,7 +7358,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7403,7 +7367,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7412,7 +7376,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7421,7 +7385,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7430,7 +7394,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7439,7 +7403,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7448,7 +7412,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7457,7 +7421,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7466,7 +7430,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7475,7 +7439,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7484,7 +7448,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7493,7 +7457,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7502,7 +7466,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7511,7 +7475,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
@@ -7520,7 +7484,7 @@
         <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7529,7 +7493,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>696</v>
@@ -7538,7 +7502,7 @@
         <v>697</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
@@ -7547,1366 +7511,1366 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>699</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D231" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E231" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B232" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C232" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="C232" s="1" t="s">
+      <c r="D232" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="D233" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E233" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B234" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D234" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E234" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D235" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E235" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B236" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D236" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E236" s="1" t="s">
         <v>713</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D237" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B238" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D238" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>718</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D239" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E239" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B240" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="D240" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E240" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="D241" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E241" s="1" t="s">
         <v>725</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D242" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B243" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D243" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E243" s="1" t="s">
         <v>730</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B244" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D244" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>733</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D245" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E245" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="C245" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B246" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D246" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B247" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D247" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E247" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B248" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D248" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E248" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D249" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E249" s="1" t="s">
         <v>745</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B250" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D250" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>748</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D251" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E251" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B252" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D252" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E252" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D253" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E253" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B254" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D254" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D255" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E255" s="1" t="s">
         <v>760</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B256" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D256" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E256" s="1" t="s">
         <v>763</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D257" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B258" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D258" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B259" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D259" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E259" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B260" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D260" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E260" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D261" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E261" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B262" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D262" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E262" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D263" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E263" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>781</v>
+        <v>747</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>786</v>
+        <v>747</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>786</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>756</v>
+        <v>786</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B268" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D268" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E268" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="C268" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B269" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D269" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E269" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="C269" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B270" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D270" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E270" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="C270" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D271" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E271" s="1" t="s">
         <v>799</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B272" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D272" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E272" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D273" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E273" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="C273" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B274" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D274" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E274" s="1" t="s">
         <v>807</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D275" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E275" s="1" t="s">
         <v>809</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B276" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D276" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E276" s="1" t="s">
         <v>812</v>
-      </c>
-      <c r="C276" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D277" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E277" s="1" t="s">
         <v>814</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B278" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D278" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E278" s="1" t="s">
         <v>817</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D279" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E279" s="1" t="s">
         <v>819</v>
-      </c>
-      <c r="C279" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E279" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B280" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="D280" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E280" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E280" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="D281" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E281" s="1" t="s">
         <v>824</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B282" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="D282" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E282" s="1" t="s">
         <v>827</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="D283" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E283" s="1" t="s">
         <v>829</v>
-      </c>
-      <c r="C283" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B284" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D284" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E284" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="C284" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E284" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D285" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E285" s="1" t="s">
         <v>834</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B286" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D286" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E286" s="1" t="s">
         <v>837</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D287" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E287" s="1" t="s">
         <v>839</v>
-      </c>
-      <c r="C287" s="1" t="s">
-        <v>840</v>
-      </c>
-      <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E287" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B288" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D288" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E288" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>840</v>
-      </c>
-      <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D289" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E289" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B290" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D290" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E290" s="1" t="s">
         <v>847</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D291" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E291" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B292" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D292" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E292" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B293" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D293" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E293" s="1" t="s">
         <v>854</v>
-      </c>
-      <c r="C293" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B294" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D294" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E294" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="C294" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D295" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E295" s="1" t="s">
         <v>859</v>
-      </c>
-      <c r="C295" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B296" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D296" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E296" s="1" t="s">
         <v>862</v>
-      </c>
-      <c r="C296" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B297" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D297" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E297" s="1" t="s">
         <v>864</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="D298" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E298" s="1" t="s">
         <v>867</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="D299" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E299" s="1" t="s">
         <v>869</v>
-      </c>
-      <c r="C299" s="1" t="s">
-        <v>870</v>
-      </c>
-      <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B300" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D300" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E300" s="1" t="s">
         <v>872</v>
-      </c>
-      <c r="C300" s="1" t="s">
-        <v>870</v>
-      </c>
-      <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B301" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D301" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E301" s="1" t="s">
         <v>874</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>875</v>
-      </c>
-      <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E301" s="1" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B302" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D302" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E302" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="C302" s="1" t="s">
-        <v>875</v>
-      </c>
-      <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D303" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E303" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>880</v>
-      </c>
-      <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B304" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="D304" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E304" s="1" t="s">
         <v>882</v>
-      </c>
-      <c r="C304" s="1" t="s">
-        <v>880</v>
-      </c>
-      <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B305" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C305" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="C305" s="1" t="s">
+      <c r="D305" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E305" s="1" t="s">
         <v>885</v>
-      </c>
-      <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B306" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C306" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="C306" s="1" t="s">
-        <v>885</v>
-      </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8915,7 +8879,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8924,7 +8888,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8933,7 +8897,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>892</v>
@@ -8942,7 +8906,7 @@
         <v>893</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8951,7 +8915,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>895</v>
@@ -8960,7 +8924,7 @@
         <v>896</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8969,7 +8933,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>898</v>
@@ -8978,7 +8942,7 @@
         <v>899</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8987,7 +8951,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>901</v>
@@ -8996,7 +8960,7 @@
         <v>902</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -9005,61 +8969,61 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>650</v>
+        <v>904</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>650</v>
+        <v>904</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>650</v>
+        <v>904</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9068,7 +9032,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9077,7 +9041,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9086,7 +9050,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9095,7 +9059,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9104,7 +9068,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9113,7 +9077,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9122,7 +9086,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9131,7 +9095,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9140,7 +9104,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9149,7 +9113,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9158,7 +9122,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9167,7 +9131,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9176,7 +9140,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9185,7 +9149,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9194,7 +9158,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9203,7 +9167,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9212,7 +9176,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9221,7 +9185,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9230,7 +9194,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9239,7 +9203,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9248,7 +9212,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9257,7 +9221,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9266,7 +9230,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9275,7 +9239,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9284,7 +9248,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9293,7 +9257,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9302,7 +9266,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9311,7 +9275,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9320,7 +9284,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9329,7 +9293,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9338,7 +9302,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9347,7 +9311,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9356,7 +9320,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9365,7 +9329,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9374,7 +9338,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9383,7 +9347,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9392,7 +9356,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9401,7 +9365,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>971</v>
@@ -9410,7 +9374,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9419,7 +9383,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>974</v>
@@ -9428,7 +9392,7 @@
         <v>975</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9437,7 +9401,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>977</v>
@@ -9446,7 +9410,7 @@
         <v>978</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9455,61 +9419,61 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>913</v>
+        <v>980</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>913</v>
+        <v>980</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>913</v>
+        <v>980</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9518,7 +9482,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9527,7 +9491,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9536,7 +9500,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9545,7 +9509,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9554,7 +9518,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9563,7 +9527,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9572,7 +9536,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9581,7 +9545,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9590,7 +9554,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9599,7 +9563,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9608,7 +9572,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9617,7 +9581,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9626,7 +9590,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9635,7 +9599,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9644,7 +9608,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9653,7 +9617,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9662,7 +9626,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9671,7 +9635,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9680,7 +9644,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9689,7 +9653,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9698,7 +9662,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9707,7 +9671,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9716,7 +9680,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9725,7 +9689,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9734,7 +9698,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9743,7 +9707,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9752,7 +9716,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9761,7 +9725,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9770,7 +9734,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9779,7 +9743,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9788,7 +9752,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9797,7 +9761,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9806,7 +9770,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9815,7 +9779,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9824,7 +9788,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9833,7 +9797,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9842,7 +9806,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9851,7 +9815,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9860,7 +9824,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9869,7 +9833,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9878,7 +9842,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9887,7 +9851,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9896,7 +9860,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9905,88 +9869,88 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
       </c>
       <c r="C362" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D362" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E362" s="1" t="s">
         <v>1057</v>
-      </c>
-      <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E362" s="1" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B363" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C363" s="1" t="s">
         <v>1059</v>
       </c>
-      <c r="C363" s="1" t="s">
+      <c r="D363" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E363" s="1" t="s">
         <v>1060</v>
-      </c>
-      <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E363" s="1" t="s">
-        <v>1061</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B364" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C364" s="1" t="s">
         <v>1062</v>
       </c>
-      <c r="C364" s="1" t="s">
+      <c r="D364" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E364" s="1" t="s">
         <v>1063</v>
-      </c>
-      <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E364" s="1" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B365" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C365" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="C365" s="1" t="s">
+      <c r="D365" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E365" s="1" t="s">
         <v>1066</v>
-      </c>
-      <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E365" s="1" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B366" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C366" s="1" t="s">
         <v>1068</v>
       </c>
-      <c r="C366" s="1" t="s">
-        <v>1054</v>
-      </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9995,7 +9959,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1070</v>
@@ -10004,7 +9968,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -10013,7 +9977,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1073</v>
@@ -10022,7 +9986,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -10031,7 +9995,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1076</v>
@@ -10040,7 +10004,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10049,7 +10013,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1079</v>
@@ -10058,7 +10022,7 @@
         <v>1080</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10067,7 +10031,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1082</v>
@@ -10076,83 +10040,11 @@
         <v>1083</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
         <v>1084</v>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="B372" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C372" s="1" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D372" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E372" s="1" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="B373" s="1" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C373" s="1" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D373" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E373" s="1" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="B374" s="1" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C374" s="1" t="s">
-        <v>1092</v>
-      </c>
-      <c r="D374" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E374" s="1" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="B375" s="1" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C375" s="1" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D375" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E375" s="1" t="s">
-        <v>1096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/05/05 週五 17:00:48.08
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -302,7 +302,7 @@
     <t xml:space="preserve">擔保品編號新舊對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月07日 16:11:30</t>
+    <t xml:space="preserve">2023年05月04日 11:22:52</t>
   </si>
   <si>
     <t xml:space="preserve">ClOther</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月24日 18:02:27</t>
+    <t xml:space="preserve">2023年05月04日 16:53:05</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月17日 10:03:39</t>
+    <t xml:space="preserve">2023年05月04日 17:19:24</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月09日 18:21:13</t>
+    <t xml:space="preserve">2023年05月02日 10:58:51</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月21日 19:39:26</t>
+    <t xml:space="preserve">2023年05月03日 11:27:17</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月26日 11:08:30</t>
+    <t xml:space="preserve">2023年05月03日 19:44:41</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -1058,7 +1058,7 @@
     <t xml:space="preserve">一般債權撥付資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月06日 15:15:41</t>
+    <t xml:space="preserve">2023年05月04日 19:21:52</t>
   </si>
   <si>
     <t xml:space="preserve">NegFinAcct</t>
@@ -1301,7 +1301,7 @@
     <t xml:space="preserve">會計借新還舊檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月25日 19:55:49</t>
+    <t xml:space="preserve">2023年05月04日 16:53:08</t>
   </si>
   <si>
     <t xml:space="preserve">AcMain</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/05/12 週五 17:11:22.98
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -284,7 +284,7 @@
     <t xml:space="preserve">擔保品主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月27日 15:19:48</t>
+    <t xml:space="preserve">2023年05月12日 12:37:44</t>
   </si>
   <si>
     <t xml:space="preserve">ClMovables</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">火險初保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月15日 20:07:01</t>
+    <t xml:space="preserve">2023年05月11日 12:33:01</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenew</t>
@@ -839,7 +839,7 @@
     <t xml:space="preserve">郵局扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月08日 14:41:06</t>
+    <t xml:space="preserve">2023年05月05日 18:16:47</t>
   </si>
   <si>
     <t xml:space="preserve">RepayActChangeLog</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月07日 13:17:53</t>
+    <t xml:space="preserve">2023年05月09日 11:34:11</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -3164,7 +3164,7 @@
     <t xml:space="preserve">查詢紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月24日 10:25:59</t>
+    <t xml:space="preserve">2023年05月11日 18:38:44</t>
   </si>
   <si>
     <t xml:space="preserve">TxLock</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/05/19 週五 17:22:58.97
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="1089">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月04日 16:53:05</t>
+    <t xml:space="preserve">2023年05月18日 10:42:39</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月02日 10:58:51</t>
+    <t xml:space="preserve">2023年05月19日 12:19:18</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -803,7 +803,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月15日 20:06:36</t>
+    <t xml:space="preserve">2023年05月19日 13:24:23</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月28日 09:31:55</t>
+    <t xml:space="preserve">2023年05月19日 12:19:14</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -1148,7 +1148,7 @@
     <t xml:space="preserve">協辦人員等級檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:27:22</t>
+    <t xml:space="preserve">2023年05月19日 14:58:04</t>
   </si>
   <si>
     <t xml:space="preserve">PfCoOfficerLog</t>
@@ -1157,7 +1157,7 @@
     <t xml:space="preserve">協辦人員等級歷程檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月27日 13:48:53</t>
+    <t xml:space="preserve">2023年05月19日 16:04:06</t>
   </si>
   <si>
     <t xml:space="preserve">PfDeparment</t>
@@ -1193,7 +1193,7 @@
     <t xml:space="preserve">內網報表業績調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:28:43</t>
+    <t xml:space="preserve">2023年05月18日 18:13:01</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetail</t>
@@ -1217,7 +1217,7 @@
     <t xml:space="preserve">介紹、協辦獎金明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:30:02</t>
+    <t xml:space="preserve">2023年05月18日 12:44:47</t>
   </si>
   <si>
     <t xml:space="preserve">PfRewardMedia</t>
@@ -1226,7 +1226,7 @@
     <t xml:space="preserve">獎金媒體發放檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月02日 16:50:40</t>
+    <t xml:space="preserve">2023年05月18日 17:28:31</t>
   </si>
   <si>
     <t xml:space="preserve">SpecInnReCheck</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">共用代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月17日 10:50:54</t>
+    <t xml:space="preserve">2023年05月15日 16:28:26</t>
   </si>
   <si>
     <t xml:space="preserve">CdComm</t>
@@ -1715,7 +1715,7 @@
     <t xml:space="preserve">批次工作主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月12日 16:34:36</t>
+    <t xml:space="preserve">2023年05月15日 17:25:02</t>
   </si>
   <si>
     <t xml:space="preserve">QuitEmp</t>
@@ -3095,6 +3095,15 @@
     <t xml:space="preserve">2020年07月02日 18:20:55</t>
   </si>
   <si>
+    <t xml:space="preserve">TxControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">作業流程控制檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月19日 12:32:26</t>
+  </si>
+  <si>
     <t xml:space="preserve">TxCruiser</t>
   </si>
   <si>
@@ -3155,7 +3164,7 @@
     <t xml:space="preserve">假日檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年07月13日 09:41:39</t>
+    <t xml:space="preserve">2021年07月15日 10:15:27</t>
   </si>
   <si>
     <t xml:space="preserve">TxInquiry</t>
@@ -3384,7 +3393,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="2">
@@ -9698,7 +9707,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9716,7 +9725,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9734,7 +9743,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9752,7 +9761,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9770,7 +9779,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9788,7 +9797,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9806,7 +9815,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9824,7 +9833,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9842,7 +9851,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9860,7 +9869,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9875,14 +9884,14 @@
         <v>1056</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>1042</v>
+        <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="363">
@@ -9890,13 +9899,13 @@
         <v>980</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>1059</v>
+        <v>1045</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9914,7 +9923,7 @@
         <v>1062</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9932,7 +9941,7 @@
         <v>1065</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9950,7 +9959,7 @@
         <v>1068</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9968,7 +9977,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9986,7 +9995,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -10004,7 +10013,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10022,7 +10031,7 @@
         <v>1080</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10040,11 +10049,29 @@
         <v>1083</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
         <v>1084</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D372" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>1087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/05/26 週五 17:02:53.67
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1092">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">擔保品不動產建物檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月21日 13:49:53</t>
+    <t xml:space="preserve">2023年05月25日 11:47:24</t>
   </si>
   <si>
     <t xml:space="preserve">ClBuildingOwner</t>
@@ -218,10 +218,10 @@
     <t xml:space="preserve">ClEva</t>
   </si>
   <si>
-    <t xml:space="preserve">擔保品重評資料檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年10月26日 10:13:38</t>
+    <t xml:space="preserve">擔保品鑑價資料檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月25日 11:34:07</t>
   </si>
   <si>
     <t xml:space="preserve">ClFac</t>
@@ -257,7 +257,7 @@
     <t xml:space="preserve">擔保品不動產土地檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年08月27日 17:43:07</t>
+    <t xml:space="preserve">2023年05月25日 12:24:11</t>
   </si>
   <si>
     <t xml:space="preserve">ClLandOwner</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月03日 19:44:41</t>
+    <t xml:space="preserve">2023年05月22日 16:44:23</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -986,7 +986,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月19日 10:44:25</t>
+    <t xml:space="preserve">2023年05月23日 12:05:13</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -2757,6 +2757,15 @@
   </si>
   <si>
     <t xml:space="preserve">2023年02月23日 14:26:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lahgtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS400建物明細資料檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月25日 15:37:55</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyDpUnpaidExpense</t>
@@ -3393,7 +3402,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="2">
@@ -9041,7 +9050,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9059,7 +9068,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9077,7 +9086,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9095,7 +9104,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9113,7 +9122,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9131,7 +9140,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9149,7 +9158,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9167,7 +9176,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9185,7 +9194,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9203,7 +9212,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9221,7 +9230,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9239,7 +9248,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9257,7 +9266,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9275,7 +9284,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9293,7 +9302,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9311,7 +9320,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9329,7 +9338,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9347,7 +9356,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9365,7 +9374,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9383,7 +9392,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9401,7 +9410,7 @@
         <v>975</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9419,7 +9428,7 @@
         <v>978</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9428,25 +9437,25 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B337" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="B337" s="1" t="s">
+      <c r="C337" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C337" s="1" t="s">
+      <c r="D337" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E337" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9455,7 +9464,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9464,7 +9473,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9473,7 +9482,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9482,7 +9491,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9491,7 +9500,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9500,7 +9509,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9509,7 +9518,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9518,7 +9527,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9527,7 +9536,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9536,7 +9545,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9545,7 +9554,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9554,7 +9563,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9563,7 +9572,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9572,7 +9581,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9581,7 +9590,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9590,7 +9599,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9599,7 +9608,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9608,7 +9617,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9617,7 +9626,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9626,7 +9635,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9635,7 +9644,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9644,7 +9653,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9653,7 +9662,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9662,7 +9671,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9671,7 +9680,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9680,7 +9689,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9689,7 +9698,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9698,7 +9707,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9707,7 +9716,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9716,7 +9725,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9725,7 +9734,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9734,7 +9743,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9743,7 +9752,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9752,7 +9761,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9761,7 +9770,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9770,7 +9779,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9779,7 +9788,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9788,7 +9797,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9797,7 +9806,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9806,7 +9815,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9815,7 +9824,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9824,7 +9833,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9833,7 +9842,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9842,7 +9851,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9851,7 +9860,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9860,7 +9869,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9869,7 +9878,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9878,7 +9887,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
@@ -9887,7 +9896,7 @@
         <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9896,34 +9905,34 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1059</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>1045</v>
+        <v>1060</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>1062</v>
+        <v>1048</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9932,7 +9941,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1064</v>
@@ -9941,7 +9950,7 @@
         <v>1065</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9950,7 +9959,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1067</v>
@@ -9959,7 +9968,7 @@
         <v>1068</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9968,7 +9977,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1070</v>
@@ -9977,7 +9986,7 @@
         <v>1071</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9986,7 +9995,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1073</v>
@@ -9995,7 +10004,7 @@
         <v>1074</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -10004,7 +10013,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1076</v>
@@ -10013,7 +10022,7 @@
         <v>1077</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10022,7 +10031,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1079</v>
@@ -10031,7 +10040,7 @@
         <v>1080</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10040,7 +10049,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1082</v>
@@ -10049,7 +10058,7 @@
         <v>1083</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
@@ -10058,7 +10067,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>1085</v>
@@ -10067,11 +10076,29 @@
         <v>1086</v>
       </c>
       <c r="D372" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E372" s="1" t="s">
         <v>1087</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D373" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>1090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/06/02 週五 17:31:38.49
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月04日 17:19:24</t>
+    <t xml:space="preserve">2023年06月02日 12:41:46</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月02日 11:43:32</t>
+    <t xml:space="preserve">2023年06月02日 10:45:21</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -995,7 +995,7 @@
     <t xml:space="preserve">資金運用概況檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年08月10日 17:08:38</t>
+    <t xml:space="preserve">2023年06月01日 11:11:26</t>
   </si>
   <si>
     <t xml:space="preserve">InnLoanMeeting</t>
@@ -1121,16 +1121,7 @@
     <t xml:space="preserve">房貸專員業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:26:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PfBsDetailAdjust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">房貸專員業績調整檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月16日 15:21:13</t>
+    <t xml:space="preserve">2023年05月30日 10:59:24</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsOfficer</t>
@@ -1199,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:29:25</t>
+    <t xml:space="preserve">2023年05月30日 14:28:22</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1208,7 +1199,7 @@
     <t xml:space="preserve">介紹人業績調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月03日 12:14:54</t>
+    <t xml:space="preserve">2023年05月30日 18:15:34</t>
   </si>
   <si>
     <t xml:space="preserve">PfReward</t>
@@ -1472,7 +1463,7 @@
     <t xml:space="preserve">地區利率檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年10月11日 17:17:12</t>
+    <t xml:space="preserve">2023年05月31日 17:57:37</t>
   </si>
   <si>
     <t xml:space="preserve">CdCl</t>
@@ -1526,7 +1517,7 @@
     <t xml:space="preserve">員工資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月22日 09:52:18</t>
+    <t xml:space="preserve">2023年05月29日 16:42:57</t>
   </si>
   <si>
     <t xml:space="preserve">CdGseq</t>
@@ -1715,7 +1706,7 @@
     <t xml:space="preserve">批次工作主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月15日 17:25:02</t>
+    <t xml:space="preserve">2023年05月31日 17:42:04</t>
   </si>
   <si>
     <t xml:space="preserve">QuitEmp</t>
@@ -1773,7 +1764,7 @@
 (使用報表：LM049、LQ005)</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月22日 13:53:36</t>
+    <t xml:space="preserve">2023年05月31日 15:39:38</t>
   </si>
   <si>
     <t xml:space="preserve">Ias39IntMethod</t>
@@ -1837,7 +1828,7 @@
 (使用報表：LM013) </t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月10日 16:15:11</t>
+    <t xml:space="preserve">2023年05月31日 15:39:56</t>
   </si>
   <si>
     <t xml:space="preserve">LifeRelHead</t>
@@ -1847,7 +1838,7 @@
 (使用報表：LM013、LM042、LM050)</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月23日 13:58:34</t>
+    <t xml:space="preserve">2023年05月31日 15:40:00</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIfrs9Ap</t>
@@ -3047,7 +3038,7 @@
     <t xml:space="preserve">歷史封存表紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月26日 11:10:02</t>
+    <t xml:space="preserve">2023年05月29日 13:38:56</t>
   </si>
   <si>
     <t xml:space="preserve">TxAttachment</t>
@@ -3165,6 +3156,15 @@
   </si>
   <si>
     <t xml:space="preserve">2021年12月15日 10:31:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxFtpUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTP權限檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月25日 18:51:49</t>
   </si>
   <si>
     <t xml:space="preserve">TxHoliday</t>
@@ -5576,7 +5576,7 @@
         <v>371</v>
       </c>
       <c r="D122" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfBsDetailAdjust.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfBsOfficer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -5594,7 +5594,7 @@
         <v>374</v>
       </c>
       <c r="D123" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfBsOfficer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfCoOfficer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -5612,7 +5612,7 @@
         <v>377</v>
       </c>
       <c r="D124" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfCoOfficer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfCoOfficerLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -5630,7 +5630,7 @@
         <v>380</v>
       </c>
       <c r="D125" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfCoOfficerLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfDeparment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -5648,7 +5648,7 @@
         <v>383</v>
       </c>
       <c r="D126" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfDeparment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E126" s="1" t="s">
@@ -5666,7 +5666,7 @@
         <v>386</v>
       </c>
       <c r="D127" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfInsCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -5684,7 +5684,7 @@
         <v>389</v>
       </c>
       <c r="D128" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfInsCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfIntranetAdjust.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -5699,14 +5699,14 @@
         <v>391</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D129" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfItDetail.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="D129" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfIntranetAdjust.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="130">
@@ -5714,13 +5714,13 @@
         <v>279</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D130" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfItDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfItDetailAdjust.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -5738,7 +5738,7 @@
         <v>397</v>
       </c>
       <c r="D131" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfItDetailAdjust.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfReward.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E131" s="1" t="s">
@@ -5756,7 +5756,7 @@
         <v>400</v>
       </c>
       <c r="D132" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfReward.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfRewardMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E132" s="1" t="s">
@@ -5774,7 +5774,7 @@
         <v>403</v>
       </c>
       <c r="D133" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\PfRewardMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\SpecInnReCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E133" s="1" t="s">
@@ -5783,25 +5783,25 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>279</v>
+        <v>405</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D134" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L5-管理性作業\SpecInnReCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcAcctCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>409</v>
@@ -5810,7 +5810,7 @@
         <v>410</v>
       </c>
       <c r="D135" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcAcctCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcAcctCheckDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -5819,7 +5819,7 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>412</v>
@@ -5828,7 +5828,7 @@
         <v>413</v>
       </c>
       <c r="D136" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcAcctCheckDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcClose.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -5837,7 +5837,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>415</v>
@@ -5846,7 +5846,7 @@
         <v>416</v>
       </c>
       <c r="D137" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcClose.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -5855,7 +5855,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>418</v>
@@ -5864,7 +5864,7 @@
         <v>419</v>
       </c>
       <c r="D138" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -5873,7 +5873,7 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>421</v>
@@ -5882,7 +5882,7 @@
         <v>422</v>
       </c>
       <c r="D139" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanIntCashFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E139" s="1" t="s">
@@ -5891,7 +5891,7 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>424</v>
@@ -5900,7 +5900,7 @@
         <v>425</v>
       </c>
       <c r="D140" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanIntCashFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanRenew.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E140" s="1" t="s">
@@ -5909,7 +5909,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>427</v>
@@ -5918,7 +5918,7 @@
         <v>428</v>
       </c>
       <c r="D141" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcLoanRenew.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E141" s="1" t="s">
@@ -5927,7 +5927,7 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>430</v>
@@ -5936,7 +5936,7 @@
         <v>431</v>
       </c>
       <c r="D142" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcReceivable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E142" s="1" t="s">
@@ -5945,7 +5945,7 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>433</v>
@@ -5954,7 +5954,7 @@
         <v>434</v>
       </c>
       <c r="D143" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\AcReceivable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcBook.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E143" s="1" t="s">
@@ -5963,7 +5963,7 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>436</v>
@@ -5972,7 +5972,7 @@
         <v>437</v>
       </c>
       <c r="D144" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcBook.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -5981,7 +5981,7 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>439</v>
@@ -5990,7 +5990,7 @@
         <v>440</v>
       </c>
       <c r="D145" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAcCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E145" s="1" t="s">
@@ -5999,7 +5999,7 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>442</v>
@@ -6008,7 +6008,7 @@
         <v>443</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraisalCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E146" s="1" t="s">
@@ -6017,7 +6017,7 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>445</v>
@@ -6026,7 +6026,7 @@
         <v>446</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdAppraiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E147" s="1" t="s">
@@ -6035,7 +6035,7 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>448</v>
@@ -6044,7 +6044,7 @@
         <v>449</v>
       </c>
       <c r="D148" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdArea.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E148" s="1" t="s">
@@ -6053,7 +6053,7 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>451</v>
@@ -6062,7 +6062,7 @@
         <v>452</v>
       </c>
       <c r="D149" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBank.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E149" s="1" t="s">
@@ -6071,7 +6071,7 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>454</v>
@@ -6080,7 +6080,7 @@
         <v>455</v>
       </c>
       <c r="D150" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBaseRate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E150" s="1" t="s">
@@ -6089,7 +6089,7 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>457</v>
@@ -6098,7 +6098,7 @@
         <v>458</v>
       </c>
       <c r="D151" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBcm.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E151" s="1" t="s">
@@ -6107,7 +6107,7 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>460</v>
@@ -6116,7 +6116,7 @@
         <v>461</v>
       </c>
       <c r="D152" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonus.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E152" s="1" t="s">
@@ -6125,7 +6125,7 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>463</v>
@@ -6134,7 +6134,7 @@
         <v>464</v>
       </c>
       <c r="D153" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBonusCo.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E153" s="1" t="s">
@@ -6143,7 +6143,7 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>466</v>
@@ -6152,7 +6152,7 @@
         <v>467</v>
       </c>
       <c r="D154" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranch.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -6161,7 +6161,7 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>469</v>
@@ -6170,7 +6170,7 @@
         <v>470</v>
       </c>
       <c r="D155" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBranchGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -6179,7 +6179,7 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>472</v>
@@ -6188,7 +6188,7 @@
         <v>473</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBudget.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -6197,7 +6197,7 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>475</v>
@@ -6206,7 +6206,7 @@
         <v>476</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdBuildingCost.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -6215,7 +6215,7 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>478</v>
@@ -6224,7 +6224,7 @@
         <v>479</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCashFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E158" s="1" t="s">
@@ -6233,7 +6233,7 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>481</v>
@@ -6242,7 +6242,7 @@
         <v>482</v>
       </c>
       <c r="D159" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCity.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCityRate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E159" s="1" t="s">
@@ -6251,7 +6251,7 @@
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>484</v>
@@ -6260,7 +6260,7 @@
         <v>485</v>
       </c>
       <c r="D160" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCityRate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -6269,7 +6269,7 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>487</v>
@@ -6278,7 +6278,7 @@
         <v>488</v>
       </c>
       <c r="D161" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdClBatch.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E161" s="1" t="s">
@@ -6287,7 +6287,7 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>490</v>
@@ -6296,7 +6296,7 @@
         <v>491</v>
       </c>
       <c r="D162" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdClBatch.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -6305,7 +6305,7 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>493</v>
@@ -6314,7 +6314,7 @@
         <v>494</v>
       </c>
       <c r="D163" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdComm.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -6323,7 +6323,7 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>496</v>
@@ -6332,7 +6332,7 @@
         <v>497</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdComm.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdConvertCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -6341,7 +6341,7 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>499</v>
@@ -6350,7 +6350,7 @@
         <v>500</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdConvertCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E165" s="1" t="s">
@@ -6359,7 +6359,7 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>502</v>
@@ -6368,7 +6368,7 @@
         <v>503</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -6377,7 +6377,7 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>505</v>
@@ -6386,7 +6386,7 @@
         <v>506</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGseq.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -6395,7 +6395,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>508</v>
@@ -6404,7 +6404,7 @@
         <v>509</v>
       </c>
       <c r="D168" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdGuarantor.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E168" s="1" t="s">
@@ -6413,7 +6413,7 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>511</v>
@@ -6422,7 +6422,7 @@
         <v>512</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdIndustry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E169" s="1" t="s">
@@ -6431,7 +6431,7 @@
     </row>
     <row r="170">
       <c r="A170" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>514</v>
@@ -6440,7 +6440,7 @@
         <v>515</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdInsurer.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLand.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E170" s="1" t="s">
@@ -6449,7 +6449,7 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>517</v>
@@ -6458,7 +6458,7 @@
         <v>518</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLand.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E171" s="1" t="s">
@@ -6467,7 +6467,7 @@
     </row>
     <row r="172">
       <c r="A172" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>520</v>
@@ -6476,7 +6476,7 @@
         <v>521</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandOffice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E172" s="1" t="s">
@@ -6485,7 +6485,7 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>523</v>
@@ -6494,7 +6494,7 @@
         <v>524</v>
       </c>
       <c r="D173" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLandSection.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E173" s="1" t="s">
@@ -6503,7 +6503,7 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>526</v>
@@ -6512,7 +6512,7 @@
         <v>527</v>
       </c>
       <c r="D174" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdLoanNotYet.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E174" s="1" t="s">
@@ -6521,7 +6521,7 @@
     </row>
     <row r="175">
       <c r="A175" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>529</v>
@@ -6530,7 +6530,7 @@
         <v>530</v>
       </c>
       <c r="D175" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdOverdue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E175" s="1" t="s">
@@ -6539,7 +6539,7 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>532</v>
@@ -6548,7 +6548,7 @@
         <v>533</v>
       </c>
       <c r="D176" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPerformance.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E176" s="1" t="s">
@@ -6557,7 +6557,7 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>535</v>
@@ -6566,7 +6566,7 @@
         <v>536</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdPfParms.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E177" s="1" t="s">
@@ -6575,7 +6575,7 @@
     </row>
     <row r="178">
       <c r="A178" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>538</v>
@@ -6584,7 +6584,7 @@
         <v>539</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdReport.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E178" s="1" t="s">
@@ -6593,7 +6593,7 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>541</v>
@@ -6602,7 +6602,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6611,7 +6611,7 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>544</v>
@@ -6620,7 +6620,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6629,7 +6629,7 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>547</v>
@@ -6638,7 +6638,7 @@
         <v>548</v>
       </c>
       <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E181" s="1" t="s">
@@ -6647,7 +6647,7 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>550</v>
@@ -6656,7 +6656,7 @@
         <v>551</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6665,7 +6665,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>553</v>
@@ -6674,7 +6674,7 @@
         <v>554</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6683,7 +6683,7 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>556</v>
@@ -6692,7 +6692,7 @@
         <v>557</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6701,7 +6701,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>559</v>
@@ -6710,7 +6710,7 @@
         <v>560</v>
       </c>
       <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E185" s="1" t="s">
@@ -6719,7 +6719,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>562</v>
@@ -6728,7 +6728,7 @@
         <v>563</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6737,7 +6737,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>565</v>
@@ -6746,7 +6746,7 @@
         <v>566</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6755,7 +6755,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>568</v>
@@ -6764,7 +6764,7 @@
         <v>569</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6773,7 +6773,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>571</v>
@@ -6782,7 +6782,7 @@
         <v>572</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6791,25 +6791,25 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
-        <v>408</v>
+        <v>574</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6818,7 +6818,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6827,7 +6827,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6836,7 +6836,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6845,7 +6845,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6854,7 +6854,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6863,7 +6863,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6872,7 +6872,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6881,7 +6881,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6890,7 +6890,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6899,7 +6899,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6908,7 +6908,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6917,7 +6917,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6926,7 +6926,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6935,7 +6935,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6944,7 +6944,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6953,7 +6953,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6962,7 +6962,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6971,7 +6971,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>605</v>
@@ -6980,7 +6980,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6989,7 +6989,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>608</v>
@@ -6998,7 +6998,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -7007,7 +7007,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>611</v>
@@ -7016,7 +7016,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -7025,7 +7025,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>614</v>
@@ -7034,7 +7034,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7043,7 +7043,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>617</v>
@@ -7052,7 +7052,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7061,7 +7061,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>620</v>
@@ -7070,7 +7070,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7079,7 +7079,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>623</v>
@@ -7088,7 +7088,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7097,7 +7097,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>626</v>
@@ -7106,7 +7106,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7115,7 +7115,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>629</v>
@@ -7124,7 +7124,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7133,7 +7133,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>632</v>
@@ -7142,7 +7142,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7151,7 +7151,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>635</v>
@@ -7160,7 +7160,7 @@
         <v>636</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7169,25 +7169,25 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
-        <v>577</v>
+        <v>638</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7196,7 +7196,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7205,7 +7205,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7214,7 +7214,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7223,7 +7223,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7232,7 +7232,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7241,7 +7241,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7250,7 +7250,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7259,7 +7259,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7268,7 +7268,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7277,7 +7277,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7286,7 +7286,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7295,7 +7295,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7304,7 +7304,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7313,7 +7313,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7322,7 +7322,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7331,7 +7331,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7340,7 +7340,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7349,7 +7349,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7358,7 +7358,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7367,7 +7367,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7376,7 +7376,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7385,7 +7385,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7394,7 +7394,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7403,7 +7403,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7412,7 +7412,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7421,7 +7421,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7430,7 +7430,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7439,7 +7439,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7448,7 +7448,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7457,7 +7457,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7466,7 +7466,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7475,7 +7475,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7484,7 +7484,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7493,7 +7493,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
@@ -7502,7 +7502,7 @@
         <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7511,34 +7511,34 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>696</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D230" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B231" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C231" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="C231" s="1" t="s">
-        <v>697</v>
-      </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
@@ -7547,34 +7547,34 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>701</v>
       </c>
       <c r="C232" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D232" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>702</v>
-      </c>
-      <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="C233" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>702</v>
-      </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
@@ -7583,34 +7583,34 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>706</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D234" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E234" s="1" t="s">
         <v>707</v>
-      </c>
-      <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>707</v>
-      </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
@@ -7619,34 +7619,34 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>711</v>
       </c>
       <c r="C236" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D236" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E236" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="C237" s="1" t="s">
-        <v>712</v>
-      </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
@@ -7655,34 +7655,34 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>716</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D238" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="C239" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="C239" s="1" t="s">
-        <v>717</v>
-      </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
@@ -7691,34 +7691,34 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>721</v>
       </c>
       <c r="C240" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D240" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E240" s="1" t="s">
         <v>722</v>
-      </c>
-      <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>722</v>
-      </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
@@ -7727,34 +7727,34 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>726</v>
       </c>
       <c r="C242" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D242" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B243" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>727</v>
-      </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
@@ -7763,34 +7763,34 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>731</v>
       </c>
       <c r="C244" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D244" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C245" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>732</v>
-      </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
@@ -7799,34 +7799,34 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>736</v>
       </c>
       <c r="C246" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D246" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B247" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>737</v>
-      </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
@@ -7835,34 +7835,34 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>741</v>
       </c>
       <c r="C248" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D248" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E248" s="1" t="s">
         <v>742</v>
-      </c>
-      <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="C249" s="1" t="s">
-        <v>742</v>
-      </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
@@ -7871,34 +7871,34 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>746</v>
       </c>
       <c r="C250" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D250" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C251" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C251" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
@@ -7907,34 +7907,34 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>751</v>
       </c>
       <c r="C252" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D252" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E252" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C253" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>752</v>
-      </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
@@ -7943,34 +7943,34 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>756</v>
       </c>
       <c r="C254" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D254" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>757</v>
-      </c>
-      <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>757</v>
-      </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
@@ -7979,34 +7979,34 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>761</v>
       </c>
       <c r="C256" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D256" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E256" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="C257" s="1" t="s">
-        <v>762</v>
-      </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
@@ -8015,34 +8015,34 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>766</v>
       </c>
       <c r="C258" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="D258" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B259" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="C259" s="1" t="s">
-        <v>767</v>
-      </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
@@ -8051,34 +8051,34 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>771</v>
       </c>
       <c r="C260" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="D260" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E260" s="1" t="s">
         <v>772</v>
-      </c>
-      <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="C261" s="1" t="s">
-        <v>772</v>
-      </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
@@ -8087,70 +8087,70 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>776</v>
       </c>
       <c r="C262" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D262" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E262" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D263" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E263" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B264" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D264" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E264" s="1" t="s">
         <v>781</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B265" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C265" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="C265" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
@@ -8159,34 +8159,34 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>785</v>
       </c>
       <c r="C266" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D266" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E266" s="1" t="s">
         <v>786</v>
-      </c>
-      <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B267" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="C267" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="C267" s="1" t="s">
-        <v>786</v>
-      </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -8195,34 +8195,34 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>790</v>
       </c>
       <c r="C268" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="D268" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E268" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B269" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C269" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="C269" s="1" t="s">
-        <v>791</v>
-      </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
@@ -8231,34 +8231,34 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>795</v>
       </c>
       <c r="C270" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="D270" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E270" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C271" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="C271" s="1" t="s">
-        <v>796</v>
-      </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
@@ -8267,34 +8267,34 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>800</v>
       </c>
       <c r="C272" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D272" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E272" s="1" t="s">
         <v>801</v>
-      </c>
-      <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="C273" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="C273" s="1" t="s">
-        <v>801</v>
-      </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
@@ -8303,34 +8303,34 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>805</v>
       </c>
       <c r="C274" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="D274" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E274" s="1" t="s">
         <v>806</v>
-      </c>
-      <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="C275" s="1" t="s">
-        <v>806</v>
-      </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
@@ -8339,34 +8339,34 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>810</v>
       </c>
       <c r="C276" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="D276" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E276" s="1" t="s">
         <v>811</v>
-      </c>
-      <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>811</v>
-      </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
@@ -8375,34 +8375,34 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>815</v>
       </c>
       <c r="C278" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="D278" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E278" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="C279" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
@@ -8411,34 +8411,34 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>820</v>
       </c>
       <c r="C280" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D280" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E280" s="1" t="s">
         <v>821</v>
-      </c>
-      <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E280" s="1" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="C281" s="1" t="s">
-        <v>821</v>
-      </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
@@ -8447,34 +8447,34 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>825</v>
       </c>
       <c r="C282" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D282" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E282" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>826</v>
-      </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
@@ -8483,34 +8483,34 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>830</v>
       </c>
       <c r="C284" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D284" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E284" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E284" s="1" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C285" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>831</v>
-      </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
@@ -8519,34 +8519,34 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>835</v>
       </c>
       <c r="C286" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="D286" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E286" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>836</v>
-      </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -8555,34 +8555,34 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>840</v>
       </c>
       <c r="C288" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D288" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E288" s="1" t="s">
         <v>841</v>
-      </c>
-      <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>841</v>
-      </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
@@ -8591,34 +8591,34 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>845</v>
       </c>
       <c r="C290" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="D290" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E290" s="1" t="s">
         <v>846</v>
-      </c>
-      <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>846</v>
-      </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
@@ -8627,34 +8627,34 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>850</v>
       </c>
       <c r="C292" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D292" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E292" s="1" t="s">
         <v>851</v>
-      </c>
-      <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B293" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C293" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>851</v>
-      </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
@@ -8663,34 +8663,34 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>855</v>
       </c>
       <c r="C294" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="D294" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E294" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>856</v>
-      </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
@@ -8699,34 +8699,34 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>860</v>
       </c>
       <c r="C296" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D296" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E296" s="1" t="s">
         <v>861</v>
-      </c>
-      <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B297" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="C297" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>861</v>
-      </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
@@ -8735,34 +8735,34 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>865</v>
       </c>
       <c r="C298" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D298" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E298" s="1" t="s">
         <v>866</v>
-      </c>
-      <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>866</v>
-      </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
@@ -8771,34 +8771,34 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>870</v>
       </c>
       <c r="C300" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D300" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E300" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B301" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>871</v>
-      </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
@@ -8807,34 +8807,34 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>875</v>
       </c>
       <c r="C302" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="D302" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E302" s="1" t="s">
         <v>876</v>
-      </c>
-      <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="C303" s="1" t="s">
-        <v>876</v>
-      </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
@@ -8843,7 +8843,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>880</v>
@@ -8852,7 +8852,7 @@
         <v>881</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8861,7 +8861,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>883</v>
@@ -8870,7 +8870,7 @@
         <v>884</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8879,7 +8879,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>886</v>
@@ -8888,7 +8888,7 @@
         <v>887</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8897,7 +8897,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8906,7 +8906,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8915,7 +8915,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>892</v>
@@ -8924,7 +8924,7 @@
         <v>893</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8933,7 +8933,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>895</v>
@@ -8942,7 +8942,7 @@
         <v>896</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8951,7 +8951,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>898</v>
@@ -8960,7 +8960,7 @@
         <v>899</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8969,25 +8969,25 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>641</v>
+        <v>901</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8996,7 +8996,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -9005,7 +9005,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -9014,7 +9014,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -9023,7 +9023,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -9032,7 +9032,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9041,7 +9041,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9050,7 +9050,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9059,7 +9059,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9068,7 +9068,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9077,7 +9077,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9086,7 +9086,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9095,7 +9095,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9104,7 +9104,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9113,7 +9113,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9122,7 +9122,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9131,7 +9131,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9140,7 +9140,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9149,7 +9149,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9158,7 +9158,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9167,7 +9167,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9176,7 +9176,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9185,7 +9185,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9194,7 +9194,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9203,7 +9203,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9212,7 +9212,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9221,7 +9221,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9230,7 +9230,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9239,7 +9239,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9248,7 +9248,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9257,7 +9257,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9266,7 +9266,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9275,7 +9275,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9284,7 +9284,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9293,7 +9293,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9302,7 +9302,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9311,7 +9311,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9320,7 +9320,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9329,7 +9329,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9338,7 +9338,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9347,7 +9347,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9356,7 +9356,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9365,7 +9365,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9374,7 +9374,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9383,7 +9383,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>971</v>
@@ -9392,7 +9392,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9401,7 +9401,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>974</v>
@@ -9410,7 +9410,7 @@
         <v>975</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9419,7 +9419,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>977</v>
@@ -9428,7 +9428,7 @@
         <v>978</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9437,25 +9437,25 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>904</v>
+        <v>980</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9464,7 +9464,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9473,7 +9473,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9482,7 +9482,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9491,7 +9491,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9500,7 +9500,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9509,7 +9509,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9518,7 +9518,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9527,7 +9527,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9536,7 +9536,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9545,7 +9545,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9554,7 +9554,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9563,7 +9563,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9572,7 +9572,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9581,7 +9581,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9590,7 +9590,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9599,7 +9599,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9608,7 +9608,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9617,7 +9617,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9626,7 +9626,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9635,7 +9635,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9644,7 +9644,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9653,7 +9653,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9662,7 +9662,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9671,7 +9671,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9680,7 +9680,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9689,7 +9689,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9698,7 +9698,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9707,7 +9707,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9716,7 +9716,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9725,7 +9725,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9734,7 +9734,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9743,7 +9743,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9752,7 +9752,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9761,7 +9761,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9770,7 +9770,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9779,7 +9779,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9788,7 +9788,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9797,7 +9797,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9806,7 +9806,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9815,7 +9815,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9824,7 +9824,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9833,7 +9833,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9842,7 +9842,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9851,7 +9851,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9869,7 +9869,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9887,7 +9887,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
@@ -9905,7 +9905,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1059</v>
@@ -9923,13 +9923,13 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>1062</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="D364" s="2" t="str">
         <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
@@ -9941,7 +9941,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1064</v>
@@ -9959,7 +9959,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1067</v>
@@ -9977,7 +9977,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1070</v>
@@ -9995,7 +9995,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1073</v>
@@ -10013,7 +10013,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1076</v>
@@ -10031,7 +10031,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1079</v>
@@ -10049,7 +10049,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1082</v>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>1085</v>
@@ -10085,7 +10085,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>1088</v>

</xml_diff>

<commit_message>
Auto-committed on 2023/06/09 週五 16:56:32.10
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -275,7 +275,7 @@
     <t xml:space="preserve">擔保品-土地修改原因檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年02月22日 17:32:27</t>
+    <t xml:space="preserve">2023年06月09日 12:04:17</t>
   </si>
   <si>
     <t xml:space="preserve">ClMain</t>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">案件申請檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月24日 18:36:20</t>
+    <t xml:space="preserve">2023年06月07日 13:54:36</t>
   </si>
   <si>
     <t xml:space="preserve">FacClose</t>
@@ -410,7 +410,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月08日 10:10:57</t>
+    <t xml:space="preserve">2023年06月08日 12:20:19</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月18日 10:42:39</t>
+    <t xml:space="preserve">2023年06月08日 11:21:37</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -986,7 +986,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月23日 12:05:13</t>
+    <t xml:space="preserve">2023年06月07日 17:52:36</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -1121,7 +1121,7 @@
     <t xml:space="preserve">房貸專員業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月30日 10:59:24</t>
+    <t xml:space="preserve">2023年06月02日 18:24:01</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsOfficer</t>
@@ -3038,7 +3038,7 @@
     <t xml:space="preserve">歷史封存表紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月29日 13:38:56</t>
+    <t xml:space="preserve">2023年06月05日 16:22:12</t>
   </si>
   <si>
     <t xml:space="preserve">TxAttachment</t>
@@ -3155,7 +3155,7 @@
     <t xml:space="preserve">交易流程控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月15日 10:31:08</t>
+    <t xml:space="preserve">2023年06月07日 13:45:05</t>
   </si>
   <si>
     <t xml:space="preserve">TxFtpUser</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/06/16 週五 16:46:22.12
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1093">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -218,10 +218,10 @@
     <t xml:space="preserve">ClEva</t>
   </si>
   <si>
-    <t xml:space="preserve">擔保品鑑價資料檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年05月25日 11:34:07</t>
+    <t xml:space="preserve">擔保品鑑價歷程檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月15日 17:12:50</t>
   </si>
   <si>
     <t xml:space="preserve">ClFac</t>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">擔保品與額度關聯檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月14日 16:11:26</t>
+    <t xml:space="preserve">2023年06月13日 16:07:51</t>
   </si>
   <si>
     <t xml:space="preserve">ClImm</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">火險初保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月11日 12:33:01</t>
+    <t xml:space="preserve">2023年06月16日 15:50:23</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenew</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月09日 11:34:11</t>
+    <t xml:space="preserve">2023年06月15日 16:38:24</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月26日 13:55:32</t>
+    <t xml:space="preserve">2023年06月12日 13:46:02</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月15日 11:15:54</t>
+    <t xml:space="preserve">2023年06月13日 17:15:24</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -1764,7 +1764,7 @@
 (使用報表：LM049、LQ005)</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月31日 15:39:38</t>
+    <t xml:space="preserve">2023年06月15日 16:46:43</t>
   </si>
   <si>
     <t xml:space="preserve">Ias39IntMethod</t>
@@ -1828,7 +1828,7 @@
 (使用報表：LM013) </t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月31日 15:39:56</t>
+    <t xml:space="preserve">2023年06月15日 16:46:26</t>
   </si>
   <si>
     <t xml:space="preserve">LifeRelHead</t>
@@ -1838,7 +1838,7 @@
 (使用報表：LM013、LM042、LM050)</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月31日 15:40:00</t>
+    <t xml:space="preserve">2023年06月15日 16:46:55</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIfrs9Ap</t>
@@ -2750,6 +2750,15 @@
     <t xml:space="preserve">2023年02月23日 14:26:45</t>
   </si>
   <si>
+    <t xml:space="preserve">Lagdtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS400不動產押品主檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月14日 11:12:23</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lahgtp</t>
   </si>
   <si>
@@ -2930,6 +2939,351 @@
     <t xml:space="preserve">2023年01月10日 17:41:58</t>
   </si>
   <si>
+    <t xml:space="preserve">YearlyHouseLoanInt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">每年房屋擔保借款繳息工作檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年03月21日 10:42:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YearlyHouseLoanIntCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">每年房屋擔保借款繳息檢核檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年03月30日 10:33:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX-系統</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAgent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代理人檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年12月09日 17:39:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlCredit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AML定審資料</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月28日 14:17:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AML檢查紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年06月07日 14:39:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlNotice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AML定審通知紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年12月16日 11:57:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlRating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eloan評級檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年02月06日 11:44:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAmlRatingAppl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eloan評級案件申請留存檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年02月03日 09:11:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxApLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ApLog敏感資料查詢紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年03月03日 17:33:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxArchiveTable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歷史封存表設定檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年12月26日 11:00:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxArchiveTableLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歷史封存表紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月05日 16:22:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAttachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">附件檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年01月07日 11:11:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAttachType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">附件類別檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年12月14日 18:37:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAuthGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">權限群組檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年05月25日 11:02:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAuthority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">群組權限檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月20日 09:41:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxAuthorize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主管授權紀錄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年10月18日 13:57:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxBizDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">營業日檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020年07月02日 18:20:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">作業流程控制檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月19日 12:32:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxCruiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">批次發動交易紀錄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年03月16日 15:23:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxCurr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">幣別檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020年06月24日 12:13:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxDataLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料變更紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年09月07日 18:30:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxErrCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">錯誤代碼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月20日 09:49:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">輸出檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年03月16日 16:10:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxFlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交易流程控制檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月12日 16:52:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxFtpUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTP權限檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月25日 18:51:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxHoliday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">假日檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年07月15日 10:15:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxInquiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">查詢紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年05月11日 18:38:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxLock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鎖定控制檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年12月14日 10:45:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">印表機設定檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年04月20日 09:49:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交易記錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年09月27日 14:21:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxTeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">使用者檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年02月15日 12:29:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxTellerAuth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">使用者權限檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年11月19日 18:33:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxTemp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交易暫存</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月12日 16:52:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxToDoDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">應處理明細檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月15日 11:08:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxToDoDetailReserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">應處理明細留存檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022年05月27日 08:59:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxToDoMain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">應處理清單主檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年11月18日 15:31:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxTranCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交易控制檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年04月17日 13:46:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxUnLock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人工解除鎖定紀錄檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021年12月14日 10:45:10</t>
+  </si>
+  <si>
     <t xml:space="preserve">UspErrorLog</t>
   </si>
   <si>
@@ -2937,357 +3291,6 @@
   </si>
   <si>
     <t xml:space="preserve">2022年01月20日 12:47:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YearlyHouseLoanInt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">每年房屋擔保借款繳息工作檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年03月21日 10:42:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YearlyHouseLoanIntCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">每年房屋擔保借款繳息檢核檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年03月30日 10:33:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XX-系統</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAgent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">代理人檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月09日 17:39:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAmlCredit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AML定審資料</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年04月28日 14:17:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAmlLog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AML檢查紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年06月07日 14:39:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAmlNotice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AML定審通知紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月16日 11:57:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAmlRating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eloan評級檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年02月06日 11:44:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAmlRatingAppl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eloan評級案件申請留存檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年02月03日 09:11:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxApLog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ApLog敏感資料查詢紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年03月03日 17:33:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxArchiveTable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">歷史封存表設定檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年12月26日 11:00:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxArchiveTableLog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">歷史封存表紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年06月05日 16:22:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAttachment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">附件檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年01月07日 11:11:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAttachType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">附件類別檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月14日 18:37:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAuthGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">權限群組檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年05月25日 11:02:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAuthority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">群組權限檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年04月20日 09:41:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxAuthorize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">主管授權紀錄</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年10月18日 13:57:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxBizDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">營業日檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020年07月02日 18:20:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxControl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">作業流程控制檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年05月19日 12:32:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxCruiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">批次發動交易紀錄</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年03月16日 15:23:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxCurr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">幣別檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020年06月24日 12:13:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxDataLog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料變更紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年09月07日 18:30:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxErrCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">錯誤代碼</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年04月20日 09:49:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxFile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">輸出檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年03月16日 16:10:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxFlow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">交易流程控制檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年06月07日 13:45:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxFtpUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTP權限檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年05月25日 18:51:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxHoliday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">假日檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年07月15日 10:15:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxInquiry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">查詢紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年05月11日 18:38:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxLock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">鎖定控制檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月14日 10:45:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxPrinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">印表機設定檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年04月20日 09:49:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxProcess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020年04月09日 17:18:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxRecord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">交易記錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年09月27日 14:21:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxTeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">使用者檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年02月15日 12:29:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxTellerAuth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">使用者權限檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年11月19日 18:33:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxTemp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">交易暫存</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年02月25日 14:27:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxToDoDetail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">應處理明細檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年09月08日 13:16:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxToDoDetailReserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">應處理明細留存檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年05月27日 08:59:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxToDoMain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">應處理清單主檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年11月18日 15:31:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxTranCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">交易控制檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年04月17日 13:46:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TxUnLock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">人工解除鎖定紀錄檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021年12月14日 10:45:10</t>
   </si>
   <si>
     <t xml:space="preserve">此檔案為自動確認GenTable目錄及檔案產生，不應手動修改。
@@ -3402,7 +3405,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="2">
@@ -9032,7 +9035,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lagdtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9050,7 +9053,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9068,7 +9071,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9086,7 +9089,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9104,7 +9107,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9122,7 +9125,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9140,7 +9143,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9158,7 +9161,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9176,7 +9179,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9194,7 +9197,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9212,7 +9215,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9230,7 +9233,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9248,7 +9251,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9266,7 +9269,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9284,7 +9287,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9302,7 +9305,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9320,7 +9323,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9338,7 +9341,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9356,7 +9359,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9374,7 +9377,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9392,7 +9395,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9929,14 +9932,14 @@
         <v>1062</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>1045</v>
+        <v>1063</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxProcess.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="365">
@@ -9944,17 +9947,17 @@
         <v>980</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="366">
@@ -9962,17 +9965,17 @@
         <v>980</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="367">
@@ -9980,17 +9983,17 @@
         <v>980</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="368">
@@ -9998,17 +10001,17 @@
         <v>980</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="369">
@@ -10016,17 +10019,17 @@
         <v>980</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="370">
@@ -10034,17 +10037,17 @@
         <v>980</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="371">
@@ -10052,17 +10055,17 @@
         <v>980</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C371" s="1" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="372">
@@ -10070,17 +10073,17 @@
         <v>980</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="D372" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E372" s="1" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="373">
@@ -10088,17 +10091,17 @@
         <v>980</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="D373" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E373" s="1" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/06/30 週五 17:05:28.55
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月21日 10:39:48</t>
+    <t xml:space="preserve">2023年06月29日 10:01:48</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -401,7 +401,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年06月02日 09:59:18</t>
+    <t xml:space="preserve">2023年06月30日 14:00:53</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月02日 12:41:46</t>
+    <t xml:space="preserve">2023年06月17日 16:23:11</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月19日 12:19:18</t>
+    <t xml:space="preserve">2023年06月21日 14:22:04</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -650,7 +650,7 @@
     <t xml:space="preserve">ACH授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月09日 18:21:36</t>
+    <t xml:space="preserve">2023年06月21日 14:22:58</t>
   </si>
   <si>
     <t xml:space="preserve">AchDeductMedia</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">銀行扣款明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月26日 00:24:13</t>
+    <t xml:space="preserve">2023年06月27日 12:10:25</t>
   </si>
   <si>
     <t xml:space="preserve">BankRemit</t>
@@ -791,10 +791,10 @@
     <t xml:space="preserve">InsuOrignal</t>
   </si>
   <si>
-    <t xml:space="preserve">火險初保檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年06月16日 15:50:23</t>
+    <t xml:space="preserve">擔保品火險檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年06月21日 16:58:24</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenew</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月19日 12:19:14</t>
+    <t xml:space="preserve">2023年06月21日 14:24:52</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -830,7 +830,7 @@
     <t xml:space="preserve">郵局授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月09日 18:20:39</t>
+    <t xml:space="preserve">2023年06月21日 14:24:50</t>
   </si>
   <si>
     <t xml:space="preserve">PostDeductMedia</t>
@@ -986,7 +986,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月07日 17:52:36</t>
+    <t xml:space="preserve">2023年06月25日 21:27:08</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -1067,7 +1067,7 @@
     <t xml:space="preserve">債務協商債權機構帳戶檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月28日 12:32:08</t>
+    <t xml:space="preserve">2023年06月26日 16:10:19</t>
   </si>
   <si>
     <t xml:space="preserve">NegFinShare</t>
@@ -1310,7 +1310,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月06日 18:59:26</t>
+    <t xml:space="preserve">2023年06月21日 16:26:55</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1364,7 +1364,7 @@
     <t xml:space="preserve">行庫資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月30日 09:45:11</t>
+    <t xml:space="preserve">2023年06月20日 17:34:59</t>
   </si>
   <si>
     <t xml:space="preserve">CdBaseRate</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月13日 17:15:24</t>
+    <t xml:space="preserve">2023年06月19日 15:52:55</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -1764,7 +1764,7 @@
 (使用報表：LM049、LQ005)</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月15日 16:46:43</t>
+    <t xml:space="preserve">2023年06月16日 18:09:29</t>
   </si>
   <si>
     <t xml:space="preserve">Ias39IntMethod</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/07 週五 17:16:59.50
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -320,7 +320,7 @@
     <t xml:space="preserve">擔保品他項權利檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月28日 14:26:26</t>
+    <t xml:space="preserve">2023年07月04日 10:52:36</t>
   </si>
   <si>
     <t xml:space="preserve">ClOtherRightsFac</t>
@@ -401,7 +401,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月30日 14:00:53</t>
+    <t xml:space="preserve">2023年07月04日 09:09:12</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月08日 11:21:37</t>
+    <t xml:space="preserve">2023年07月06日 09:52:01</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月21日 14:22:04</t>
+    <t xml:space="preserve">2023年07月04日 11:40:10</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -668,7 +668,7 @@
     <t xml:space="preserve">銀扣授權帳號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月19日 09:44:33</t>
+    <t xml:space="preserve">2023年07月06日 10:50:53</t>
   </si>
   <si>
     <t xml:space="preserve">BankDeductDtl</t>
@@ -803,7 +803,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月19日 13:24:23</t>
+    <t xml:space="preserve">2023年07月06日 14:21:29</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1112,7 +1112,7 @@
     <t xml:space="preserve">債務協商交易檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年02月14日 18:41:08</t>
+    <t xml:space="preserve">2023年07月05日 20:31:19</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsDetail</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月30日 14:28:22</t>
+    <t xml:space="preserve">2023年07月07日 13:09:36</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1328,7 +1328,7 @@
     <t xml:space="preserve">會計科子細目設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年03月14日 17:11:12</t>
+    <t xml:space="preserve">2023年07月06日 14:17:01</t>
   </si>
   <si>
     <t xml:space="preserve">CdAppraisalCompany</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月19日 15:52:55</t>
+    <t xml:space="preserve">2023年07月06日 10:06:14</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -3236,7 +3236,7 @@
     <t xml:space="preserve">交易暫存</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月12日 16:52:10</t>
+    <t xml:space="preserve">2023年07月04日 15:21:57</t>
   </si>
   <si>
     <t xml:space="preserve">TxToDoDetail</t>
@@ -3245,7 +3245,7 @@
     <t xml:space="preserve">應處理明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月15日 11:08:44</t>
+    <t xml:space="preserve">2023年07月07日 10:26:14</t>
   </si>
   <si>
     <t xml:space="preserve">TxToDoDetailReserve</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/14 週五 17:23:32.93
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -803,7 +803,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月06日 14:21:29</t>
+    <t xml:space="preserve">2023年07月13日 11:23:02</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月18日 18:59:38</t>
+    <t xml:space="preserve">2023年07月07日 18:02:38</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1256,7 +1256,7 @@
     <t xml:space="preserve">會計業務關帳控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月16日 10:12:52</t>
+    <t xml:space="preserve">2023年07月11日 18:01:32</t>
   </si>
   <si>
     <t xml:space="preserve">AcDetail</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月15日 16:38:24</t>
+    <t xml:space="preserve">2023年07月14日 17:18:47</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1733,7 +1733,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月06日 10:06:14</t>
+    <t xml:space="preserve">2023年07月10日 16:04:48</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2933,10 +2933,10 @@
     <t xml:space="preserve">SlipMedia2022</t>
   </si>
   <si>
-    <t xml:space="preserve">傳票媒體檔2022年格式</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023年01月10日 17:41:58</t>
+    <t xml:space="preserve">總帳傳票媒體檔2022年格式</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年07月14日 14:59:37</t>
   </si>
   <si>
     <t xml:space="preserve">YearlyHouseLoanInt</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/21 週五 17:18:54.18
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月17日 16:23:11</t>
+    <t xml:space="preserve">2023年07月19日 10:19:14</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -986,7 +986,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月25日 21:27:08</t>
+    <t xml:space="preserve">2023年07月19日 14:21:06</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月07日 18:02:38</t>
+    <t xml:space="preserve">2023年07月20日 10:26:50</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月14日 17:18:47</t>
+    <t xml:space="preserve">2023年07月20日 13:03:01</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1490,7 +1490,7 @@
     <t xml:space="preserve">共用代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月15日 16:28:26</t>
+    <t xml:space="preserve">2023年07月20日 09:22:48</t>
   </si>
   <si>
     <t xml:space="preserve">CdComm</t>
@@ -1697,7 +1697,7 @@
     <t xml:space="preserve">批次工作明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:44:50</t>
+    <t xml:space="preserve">2023年07月19日 18:11:04</t>
   </si>
   <si>
     <t xml:space="preserve">JobMain</t>
@@ -2936,7 +2936,7 @@
     <t xml:space="preserve">總帳傳票媒體檔2022年格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月14日 14:59:37</t>
+    <t xml:space="preserve">2023年07月20日 09:24:14</t>
   </si>
   <si>
     <t xml:space="preserve">YearlyHouseLoanInt</t>
@@ -3155,7 +3155,7 @@
     <t xml:space="preserve">交易流程控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月12日 16:52:56</t>
+    <t xml:space="preserve">2023年07月14日 18:47:21</t>
   </si>
   <si>
     <t xml:space="preserve">TxFtpUser</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/28 週五 17:03:56.30
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月29日 10:01:48</t>
+    <t xml:space="preserve">2023年07月25日 16:06:03</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -1013,7 +1013,7 @@
     <t xml:space="preserve">覆審案件明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:22:18</t>
+    <t xml:space="preserve">2023年07月25日 10:02:32</t>
   </si>
   <si>
     <t xml:space="preserve">JcicAtomDetail</t>
@@ -1166,7 +1166,7 @@
     <t xml:space="preserve">業績計算明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月31日 18:31:13</t>
+    <t xml:space="preserve">2023年07月24日 11:46:08</t>
   </si>
   <si>
     <t xml:space="preserve">PfInsCheck</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月07日 13:09:36</t>
+    <t xml:space="preserve">2023年07月24日 13:15:06</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1445,7 +1445,7 @@
     <t xml:space="preserve">現金流量預估資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年11月29日 14:21:19</t>
+    <t xml:space="preserve">2023年07月25日 16:06:00</t>
   </si>
   <si>
     <t xml:space="preserve">CdCity</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月12日 13:46:02</t>
+    <t xml:space="preserve">2023年07月28日 16:47:06</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1697,7 +1697,7 @@
     <t xml:space="preserve">批次工作明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月19日 18:11:04</t>
+    <t xml:space="preserve">2023年07月26日 22:35:15</t>
   </si>
   <si>
     <t xml:space="preserve">JobMain</t>
@@ -1706,7 +1706,7 @@
     <t xml:space="preserve">批次工作主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月31日 17:42:04</t>
+    <t xml:space="preserve">2023年07月24日 16:41:34</t>
   </si>
   <si>
     <t xml:space="preserve">QuitEmp</t>
@@ -3290,7 +3290,7 @@
     <t xml:space="preserve">預存程序錯誤記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:47:10</t>
+    <t xml:space="preserve">2023年07月25日 13:46:59</t>
   </si>
   <si>
     <t xml:space="preserve">此檔案為自動確認GenTable目錄及檔案產生，不應手動修改。

</xml_diff>

<commit_message>
Auto-committed on 2023/08/04 週五 16:06:39.95
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -401,7 +401,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月04日 09:09:12</t>
+    <t xml:space="preserve">2023年08月02日 11:17:36</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -491,7 +491,7 @@
     <t xml:space="preserve">法拍費用檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:38:18</t>
+    <t xml:space="preserve">2023年08月04日 10:03:23</t>
   </si>
   <si>
     <t xml:space="preserve">ForeclosureFinished</t>
@@ -602,7 +602,7 @@
     <t xml:space="preserve">未齊件管理檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月26日 09:37:17</t>
+    <t xml:space="preserve">2023年07月31日 11:03:49</t>
   </si>
   <si>
     <t xml:space="preserve">LoanOverdue</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月03日 11:27:17</t>
+    <t xml:space="preserve">2023年07月31日 17:33:34</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -1148,7 +1148,7 @@
     <t xml:space="preserve">協辦人員等級歷程檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月19日 16:04:06</t>
+    <t xml:space="preserve">2023年07月31日 20:07:36</t>
   </si>
   <si>
     <t xml:space="preserve">PfDeparment</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月24日 13:15:06</t>
+    <t xml:space="preserve">2023年08月02日 16:37:38</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月20日 13:03:01</t>
+    <t xml:space="preserve">2023年07月31日 17:17:31</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1382,7 +1382,7 @@
     <t xml:space="preserve">分公司資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月22日 11:22:59</t>
+    <t xml:space="preserve">2023年08月02日 16:18:18</t>
   </si>
   <si>
     <t xml:space="preserve">CdBonus</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月28日 16:47:06</t>
+    <t xml:space="preserve">2023年07月31日 16:53:28</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/08/11 週五 17:06:55.56
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -401,7 +401,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月02日 11:17:36</t>
+    <t xml:space="preserve">2023年08月10日 15:17:59</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月19日 10:19:14</t>
+    <t xml:space="preserve">2023年08月10日 16:55:28</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -1013,7 +1013,7 @@
     <t xml:space="preserve">覆審案件明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月25日 10:02:32</t>
+    <t xml:space="preserve">2023年08月08日 16:47:13</t>
   </si>
   <si>
     <t xml:space="preserve">JcicAtomDetail</t>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月20日 10:26:50</t>
+    <t xml:space="preserve">2023年08月07日 01:12:26</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1121,7 +1121,7 @@
     <t xml:space="preserve">房貸專員業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月02日 18:24:01</t>
+    <t xml:space="preserve">2023年08月11日 16:11:12</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsOfficer</t>
@@ -1139,7 +1139,7 @@
     <t xml:space="preserve">協辦人員等級檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月19日 14:58:04</t>
+    <t xml:space="preserve">2023年08月07日 13:41:09</t>
   </si>
   <si>
     <t xml:space="preserve">PfCoOfficerLog</t>
@@ -1148,7 +1148,7 @@
     <t xml:space="preserve">協辦人員等級歷程檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月31日 20:07:36</t>
+    <t xml:space="preserve">2023年08月10日 15:48:25</t>
   </si>
   <si>
     <t xml:space="preserve">PfDeparment</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月02日 16:37:38</t>
+    <t xml:space="preserve">2023年08月07日 09:37:13</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月31日 17:17:31</t>
+    <t xml:space="preserve">2023年08月07日 11:39:01</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1310,7 +1310,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月21日 16:26:55</t>
+    <t xml:space="preserve">2023年08月07日 11:36:40</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>
@@ -1697,7 +1697,7 @@
     <t xml:space="preserve">批次工作明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月26日 22:35:15</t>
+    <t xml:space="preserve">2023年08月08日 10:30:51</t>
   </si>
   <si>
     <t xml:space="preserve">JobMain</t>
@@ -1706,7 +1706,7 @@
     <t xml:space="preserve">批次工作主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月24日 16:41:34</t>
+    <t xml:space="preserve">2023年08月08日 12:04:08</t>
   </si>
   <si>
     <t xml:space="preserve">QuitEmp</t>
@@ -2927,7 +2927,7 @@
     <t xml:space="preserve">傳票媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:46:45</t>
+    <t xml:space="preserve">2023年08月11日 15:31:02</t>
   </si>
   <si>
     <t xml:space="preserve">SlipMedia2022</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/08/18 週五 16:34:58.24
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1096">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -1626,6 +1626,15 @@
   </si>
   <si>
     <t xml:space="preserve">2023年03月16日 15:20:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CdRuleCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">管制代碼檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年08月17日 09:13:56</t>
   </si>
   <si>
     <t xml:space="preserve">CdStock</t>
@@ -3405,7 +3414,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="2">
@@ -6587,7 +6596,7 @@
         <v>539</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdRuleCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E178" s="1" t="s">
@@ -6605,7 +6614,7 @@
         <v>542</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdStock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E179" s="1" t="s">
@@ -6623,7 +6632,7 @@
         <v>545</v>
       </c>
       <c r="D180" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSupv.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E180" s="1" t="s">
@@ -6641,7 +6650,7 @@
         <v>548</v>
       </c>
       <c r="D181" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdSyndFee.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E181" s="1" t="s">
@@ -6659,7 +6668,7 @@
         <v>551</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdTeamReward.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E182" s="1" t="s">
@@ -6677,7 +6686,7 @@
         <v>554</v>
       </c>
       <c r="D183" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdVarValue.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E183" s="1" t="s">
@@ -6695,7 +6704,7 @@
         <v>557</v>
       </c>
       <c r="D184" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CdWorkMonth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E184" s="1" t="s">
@@ -6713,7 +6722,7 @@
         <v>560</v>
       </c>
       <c r="D185" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\CoreAcMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E185" s="1" t="s">
@@ -6731,7 +6740,7 @@
         <v>563</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E186" s="1" t="s">
@@ -6749,7 +6758,7 @@
         <v>566</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\JobMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E187" s="1" t="s">
@@ -6767,7 +6776,7 @@
         <v>569</v>
       </c>
       <c r="D188" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\QuitEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E188" s="1" t="s">
@@ -6785,7 +6794,7 @@
         <v>572</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\StgCdEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -6794,25 +6803,25 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="C190" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L6-共同作業\SystemParas.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E190" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="D190" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>578</v>
@@ -6821,7 +6830,7 @@
         <v>579</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CreditRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -6830,7 +6839,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>581</v>
@@ -6839,7 +6848,7 @@
         <v>582</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\CustomerAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -6848,7 +6857,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>584</v>
@@ -6857,7 +6866,7 @@
         <v>585</v>
       </c>
       <c r="D193" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\FinHoldRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -6866,7 +6875,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>587</v>
@@ -6875,7 +6884,7 @@
         <v>588</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39IntMethod.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -6884,7 +6893,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>590</v>
@@ -6893,7 +6902,7 @@
         <v>591</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LGD.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -6902,7 +6911,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>593</v>
@@ -6911,7 +6920,7 @@
         <v>594</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39LoanCommit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -6920,7 +6929,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>596</v>
@@ -6929,7 +6938,7 @@
         <v>597</v>
       </c>
       <c r="D197" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ias39Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -6938,7 +6947,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>599</v>
@@ -6947,7 +6956,7 @@
         <v>600</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9FacData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -6956,7 +6965,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>602</v>
@@ -6965,7 +6974,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\Ifrs9LoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6974,7 +6983,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>605</v>
@@ -6983,7 +6992,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6992,7 +7001,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>608</v>
@@ -7001,7 +7010,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -7010,7 +7019,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>611</v>
@@ -7019,7 +7028,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -7028,7 +7037,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>614</v>
@@ -7037,7 +7046,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7046,7 +7055,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>617</v>
@@ -7055,7 +7064,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7064,7 +7073,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>620</v>
@@ -7073,7 +7082,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7082,7 +7091,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>623</v>
@@ -7091,7 +7100,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7100,7 +7109,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>626</v>
@@ -7109,7 +7118,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7118,7 +7127,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>629</v>
@@ -7127,7 +7136,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7136,7 +7145,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>632</v>
@@ -7145,7 +7154,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7154,7 +7163,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>635</v>
@@ -7163,7 +7172,7 @@
         <v>636</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7172,25 +7181,25 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="C211" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>642</v>
@@ -7199,7 +7208,7 @@
         <v>643</v>
       </c>
       <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E212" s="1" t="s">
@@ -7208,7 +7217,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>645</v>
@@ -7217,7 +7226,7 @@
         <v>646</v>
       </c>
       <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E213" s="1" t="s">
@@ -7226,7 +7235,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7235,7 +7244,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7244,7 +7253,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7253,7 +7262,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7262,7 +7271,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7271,7 +7280,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7280,7 +7289,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7289,7 +7298,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7298,7 +7307,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7307,7 +7316,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7316,7 +7325,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7325,7 +7334,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7334,7 +7343,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7343,7 +7352,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7352,7 +7361,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7361,7 +7370,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7370,7 +7379,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7379,7 +7388,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7388,7 +7397,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7397,7 +7406,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7406,7 +7415,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7415,7 +7424,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7424,7 +7433,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7433,7 +7442,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7442,7 +7451,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7451,7 +7460,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7460,7 +7469,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7469,7 +7478,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7478,7 +7487,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7487,7 +7496,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7496,7 +7505,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
@@ -7505,7 +7514,7 @@
         <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7514,34 +7523,34 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>696</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
@@ -7550,34 +7559,34 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>701</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
@@ -7586,34 +7595,34 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>706</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
@@ -7622,34 +7631,34 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>711</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
@@ -7658,34 +7667,34 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>716</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
@@ -7694,34 +7703,34 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>721</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
@@ -7730,34 +7739,34 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>726</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
@@ -7766,34 +7775,34 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>731</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
@@ -7802,34 +7811,34 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>736</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
@@ -7838,34 +7847,34 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>741</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
@@ -7874,34 +7883,34 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>746</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
@@ -7910,34 +7919,34 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>751</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
@@ -7946,34 +7955,34 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>756</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
@@ -7982,34 +7991,34 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>761</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
@@ -8018,34 +8027,34 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>766</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
@@ -8054,34 +8063,34 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>771</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
@@ -8090,70 +8099,70 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>776</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>744</v>
+        <v>777</v>
       </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>783</v>
+        <v>747</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
@@ -8162,34 +8171,34 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>785</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -8198,34 +8207,34 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>790</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
@@ -8234,34 +8243,34 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>795</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
@@ -8270,34 +8279,34 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>800</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
@@ -8306,34 +8315,34 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>805</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
@@ -8342,34 +8351,34 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>810</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
@@ -8378,34 +8387,34 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>815</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
@@ -8414,34 +8423,34 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>820</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
@@ -8450,34 +8459,34 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>825</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
@@ -8486,34 +8495,34 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>830</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
@@ -8522,34 +8531,34 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>835</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -8558,34 +8567,34 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>840</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
@@ -8594,34 +8603,34 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>845</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
@@ -8630,34 +8639,34 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>850</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
@@ -8666,34 +8675,34 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>855</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
@@ -8702,34 +8711,34 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>860</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
@@ -8738,34 +8747,34 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>865</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
@@ -8774,34 +8783,34 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>870</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
@@ -8810,34 +8819,34 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>875</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
@@ -8846,7 +8855,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>880</v>
@@ -8855,7 +8864,7 @@
         <v>881</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
@@ -8864,7 +8873,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>883</v>
@@ -8873,7 +8882,7 @@
         <v>884</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8882,7 +8891,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>886</v>
@@ -8891,7 +8900,7 @@
         <v>887</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8900,7 +8909,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8909,7 +8918,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8918,7 +8927,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>892</v>
@@ -8927,7 +8936,7 @@
         <v>893</v>
       </c>
       <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MonthlyQ53.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E308" s="1" t="s">
@@ -8936,7 +8945,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>895</v>
@@ -8945,7 +8954,7 @@
         <v>896</v>
       </c>
       <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -8954,7 +8963,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>898</v>
@@ -8963,7 +8972,7 @@
         <v>899</v>
       </c>
       <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicW020.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8972,25 +8981,25 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B311" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="B311" s="1" t="s">
+      <c r="C311" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="C311" s="1" t="s">
+      <c r="D311" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicZZ50.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E311" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E311" s="1" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8999,7 +9008,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -9008,7 +9017,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -9017,7 +9026,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -9026,7 +9035,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -9035,7 +9044,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lagdtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DataTransferMapping.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9044,7 +9053,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9053,7 +9062,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lagdtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9062,7 +9071,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9071,7 +9080,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9080,7 +9089,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9089,7 +9098,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9098,7 +9107,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9107,7 +9116,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9116,7 +9125,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9125,7 +9134,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9134,7 +9143,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9143,7 +9152,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9152,7 +9161,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9161,7 +9170,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9170,7 +9179,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9179,7 +9188,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9188,7 +9197,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9197,7 +9206,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9206,7 +9215,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9215,7 +9224,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9224,7 +9233,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9233,7 +9242,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9242,7 +9251,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9251,7 +9260,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9260,7 +9269,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9269,7 +9278,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9278,7 +9287,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9287,7 +9296,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9296,7 +9305,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9305,7 +9314,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9314,7 +9323,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9323,7 +9332,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9332,7 +9341,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9341,7 +9350,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9350,7 +9359,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9359,7 +9368,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9368,7 +9377,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9377,7 +9386,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9386,7 +9395,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>971</v>
@@ -9395,7 +9404,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9404,7 +9413,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>974</v>
@@ -9413,7 +9422,7 @@
         <v>975</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9422,7 +9431,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>977</v>
@@ -9431,7 +9440,7 @@
         <v>978</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9440,25 +9449,25 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B337" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="B337" s="1" t="s">
+      <c r="C337" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C337" s="1" t="s">
+      <c r="D337" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E337" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9467,7 +9476,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9476,7 +9485,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9485,7 +9494,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9494,7 +9503,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9503,7 +9512,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9512,7 +9521,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9521,7 +9530,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9530,7 +9539,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9539,7 +9548,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9548,7 +9557,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9557,7 +9566,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9566,7 +9575,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9575,7 +9584,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9584,7 +9593,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9593,7 +9602,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9602,7 +9611,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9611,7 +9620,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9620,7 +9629,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9629,7 +9638,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9638,7 +9647,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9647,7 +9656,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9656,7 +9665,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9665,7 +9674,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9674,7 +9683,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9683,7 +9692,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9692,7 +9701,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9701,7 +9710,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9710,7 +9719,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9719,7 +9728,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9728,7 +9737,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9737,7 +9746,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9746,7 +9755,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9755,7 +9764,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9764,7 +9773,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9773,7 +9782,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9782,7 +9791,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9791,7 +9800,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9800,7 +9809,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9809,7 +9818,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9818,7 +9827,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9827,7 +9836,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9836,7 +9845,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9845,7 +9854,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9854,7 +9863,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9863,7 +9872,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9872,7 +9881,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9881,7 +9890,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9890,7 +9899,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
@@ -9899,7 +9908,7 @@
         <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9908,7 +9917,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1059</v>
@@ -9917,7 +9926,7 @@
         <v>1060</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9926,7 +9935,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>1062</v>
@@ -9935,7 +9944,7 @@
         <v>1063</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9944,7 +9953,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1065</v>
@@ -9953,7 +9962,7 @@
         <v>1066</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9962,7 +9971,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1068</v>
@@ -9971,7 +9980,7 @@
         <v>1069</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9980,7 +9989,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1071</v>
@@ -9989,7 +9998,7 @@
         <v>1072</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9998,7 +10007,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1074</v>
@@ -10007,7 +10016,7 @@
         <v>1075</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -10016,7 +10025,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1077</v>
@@ -10025,7 +10034,7 @@
         <v>1078</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10034,7 +10043,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1080</v>
@@ -10043,7 +10052,7 @@
         <v>1081</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10052,7 +10061,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1083</v>
@@ -10061,7 +10070,7 @@
         <v>1084</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
@@ -10070,7 +10079,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>1086</v>
@@ -10079,7 +10088,7 @@
         <v>1087</v>
       </c>
       <c r="D372" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E372" s="1" t="s">
@@ -10088,7 +10097,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>1089</v>
@@ -10097,11 +10106,29 @@
         <v>1090</v>
       </c>
       <c r="D373" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E373" s="1" t="s">
         <v>1091</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D374" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>1094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/01 週五 16:57:10.12
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="1102">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -410,7 +410,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月21日 10:38:06</t>
+    <t xml:space="preserve">2023年08月30日 14:06:06</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月06日 09:52:01</t>
+    <t xml:space="preserve">2023年08月30日 17:17:55</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -758,7 +758,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月26日 11:27:13</t>
+    <t xml:space="preserve">2023年09月01日 09:44:29</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -776,7 +776,7 @@
     <t xml:space="preserve">員工扣薪日程表</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年03月30日 11:25:22</t>
+    <t xml:space="preserve">2023年08月28日 13:10:56</t>
   </si>
   <si>
     <t xml:space="preserve">InsuComm</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">最大債權撥付資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年12月12日 00:27:10</t>
+    <t xml:space="preserve">2023年09月01日 10:23:16</t>
   </si>
   <si>
     <t xml:space="preserve">NegAppr02</t>
@@ -1697,7 +1697,7 @@
     <t xml:space="preserve">核心會計總帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月24日 09:51:29</t>
+    <t xml:space="preserve">2023年08月31日 16:08:15</t>
   </si>
   <si>
     <t xml:space="preserve">JobDetail</t>
@@ -2777,6 +2777,15 @@
     <t xml:space="preserve">2023年05月25日 15:37:55</t>
   </si>
   <si>
+    <t xml:space="preserve">LaLgtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS400土地明細資料檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年08月31日 11:24:31</t>
+  </si>
+  <si>
     <t xml:space="preserve">MonthlyDpUnpaidExpense</t>
   </si>
   <si>
@@ -2829,6 +2838,15 @@
   </si>
   <si>
     <t xml:space="preserve">2021年09月28日 15:07:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MonthlyLM042RBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM042RBC會計報表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年08月28日 18:23:45</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM052AssetClass</t>
@@ -3414,7 +3432,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1095</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="2">
@@ -9098,7 +9116,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\LaLgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9116,7 +9134,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9134,7 +9152,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9152,7 +9170,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9170,7 +9188,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9188,7 +9206,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9206,7 +9224,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9224,7 +9242,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM042RBC.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9242,7 +9260,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9260,7 +9278,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9278,7 +9296,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9296,7 +9314,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9314,7 +9332,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9332,7 +9350,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9350,7 +9368,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9368,7 +9386,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9386,7 +9404,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9404,7 +9422,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptSubCom.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9422,7 +9440,7 @@
         <v>975</v>
       </c>
       <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E335" s="1" t="s">
@@ -9440,7 +9458,7 @@
         <v>978</v>
       </c>
       <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E336" s="1" t="s">
@@ -9458,7 +9476,7 @@
         <v>981</v>
       </c>
       <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E337" s="1" t="s">
@@ -9467,43 +9485,43 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B338" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="C338" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="C338" s="1" t="s">
+      <c r="D338" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E338" s="1" t="s">
         <v>985</v>
-      </c>
-      <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E338" s="1" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>983</v>
+        <v>904</v>
       </c>
       <c r="B339" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C339" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="C339" s="1" t="s">
+      <c r="D339" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E339" s="1" t="s">
         <v>988</v>
-      </c>
-      <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E339" s="1" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9512,7 +9530,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9521,7 +9539,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9530,7 +9548,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9539,7 +9557,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9548,7 +9566,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9557,7 +9575,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9566,7 +9584,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9575,7 +9593,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9584,7 +9602,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9593,7 +9611,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9602,7 +9620,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9611,7 +9629,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9620,7 +9638,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9629,7 +9647,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9638,7 +9656,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9647,7 +9665,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9656,7 +9674,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9665,7 +9683,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9674,7 +9692,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9683,7 +9701,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9692,7 +9710,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9701,7 +9719,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9710,7 +9728,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9719,7 +9737,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9728,7 +9746,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9737,7 +9755,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9746,7 +9764,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9755,7 +9773,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9764,7 +9782,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9773,7 +9791,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9782,7 +9800,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9791,7 +9809,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9800,7 +9818,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9809,7 +9827,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9818,7 +9836,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9827,7 +9845,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9836,7 +9854,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9845,7 +9863,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9854,7 +9872,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9863,7 +9881,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9872,7 +9890,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9881,7 +9899,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9890,7 +9908,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9899,7 +9917,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
@@ -9908,7 +9926,7 @@
         <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9917,7 +9935,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1059</v>
@@ -9926,7 +9944,7 @@
         <v>1060</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9935,7 +9953,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>1062</v>
@@ -9944,7 +9962,7 @@
         <v>1063</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9953,7 +9971,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1065</v>
@@ -9962,7 +9980,7 @@
         <v>1066</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9971,7 +9989,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1068</v>
@@ -9980,7 +9998,7 @@
         <v>1069</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9989,7 +10007,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1071</v>
@@ -9998,7 +10016,7 @@
         <v>1072</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -10007,7 +10025,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1074</v>
@@ -10016,7 +10034,7 @@
         <v>1075</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -10025,7 +10043,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1077</v>
@@ -10034,7 +10052,7 @@
         <v>1078</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10043,7 +10061,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1080</v>
@@ -10052,7 +10070,7 @@
         <v>1081</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10061,7 +10079,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1083</v>
@@ -10070,7 +10088,7 @@
         <v>1084</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
@@ -10079,7 +10097,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>1086</v>
@@ -10088,7 +10106,7 @@
         <v>1087</v>
       </c>
       <c r="D372" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E372" s="1" t="s">
@@ -10097,7 +10115,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>1089</v>
@@ -10106,7 +10124,7 @@
         <v>1090</v>
       </c>
       <c r="D373" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E373" s="1" t="s">
@@ -10115,7 +10133,7 @@
     </row>
     <row r="374">
       <c r="A374" s="1" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="B374" s="1" t="s">
         <v>1092</v>
@@ -10124,11 +10142,47 @@
         <v>1093</v>
       </c>
       <c r="D374" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E374" s="1" t="s">
         <v>1094</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D375" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E375" s="1" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D376" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/08 週五 16:45:48.45
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -491,7 +491,7 @@
     <t xml:space="preserve">法拍費用檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月04日 10:03:23</t>
+    <t xml:space="preserve">2023年09月08日 16:10:48</t>
   </si>
   <si>
     <t xml:space="preserve">ForeclosureFinished</t>
@@ -932,7 +932,7 @@
     <t xml:space="preserve">區域資料主檔 </t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月17日 17:41:15</t>
+    <t xml:space="preserve">2023年09月04日 10:36:19</t>
   </si>
   <si>
     <t xml:space="preserve">HlAreaLnYg6Pt</t>
@@ -941,7 +941,7 @@
     <t xml:space="preserve">區域中心房貸專員業績統計</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月10日 14:20:01</t>
+    <t xml:space="preserve">2023年09月04日 10:17:18</t>
   </si>
   <si>
     <t xml:space="preserve">HlCusData</t>
@@ -968,7 +968,7 @@
     <t xml:space="preserve">介紹人業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月17日 17:30:08</t>
+    <t xml:space="preserve">2023年09月04日 10:33:04</t>
   </si>
   <si>
     <t xml:space="preserve">HlThreeLaqhcp</t>
@@ -977,7 +977,7 @@
     <t xml:space="preserve">單位、區部、部室業績累計檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年05月19日 10:47:31</t>
+    <t xml:space="preserve">2023年09月04日 10:33:17</t>
   </si>
   <si>
     <t xml:space="preserve">InnDocRecord</t>
@@ -995,7 +995,7 @@
     <t xml:space="preserve">資金運用概況檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年06月01日 11:11:26</t>
+    <t xml:space="preserve">2023年09月07日 15:34:48</t>
   </si>
   <si>
     <t xml:space="preserve">InnLoanMeeting</t>
@@ -1112,7 +1112,7 @@
     <t xml:space="preserve">債務協商交易檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月05日 20:31:19</t>
+    <t xml:space="preserve">2023年09月06日 17:56:30</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsDetail</t>
@@ -1175,7 +1175,7 @@
     <t xml:space="preserve">房貸獎勵保費檢核檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月22日 16:12:10</t>
+    <t xml:space="preserve">2023年09月04日 21:46:32</t>
   </si>
   <si>
     <t xml:space="preserve">PfIntranetAdjust</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月07日 09:37:13</t>
+    <t xml:space="preserve">2023年09月05日 11:21:08</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>
@@ -1208,7 +1208,7 @@
     <t xml:space="preserve">介紹、協辦獎金明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月18日 12:44:47</t>
+    <t xml:space="preserve">2023年09月05日 11:21:58</t>
   </si>
   <si>
     <t xml:space="preserve">PfRewardMedia</t>
@@ -1217,7 +1217,7 @@
     <t xml:space="preserve">獎金媒體發放檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年05月18日 17:28:31</t>
+    <t xml:space="preserve">2023年09月07日 16:03:47</t>
   </si>
   <si>
     <t xml:space="preserve">SpecInnReCheck</t>
@@ -1238,7 +1238,7 @@
     <t xml:space="preserve">會計業務檢核檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年04月06日 18:43:32</t>
+    <t xml:space="preserve">2023年09月06日 16:34:55</t>
   </si>
   <si>
     <t xml:space="preserve">AcAcctCheckDetail</t>
@@ -1301,7 +1301,7 @@
     <t xml:space="preserve">會計總帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年01月07日 15:32:43</t>
+    <t xml:space="preserve">2023年09月06日 16:34:50</t>
   </si>
   <si>
     <t xml:space="preserve">AcReceivable</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月31日 16:53:28</t>
+    <t xml:space="preserve">2023年09月08日 15:30:45</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1742,7 +1742,7 @@
     <t xml:space="preserve">系統參數設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年07月10日 16:04:48</t>
+    <t xml:space="preserve">2023年09月01日 17:22:53</t>
   </si>
   <si>
     <t xml:space="preserve">L7-介接外部系統</t>
@@ -2423,7 +2423,7 @@
     <t xml:space="preserve">前置調解受理申請暨請求回報債權通知資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年09月07日 14:44:00</t>
+    <t xml:space="preserve">2023年09月05日 13:13:32</t>
   </si>
   <si>
     <t xml:space="preserve">JcicZ440Log</t>
@@ -2801,7 +2801,7 @@
     <t xml:space="preserve">額度月報工作檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月25日 12:47:32</t>
+    <t xml:space="preserve">2023年09月08日 15:04:41</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM003</t>
@@ -2846,7 +2846,7 @@
     <t xml:space="preserve">LM042RBC會計報表</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年08月28日 18:23:45</t>
+    <t xml:space="preserve">2023年09月08日 11:48:44</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM052AssetClass</t>
@@ -2855,7 +2855,7 @@
     <t xml:space="preserve">LM052資產分類表</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:45:29</t>
+    <t xml:space="preserve">2023年09月08日 15:29:06</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM052LoanAsset</t>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/22 週五 16:59:26.34
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1096">
   <si>
     <t xml:space="preserve">分類</t>
   </si>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:08:07</t>
+    <t xml:space="preserve">2023年09月21日 11:37:51</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -518,7 +518,7 @@
     <t xml:space="preserve">保證人檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:22:05</t>
+    <t xml:space="preserve">2023年09月20日 14:04:49</t>
   </si>
   <si>
     <t xml:space="preserve">ReltMain</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:25:25</t>
+    <t xml:space="preserve">2023年09月20日 15:31:11</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:25:36</t>
+    <t xml:space="preserve">2023年09月20日 15:55:32</t>
   </si>
   <si>
     <t xml:space="preserve">BatxBaseRateChange</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">最大債權撥付資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:37:56</t>
+    <t xml:space="preserve">2023年09月15日 17:17:54</t>
   </si>
   <si>
     <t xml:space="preserve">NegAppr02</t>
@@ -1148,7 +1148,7 @@
     <t xml:space="preserve">協辦人員等級歷程檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:40:41</t>
+    <t xml:space="preserve">2023年09月20日 11:22:36</t>
   </si>
   <si>
     <t xml:space="preserve">PfDeparment</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 15:15:05</t>
+    <t xml:space="preserve">2023年09月22日 11:16:56</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月15日 12:06:23</t>
+    <t xml:space="preserve">2023年09月22日 16:21:41</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1821,6 +1821,33 @@
     <t xml:space="preserve">2023年09月14日 15:29:12</t>
   </si>
   <si>
+    <t xml:space="preserve">L7206Cust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">利害關係人借款人檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年09月22日 14:38:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7206Emp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">利害關係人員工檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年09月22日 14:38:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7206Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">利害關係人負責人檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年09月22日 14:38:15</t>
+  </si>
+  <si>
     <t xml:space="preserve">LifeRelEmp</t>
   </si>
   <si>
@@ -2756,7 +2783,7 @@
     <t xml:space="preserve">額度月報工作檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月15日 15:40:33</t>
+    <t xml:space="preserve">2023年09月19日 13:03:24</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM003</t>
@@ -2828,7 +2855,7 @@
     <t xml:space="preserve">LM052備抵損失資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 16:18:25</t>
+    <t xml:space="preserve">2023年09月21日 16:27:12</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLM052Ovdu</t>
@@ -2846,7 +2873,7 @@
     <t xml:space="preserve">LM055重要放款餘額明細表</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月15日 09:45:32</t>
+    <t xml:space="preserve">2023年09月18日 14:27:34</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyLoanBal</t>
@@ -3387,7 +3414,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1086</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="2">
@@ -6947,7 +6974,7 @@
         <v>603</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\L7206Cust.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E199" s="1" t="s">
@@ -6965,7 +6992,7 @@
         <v>606</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\L7206Emp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E200" s="1" t="s">
@@ -6983,7 +7010,7 @@
         <v>609</v>
       </c>
       <c r="D201" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\L7206Manager.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E201" s="1" t="s">
@@ -7001,7 +7028,7 @@
         <v>612</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelEmp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -7019,7 +7046,7 @@
         <v>615</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LifeRelHead.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -7037,7 +7064,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ap.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -7055,7 +7082,7 @@
         <v>621</v>
       </c>
       <c r="D205" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Bp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -7073,7 +7100,7 @@
         <v>624</v>
       </c>
       <c r="D206" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Cp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -7091,7 +7118,7 @@
         <v>627</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Dp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E207" s="1" t="s">
@@ -7109,7 +7136,7 @@
         <v>630</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Fp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E208" s="1" t="s">
@@ -7127,7 +7154,7 @@
         <v>633</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Gp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E209" s="1" t="s">
@@ -7145,7 +7172,7 @@
         <v>636</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Hp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E210" s="1" t="s">
@@ -7154,61 +7181,61 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="C211" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Ip.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="D211" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
-        <v>638</v>
+        <v>574</v>
       </c>
       <c r="B212" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\LoanIfrs9Jp.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E212" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="D212" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
-        <v>638</v>
+        <v>574</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L7-介接外部系統\StakeholdersStaff.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E213" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="D213" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>648</v>
@@ -7217,7 +7244,7 @@
         <v>649</v>
       </c>
       <c r="D214" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\AmlCustList.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E214" s="1" t="s">
@@ -7226,7 +7253,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>651</v>
@@ -7235,7 +7262,7 @@
         <v>652</v>
       </c>
       <c r="D215" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB080.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E215" s="1" t="s">
@@ -7244,7 +7271,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>654</v>
@@ -7253,7 +7280,7 @@
         <v>655</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB085.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E216" s="1" t="s">
@@ -7262,7 +7289,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>657</v>
@@ -7271,7 +7298,7 @@
         <v>658</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB090.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E217" s="1" t="s">
@@ -7280,7 +7307,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>660</v>
@@ -7289,7 +7316,7 @@
         <v>661</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB091.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E218" s="1" t="s">
@@ -7298,7 +7325,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>663</v>
@@ -7307,7 +7334,7 @@
         <v>664</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB092.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E219" s="1" t="s">
@@ -7316,7 +7343,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>666</v>
@@ -7325,7 +7352,7 @@
         <v>667</v>
       </c>
       <c r="D220" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB093.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E220" s="1" t="s">
@@ -7334,7 +7361,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>669</v>
@@ -7343,7 +7370,7 @@
         <v>670</v>
       </c>
       <c r="D221" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB094.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E221" s="1" t="s">
@@ -7352,7 +7379,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>672</v>
@@ -7361,7 +7388,7 @@
         <v>673</v>
       </c>
       <c r="D222" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB095.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -7370,7 +7397,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>675</v>
@@ -7379,7 +7406,7 @@
         <v>676</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB096.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -7388,7 +7415,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>678</v>
@@ -7397,7 +7424,7 @@
         <v>679</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB201.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -7406,7 +7433,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>681</v>
@@ -7415,7 +7442,7 @@
         <v>682</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB204.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -7424,7 +7451,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>684</v>
@@ -7433,7 +7460,7 @@
         <v>685</v>
       </c>
       <c r="D226" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB207.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -7442,7 +7469,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>687</v>
@@ -7451,7 +7478,7 @@
         <v>688</v>
       </c>
       <c r="D227" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB211.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -7460,7 +7487,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>690</v>
@@ -7469,7 +7496,7 @@
         <v>691</v>
       </c>
       <c r="D228" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicB680.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -7478,7 +7505,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>693</v>
@@ -7487,7 +7514,7 @@
         <v>694</v>
       </c>
       <c r="D229" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicMonthlyLoanData.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -7496,1366 +7523,1366 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>696</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="D230" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicReFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D231" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicRel.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="D232" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B233" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C233" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>704</v>
-      </c>
       <c r="D233" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ040Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="D234" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B235" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="C235" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>709</v>
-      </c>
       <c r="D235" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ041Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="D236" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="C237" s="1" t="s">
-        <v>714</v>
-      </c>
       <c r="D237" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ042Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="D238" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C239" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="C239" s="1" t="s">
-        <v>719</v>
-      </c>
       <c r="D239" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ043Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>724</v>
-      </c>
       <c r="D241" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ044Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="D242" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B243" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>729</v>
-      </c>
       <c r="D243" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ045Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="D244" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C245" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>734</v>
-      </c>
       <c r="D245" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ046Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="D246" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B247" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>739</v>
-      </c>
       <c r="D247" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ047Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="D248" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B249" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="C249" s="1" t="s">
-        <v>744</v>
-      </c>
       <c r="D249" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ048Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="D250" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B251" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C251" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="C251" s="1" t="s">
-        <v>749</v>
-      </c>
       <c r="D251" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ049Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="D252" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B253" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C253" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="D253" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ050Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="D254" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>759</v>
-      </c>
       <c r="D255" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ051Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="D256" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="C257" s="1" t="s">
-        <v>764</v>
-      </c>
       <c r="D257" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ052Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="D258" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B259" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="C259" s="1" t="s">
-        <v>769</v>
-      </c>
       <c r="D259" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ053Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="D260" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C261" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="C261" s="1" t="s">
-        <v>774</v>
-      </c>
       <c r="D261" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ054Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D262" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B263" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="C263" s="1" t="s">
-        <v>744</v>
-      </c>
       <c r="D263" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ055Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>744</v>
+        <v>783</v>
       </c>
       <c r="D264" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>783</v>
       </c>
       <c r="D265" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ056Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>783</v>
+        <v>753</v>
       </c>
       <c r="D266" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>788</v>
+        <v>753</v>
       </c>
       <c r="D267" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ060Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="D268" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B269" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C269" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="C269" s="1" t="s">
-        <v>793</v>
-      </c>
       <c r="D269" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ061Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="D270" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="C271" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C271" s="1" t="s">
-        <v>798</v>
-      </c>
       <c r="D271" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ062Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="D272" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B273" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C273" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="C273" s="1" t="s">
-        <v>803</v>
-      </c>
       <c r="D273" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ063Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="D274" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="C275" s="1" t="s">
-        <v>808</v>
-      </c>
       <c r="D275" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ440Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="D276" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>813</v>
-      </c>
       <c r="D277" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ442Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="D278" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="C279" s="1" t="s">
-        <v>818</v>
-      </c>
       <c r="D279" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ443Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="D280" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="C281" s="1" t="s">
-        <v>823</v>
-      </c>
       <c r="D281" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ444Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="D282" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>828</v>
-      </c>
       <c r="D283" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ446Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="D284" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C285" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>833</v>
-      </c>
       <c r="D285" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ447Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="D286" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>838</v>
-      </c>
       <c r="D287" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ448Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="D288" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>843</v>
-      </c>
       <c r="D289" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ450Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="D290" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>848</v>
-      </c>
       <c r="D291" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ451Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="D292" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B293" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C293" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>853</v>
-      </c>
       <c r="D293" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ454Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="D294" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>858</v>
-      </c>
       <c r="D295" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ570Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D296" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B297" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C297" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>863</v>
-      </c>
       <c r="D297" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ571Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="D298" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>868</v>
-      </c>
       <c r="D299" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ572Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="D300" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B301" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>873</v>
-      </c>
       <c r="D301" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ573Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="D302" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="C303" s="1" t="s">
-        <v>878</v>
-      </c>
       <c r="D303" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ574Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="D304" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D305" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\JcicZ575Log.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E305" s="1" t="s">
@@ -8864,7 +8891,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>886</v>
@@ -8873,7 +8900,7 @@
         <v>887</v>
       </c>
       <c r="D306" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryChkDtl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E306" s="1" t="s">
@@ -8882,7 +8909,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>889</v>
@@ -8891,7 +8918,7 @@
         <v>890</v>
       </c>
       <c r="D307" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E307" s="1" t="s">
@@ -8900,61 +8927,61 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B308" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="B308" s="1" t="s">
+      <c r="C308" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="C308" s="1" t="s">
+      <c r="D308" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryParas.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E308" s="1" t="s">
         <v>894</v>
-      </c>
-      <c r="D308" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E308" s="1" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>892</v>
+        <v>647</v>
       </c>
       <c r="B309" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C309" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="C309" s="1" t="s">
+      <c r="D309" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\MlaundryRecord.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E309" s="1" t="s">
         <v>897</v>
-      </c>
-      <c r="D309" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E309" s="1" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>892</v>
+        <v>647</v>
       </c>
       <c r="B310" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C310" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="C310" s="1" t="s">
+      <c r="D310" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L8-遵循法令作業\TbJcicMu01.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E310" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="D310" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lagdtp.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>902</v>
@@ -8963,7 +8990,7 @@
         <v>903</v>
       </c>
       <c r="D311" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E311" s="1" t="s">
@@ -8972,7 +8999,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>905</v>
@@ -8981,7 +9008,7 @@
         <v>906</v>
       </c>
       <c r="D312" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\LaLgtp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\DailyTav.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E312" s="1" t="s">
@@ -8990,7 +9017,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>908</v>
@@ -8999,7 +9026,7 @@
         <v>909</v>
       </c>
       <c r="D313" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lagdtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E313" s="1" t="s">
@@ -9008,7 +9035,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>911</v>
@@ -9017,7 +9044,7 @@
         <v>912</v>
       </c>
       <c r="D314" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\Lahgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E314" s="1" t="s">
@@ -9026,7 +9053,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>914</v>
@@ -9035,7 +9062,7 @@
         <v>915</v>
       </c>
       <c r="D315" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\LaLgtp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E315" s="1" t="s">
@@ -9044,7 +9071,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>917</v>
@@ -9053,7 +9080,7 @@
         <v>918</v>
       </c>
       <c r="D316" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyDpUnpaidExpense.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -9062,7 +9089,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>920</v>
@@ -9071,7 +9098,7 @@
         <v>921</v>
       </c>
       <c r="D317" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyFacBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E317" s="1" t="s">
@@ -9080,7 +9107,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>923</v>
@@ -9089,7 +9116,7 @@
         <v>924</v>
       </c>
       <c r="D318" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM003.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E318" s="1" t="s">
@@ -9098,7 +9125,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>926</v>
@@ -9107,7 +9134,7 @@
         <v>927</v>
       </c>
       <c r="D319" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM042RBC.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM028.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E319" s="1" t="s">
@@ -9116,7 +9143,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>929</v>
@@ -9125,7 +9152,7 @@
         <v>930</v>
       </c>
       <c r="D320" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM032.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E320" s="1" t="s">
@@ -9134,7 +9161,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>932</v>
@@ -9143,7 +9170,7 @@
         <v>933</v>
       </c>
       <c r="D321" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM036Portfolio.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E321" s="1" t="s">
@@ -9152,7 +9179,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>935</v>
@@ -9161,7 +9188,7 @@
         <v>936</v>
       </c>
       <c r="D322" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM042RBC.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E322" s="1" t="s">
@@ -9170,7 +9197,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>938</v>
@@ -9179,7 +9206,7 @@
         <v>939</v>
       </c>
       <c r="D323" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052AssetClass.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E323" s="1" t="s">
@@ -9188,7 +9215,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>941</v>
@@ -9197,7 +9224,7 @@
         <v>942</v>
       </c>
       <c r="D324" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM055AssetLoss.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052LoanAsset.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E324" s="1" t="s">
@@ -9206,7 +9233,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>944</v>
@@ -9215,7 +9242,7 @@
         <v>945</v>
       </c>
       <c r="D325" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Loss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E325" s="1" t="s">
@@ -9224,7 +9251,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>947</v>
@@ -9233,7 +9260,7 @@
         <v>948</v>
       </c>
       <c r="D326" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM052Ovdu.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E326" s="1" t="s">
@@ -9242,7 +9269,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>950</v>
@@ -9251,7 +9278,7 @@
         <v>951</v>
       </c>
       <c r="D327" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLM055AssetLoss.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E327" s="1" t="s">
@@ -9260,7 +9287,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>953</v>
@@ -9269,7 +9296,7 @@
         <v>954</v>
       </c>
       <c r="D328" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\MonthlyLoanBal.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E328" s="1" t="s">
@@ -9278,7 +9305,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>956</v>
@@ -9287,7 +9314,7 @@
         <v>957</v>
       </c>
       <c r="D329" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptJcic.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E329" s="1" t="s">
@@ -9296,7 +9323,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>959</v>
@@ -9305,7 +9332,7 @@
         <v>960</v>
       </c>
       <c r="D330" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationCompany.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E330" s="1" t="s">
@@ -9314,7 +9341,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>962</v>
@@ -9323,7 +9350,7 @@
         <v>963</v>
       </c>
       <c r="D331" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationFamily.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E331" s="1" t="s">
@@ -9332,7 +9359,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>965</v>
@@ -9341,7 +9368,7 @@
         <v>966</v>
       </c>
       <c r="D332" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\RptRelationSelf.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E332" s="1" t="s">
@@ -9350,7 +9377,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>968</v>
@@ -9359,7 +9386,7 @@
         <v>969</v>
       </c>
       <c r="D333" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipEbsRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E333" s="1" t="s">
@@ -9368,7 +9395,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>971</v>
@@ -9377,7 +9404,7 @@
         <v>972</v>
       </c>
       <c r="D334" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E334" s="1" t="s">
@@ -9386,61 +9413,61 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B335" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="C335" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="C335" s="1" t="s">
+      <c r="D335" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\SlipMedia2022.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E335" s="1" t="s">
         <v>976</v>
-      </c>
-      <c r="D335" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E335" s="1" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>974</v>
+        <v>901</v>
       </c>
       <c r="B336" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C336" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="C336" s="1" t="s">
+      <c r="D336" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanInt.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E336" s="1" t="s">
         <v>979</v>
-      </c>
-      <c r="D336" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>974</v>
+        <v>901</v>
       </c>
       <c r="B337" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C337" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C337" s="1" t="s">
+      <c r="D337" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L9-報表作業\YearlyHouseLoanIntCheck.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E337" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="D337" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
-        <v>連結</v>
-      </c>
-      <c r="E337" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>984</v>
@@ -9449,7 +9476,7 @@
         <v>985</v>
       </c>
       <c r="D338" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAgent.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E338" s="1" t="s">
@@ -9458,7 +9485,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>987</v>
@@ -9467,7 +9494,7 @@
         <v>988</v>
       </c>
       <c r="D339" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlCredit.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E339" s="1" t="s">
@@ -9476,7 +9503,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>990</v>
@@ -9485,7 +9512,7 @@
         <v>991</v>
       </c>
       <c r="D340" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E340" s="1" t="s">
@@ -9494,7 +9521,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>993</v>
@@ -9503,7 +9530,7 @@
         <v>994</v>
       </c>
       <c r="D341" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlNotice.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E341" s="1" t="s">
@@ -9512,7 +9539,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>996</v>
@@ -9521,7 +9548,7 @@
         <v>997</v>
       </c>
       <c r="D342" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRating.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E342" s="1" t="s">
@@ -9530,7 +9557,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>999</v>
@@ -9539,7 +9566,7 @@
         <v>1000</v>
       </c>
       <c r="D343" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAmlRatingAppl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E343" s="1" t="s">
@@ -9548,7 +9575,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>1002</v>
@@ -9557,7 +9584,7 @@
         <v>1003</v>
       </c>
       <c r="D344" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxApLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E344" s="1" t="s">
@@ -9566,7 +9593,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1005</v>
@@ -9575,7 +9602,7 @@
         <v>1006</v>
       </c>
       <c r="D345" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTable.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E345" s="1" t="s">
@@ -9584,7 +9611,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1008</v>
@@ -9593,7 +9620,7 @@
         <v>1009</v>
       </c>
       <c r="D346" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxArchiveTableLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E346" s="1" t="s">
@@ -9602,7 +9629,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1011</v>
@@ -9611,7 +9638,7 @@
         <v>1012</v>
       </c>
       <c r="D347" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachment.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E347" s="1" t="s">
@@ -9620,7 +9647,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1014</v>
@@ -9629,7 +9656,7 @@
         <v>1015</v>
       </c>
       <c r="D348" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAttachType.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E348" s="1" t="s">
@@ -9638,7 +9665,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1017</v>
@@ -9647,7 +9674,7 @@
         <v>1018</v>
       </c>
       <c r="D349" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthGroup.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E349" s="1" t="s">
@@ -9656,7 +9683,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1020</v>
@@ -9665,7 +9692,7 @@
         <v>1021</v>
       </c>
       <c r="D350" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthority.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E350" s="1" t="s">
@@ -9674,7 +9701,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1023</v>
@@ -9683,7 +9710,7 @@
         <v>1024</v>
       </c>
       <c r="D351" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxAuthorize.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E351" s="1" t="s">
@@ -9692,7 +9719,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1026</v>
@@ -9701,7 +9728,7 @@
         <v>1027</v>
       </c>
       <c r="D352" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxBizDate.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E352" s="1" t="s">
@@ -9710,7 +9737,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1029</v>
@@ -9719,7 +9746,7 @@
         <v>1030</v>
       </c>
       <c r="D353" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxControl.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E353" s="1" t="s">
@@ -9728,7 +9755,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>1032</v>
@@ -9737,7 +9764,7 @@
         <v>1033</v>
       </c>
       <c r="D354" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCruiser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E354" s="1" t="s">
@@ -9746,7 +9773,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>1035</v>
@@ -9755,7 +9782,7 @@
         <v>1036</v>
       </c>
       <c r="D355" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxCurr.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E355" s="1" t="s">
@@ -9764,7 +9791,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1038</v>
@@ -9773,7 +9800,7 @@
         <v>1039</v>
       </c>
       <c r="D356" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxDataLog.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E356" s="1" t="s">
@@ -9782,7 +9809,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1041</v>
@@ -9791,7 +9818,7 @@
         <v>1042</v>
       </c>
       <c r="D357" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxErrCode.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E357" s="1" t="s">
@@ -9800,7 +9827,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>1044</v>
@@ -9809,7 +9836,7 @@
         <v>1045</v>
       </c>
       <c r="D358" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFile.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E358" s="1" t="s">
@@ -9818,7 +9845,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1047</v>
@@ -9827,7 +9854,7 @@
         <v>1048</v>
       </c>
       <c r="D359" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFlow.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E359" s="1" t="s">
@@ -9836,7 +9863,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>1050</v>
@@ -9845,7 +9872,7 @@
         <v>1051</v>
       </c>
       <c r="D360" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxFtpUser.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E360" s="1" t="s">
@@ -9854,7 +9881,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>1053</v>
@@ -9863,7 +9890,7 @@
         <v>1054</v>
       </c>
       <c r="D361" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxHoliday.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E361" s="1" t="s">
@@ -9872,7 +9899,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>1056</v>
@@ -9881,7 +9908,7 @@
         <v>1057</v>
       </c>
       <c r="D362" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxInquiry.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E362" s="1" t="s">
@@ -9890,7 +9917,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>1059</v>
@@ -9899,7 +9926,7 @@
         <v>1060</v>
       </c>
       <c r="D363" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxLock.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E363" s="1" t="s">
@@ -9908,7 +9935,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>1062</v>
@@ -9917,7 +9944,7 @@
         <v>1063</v>
       </c>
       <c r="D364" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxPrinter.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E364" s="1" t="s">
@@ -9926,7 +9953,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>1065</v>
@@ -9935,7 +9962,7 @@
         <v>1066</v>
       </c>
       <c r="D365" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxRecord.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E365" s="1" t="s">
@@ -9944,7 +9971,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>1068</v>
@@ -9953,7 +9980,7 @@
         <v>1069</v>
       </c>
       <c r="D366" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTeller.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E366" s="1" t="s">
@@ -9962,7 +9989,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>1071</v>
@@ -9971,7 +9998,7 @@
         <v>1072</v>
       </c>
       <c r="D367" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTellerAuth.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E367" s="1" t="s">
@@ -9980,7 +10007,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>1074</v>
@@ -9989,7 +10016,7 @@
         <v>1075</v>
       </c>
       <c r="D368" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTemp.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E368" s="1" t="s">
@@ -9998,7 +10025,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>1077</v>
@@ -10007,7 +10034,7 @@
         <v>1078</v>
       </c>
       <c r="D369" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetail.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E369" s="1" t="s">
@@ -10016,7 +10043,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>1080</v>
@@ -10025,7 +10052,7 @@
         <v>1081</v>
       </c>
       <c r="D370" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoDetailReserve.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E370" s="1" t="s">
@@ -10034,7 +10061,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>1083</v>
@@ -10043,11 +10070,65 @@
         <v>1084</v>
       </c>
       <c r="D371" s="2" t="str">
-        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxToDoMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
       <c r="E371" s="1" t="s">
         <v>1085</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D372" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxTranCode.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D373" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\TxUnLock.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D374" s="2" t="str">
+        <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\XX-系統\UspErrorLog.xlsx]DBD!A1", "連結")</f>
+        <v>連結</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>1094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/28 週四 16:49:01.67
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -758,7 +758,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:27:16</t>
+    <t xml:space="preserve">2023年09月27日 11:50:05</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">最大債權撥付資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月15日 17:17:54</t>
+    <t xml:space="preserve">2023年09月22日 21:34:51</t>
   </si>
   <si>
     <t xml:space="preserve">NegAppr02</t>
@@ -1217,7 +1217,7 @@
     <t xml:space="preserve">獎金媒體發放檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 14:42:14</t>
+    <t xml:space="preserve">2023年09月27日 17:36:11</t>
   </si>
   <si>
     <t xml:space="preserve">SpecInnReCheck</t>
@@ -1265,7 +1265,7 @@
     <t xml:space="preserve">會計帳務明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月22日 11:16:56</t>
+    <t xml:space="preserve">2023年09月28日 14:06:18</t>
   </si>
   <si>
     <t xml:space="preserve">AcLoanInt</t>
@@ -1499,7 +1499,7 @@
     <t xml:space="preserve">雜項資料檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月22日 16:21:41</t>
+    <t xml:space="preserve">2023年09月28日 16:29:24</t>
   </si>
   <si>
     <t xml:space="preserve">CdConvertCode</t>
@@ -1625,7 +1625,7 @@
     <t xml:space="preserve">報表代號對照檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2023年09月14日 15:21:58</t>
+    <t xml:space="preserve">2023年09月26日 13:21:40</t>
   </si>
   <si>
     <t xml:space="preserve">CdRuleCode</t>
@@ -3152,10 +3152,10 @@
     <t xml:space="preserve">TxFile</t>
   </si>
   <si>
-    <t xml:space="preserve">輸出檔</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022年03月16日 16:10:33</t>
+    <t xml:space="preserve">報表輸出檔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023年09月26日 13:52:05</t>
   </si>
   <si>
     <t xml:space="preserve">TxFlow</t>
@@ -3209,7 +3209,7 @@
     <t xml:space="preserve">印表機設定檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年04月20日 09:49:58</t>
+    <t xml:space="preserve">2023年09月25日 15:44:03</t>
   </si>
   <si>
     <t xml:space="preserve">TxRecord</t>

</xml_diff>